<commit_message>
Update design parameters and add fuel_max calculations in design JSON files; implement range equation and payload-range visualization in new scripts.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>53392355.25717556</v>
+        <v>51507919.18927524</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>53392355.25717556</v>
+        <v>51507919.18927524</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>53392355.25717556</v>
+        <v>51507919.18927524</v>
       </c>
     </row>
     <row r="3">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>491781.437347126</v>
+        <v>265905.7682338378</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>74563.76196904253</v>
+        <v>74123.39690932246</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>460402.3400181599</v>
+        <v>247105.4339477974</v>
       </c>
     </row>
     <row r="5">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4824375.900375306</v>
+        <v>2608535.586373949</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>731470.5049163073</v>
+        <v>727150.5236804534</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>4516546.955578149</v>
+        <v>2424104.307027892</v>
       </c>
     </row>
     <row r="6">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2065065.131393465</v>
+        <v>1289311.913317399</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>619642.6671634965</v>
+        <v>-259886.5473271068</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>1956354.367532743</v>
+        <v>1223994.993373831</v>
       </c>
     </row>
     <row r="7">
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>200000</v>
+        <v>90000</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>4036058.75729384</v>
+        <v>2172211.913317399</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>624543.3876684128</v>
+        <v>623013.4526728932</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>3927040.164488322</v>
+        <v>2106894.993373831</v>
       </c>
     </row>
     <row r="8">
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2064640.131393465</v>
+        <v>1285142.663317399</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>619217.6671634965</v>
+        <v>-264055.7973271068</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>1955929.367532743</v>
+        <v>1219825.743373831</v>
       </c>
     </row>
     <row r="9">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>788317.1430814654</v>
+        <v>436323.6730565503</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>106927.1172478945</v>
+        <v>104137.0710075602</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>589506.7910898275</v>
+        <v>317209.3136540609</v>
       </c>
     </row>
     <row r="10">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>788317.1430814654</v>
+        <v>436323.6730565503</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>106927.1172478945</v>
+        <v>104137.0710075602</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>589506.7910898275</v>
+        <v>317209.3136540609</v>
       </c>
     </row>
     <row r="11">
@@ -802,11 +802,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>altitude_range_WIG (m)</t>
+          <t>max_payload</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>943600</v>
+        <v>100000</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1447.38035000507</v>
+        <v>782.6138047231788</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>219.450495090008</v>
+        <v>218.1569152626498</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -830,17 +830,17 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>1355.029750620472</v>
+        <v>727.2722528154185</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>altitude_range_WOG (m)</t>
+          <t>altitude_range_WIG (m)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>538000</v>
+        <v>943600</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -870,11 +870,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>altitude_payload (kg)</t>
+          <t>altitude_range_WOG (m)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>200000</v>
+        <v>538000</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>131.7898486229529</v>
+        <v>96.90905869256055</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>51.31672184658813</v>
+        <v>51.16525171590381</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -898,17 +898,17 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>127.5161048944237</v>
+        <v>93.41984282680538</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>altitude_crew</t>
+          <t>altitude_payload (kg)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>425</v>
+        <v>90000</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>10.98248738524608</v>
+        <v>8.075754891046712</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -924,7 +924,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>4.276393487215677</v>
+        <v>4.263770976325318</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -932,17 +932,17 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>10.62634207453531</v>
+        <v>7.784986902233783</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>cruise_speed (m/s)</t>
+          <t>altitude_crew</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>115.749</v>
+        <v>425</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -972,11 +972,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>jet_consumption (kg/(N·s))</t>
+          <t>cruise_speed (m/s)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2.7e-05</v>
+        <v>115.749</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.03035135135061797</v>
+        <v>0.04127581109511973</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>0.07794730169939618</v>
+        <v>0.07817805768278223</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1000,17 +1000,17 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>0.03136858676252525</v>
+        <v>0.04281745589548629</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>prop_consumption (kg/J)</t>
+          <t>jet_consumption (kg/(N·s))</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2.1e-08</v>
+        <v>2.7e-05</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1018,7 +1018,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2.04047861067412</v>
+        <v>1.83527261507357</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>1.500149381862434</v>
+        <v>1.49884578273208</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1034,17 +1034,17 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>2.016991471724409</v>
+        <v>1.812794897626504</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>prop_efficiency</t>
+          <t>prop_consumption (kg/J)</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.82</v>
+        <v>2.1e-08</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.106256618406918</v>
+        <v>0.1101440556657076</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>0.106256618406918</v>
+        <v>0.1101440556657076</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1068,17 +1068,17 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>0.106256618406918</v>
+        <v>0.1101440556657076</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cd0</t>
+          <t>prop_efficiency</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.02</v>
+        <v>0.85</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1099,11 +1099,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>oswald_factor</t>
+          <t>Cd0</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.85</v>
+        <v>0.02</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1133,11 +1133,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>aspect_ratio</t>
+          <t>oswald_factor</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>12</v>
+        <v>0.85</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1145,7 +1145,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.09449070774320456</v>
+        <v>0.1162209426725255</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1161,17 +1161,17 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>0.2473118850633875</v>
+        <v>0.295726056294236</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Cl_alpha</t>
+          <t>aspect_ratio</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>6883999.471120794</v>
+        <v>6601813.591169997</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1201,11 +1201,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>tfo</t>
+          <t>Cl_alpha</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.001</v>
+        <v>5</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>45403062.62994352</v>
+        <v>23682944.76363733</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1226,17 +1226,17 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>42506029.49062131</v>
+        <v>22008489.63093534</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>reserve_fuel (N)</t>
+          <t>tfo</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1252,150 +1252,160 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>reserve_fuel (N)</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.016991471724409</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>n_engines</t>
+          <t>k</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>1.812794897626504</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CLmax_clean</t>
+          <t>n_engines</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CLmax_takeoff</t>
+          <t>CLmax_clean</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CLmax_landing</t>
+          <t>CLmax_takeoff</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>stall_speed_clean (m/s)</t>
+          <t>CLmax_landing</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>77.16</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>stall_speed_takeoff (m/s)</t>
+          <t>stall_speed_clean (m/s)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>61.728</v>
+        <v>77.16</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>stall_speed_landing (m/s)</t>
+          <t>stall_speed_takeoff (m/s)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>51.44</v>
+        <v>61.728</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>high_altitude (m)</t>
+          <t>stall_speed_landing (m/s)</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3048</v>
+        <v>51.44</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>L (m)</t>
+          <t>high_altitude (m)</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>70</v>
+        <v>3048</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>r (m)</t>
+          <t>L (m)</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>hull_surface (m²)</t>
+          <t>r (m)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>251.3274122871834</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>gravitational_acceleration (m/s²)</t>
+          <t>hull_surface (m²)</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>9.81</v>
+        <v>251.3274122871834</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>kinematic_viscosity (m²/s)</t>
+          <t>gravitational_acceleration (m/s²)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1.002e-06</v>
+        <v>9.81</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>kinematic_viscosity (m²/s)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1.002e-06</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>rho_water (kg/m³)</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B41" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1607,7 +1617,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1294355.019527516</v>
+        <v>1301166.277536666</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1615,7 +1625,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>640031.3648169918</v>
+        <v>-237910.1813767925</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1623,7 +1633,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>1454706.096297423</v>
+        <v>1461971.409645771</v>
       </c>
     </row>
     <row r="7">
@@ -1675,7 +1685,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1293930.019527516</v>
+        <v>1296997.027536666</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1683,7 +1693,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>639606.3648169918</v>
+        <v>-242079.4313767925</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1691,7 +1701,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>1454281.096297423</v>
+        <v>1457802.159645771</v>
       </c>
     </row>
     <row r="9">
@@ -2640,7 +2650,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1286272.024988764</v>
+        <v>1293060.394926933</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2648,7 +2658,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>635453.8510215732</v>
+        <v>-242500.6570095802</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -2656,7 +2666,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>1228949.429234578</v>
+        <v>1235575.482640902</v>
       </c>
     </row>
     <row r="7">
@@ -2708,7 +2718,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1285847.024988764</v>
+        <v>1288891.144926933</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2716,7 +2726,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>635028.8510215732</v>
+        <v>-246669.9070095802</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -2724,7 +2734,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>1228524.429234578</v>
+        <v>1231406.232640902</v>
       </c>
     </row>
     <row r="9">
@@ -3624,7 +3634,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1286607.095465756</v>
+        <v>1293396.414200417</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3632,7 +3642,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>635603.8390508143</v>
+        <v>-242350.2442693433</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -3640,7 +3650,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>1229028.43103543</v>
+        <v>1235654.70814583</v>
       </c>
     </row>
     <row r="7">
@@ -3692,7 +3702,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1286182.095465756</v>
+        <v>1289227.164200417</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3700,7 +3710,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>635178.8390508143</v>
+        <v>-246519.4942693433</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -3708,7 +3718,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>1228603.43103543</v>
+        <v>1231485.45814583</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Add Cd0Estimation class and integrate into main iteration process
- Introduced Cd0Estimation class for drag coefficient calculations.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,13 +438,13 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -500,7 +500,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cruise_altitude [km]</t>
+          <t>cruise_altitude [m]</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2578223.849301696</v>
+        <v>2574437.066356279</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>416746.9333812621</v>
+        <v>414301.2515731714</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>390879.5366012343</v>
+        <v>388403.4960463954</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>25867.39678002783</v>
+        <v>25897.75552677596</v>
       </c>
     </row>
     <row r="6">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>1271829.442071132</v>
+        <v>1270492.127716752</v>
       </c>
     </row>
     <row r="7">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1271404.442071132</v>
+        <v>1270067.127716752</v>
       </c>
     </row>
     <row r="8">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>16.55882593020626</v>
+        <v>16.79397971338663</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>2161476.915920434</v>
+        <v>2160135.814783108</v>
       </c>
     </row>
     <row r="9">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.04701065162617812</v>
+        <v>0.04704521330223214</v>
       </c>
     </row>
     <row r="10">
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="K10" s="2" t="n">
-        <v>1.757359077433866</v>
+        <v>1.756933311801416</v>
       </c>
     </row>
     <row r="11">
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02434723936958912</v>
+        <v>0.02367017989497004</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.09385590949149301</v>
+        <v>0.09582402833754056</v>
       </c>
     </row>
     <row r="12">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>27470021.4751569</v>
+        <v>26866299.72690997</v>
       </c>
     </row>
     <row r="15">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>29.09980306009526</v>
+        <v>29.50590239616616</v>
       </c>
     </row>
     <row r="17">
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>262815.88677897</v>
+        <v>262429.8742463078</v>
       </c>
     </row>
     <row r="18">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>723.9814528557438</v>
+        <v>722.9181004124157</v>
       </c>
     </row>
     <row r="19">
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>85.08709966003917</v>
+        <v>85.02459058486643</v>
       </c>
     </row>
     <row r="20">
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>8.508709966003916</v>
+        <v>8.502459058486643</v>
       </c>
     </row>
     <row r="21">
@@ -1115,7 +1115,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.1457627615200027</v>
+        <v>0.1448394220378516</v>
       </c>
     </row>
     <row r="22">
@@ -1127,17 +1127,13 @@
       <c r="B22" s="2" t="n">
         <v>160</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="D23" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="E23" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>1.453895622250116</v>
       </c>
     </row>
     <row r="24">
@@ -1151,13 +1147,15 @@
           <t>General States</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>0.4</v>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1171,11 +1169,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E25" s="4" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="26">
@@ -1189,11 +1187,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>5</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1207,100 +1205,126 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>dihedral [deg]</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>viscosity_air [m²/s]</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1.484e-05</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>sweep_x_c [deg]</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E28" s="2" t="n">
         <v>2.454031674527076</v>
       </c>
     </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rho_air</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1.225</v>
+      </c>
+      <c r="D29" t="inlineStr">
         <is>
           <t>chord_root [m]</t>
         </is>
       </c>
-      <c r="E28" s="2" t="n">
-        <v>12.15529995143417</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
       <c r="E29" s="2" t="n">
-        <v>4.862119980573667</v>
+        <v>12.06448415554899</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>18.23294992715125</v>
+        <v>4.825793662219597</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>21.05644</v>
+        <v>18.09672623332349</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>20.27502786026495</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>9.029651392493951</v>
+        <v>20.28086601857185</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>723.9814528557438</v>
+        <v>8.962188229836395</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>85.08709966003917</v>
+        <v>713.203711903514</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>84.45138908884293</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E37" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1310,895 +1334,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="23" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Requirements</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Inputs</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>General Outputs</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Design Mission</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>design_range [m]</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>3704000</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>cruise_altitude [km]</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>d_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>6.204804790550249</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>MTOW [N]</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2654906.911330992</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>design_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aircraft_type</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>PROP</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>r_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>3.102402395275125</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>466272.4468572183</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>design_crew</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>wing_type</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>l_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>52.74084071967712</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>fuel_mission [N]</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>441011.3363928772</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ferry_range [m]</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>12038000</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>n_wings</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>l_tailcone [m]</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>27.92162155747612</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>fuel_reserve [N]</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>25261.11046434118</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>reserve_range [m]</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>185200</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>n_fuselages</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>l_nose [m]</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>9.307207185825375</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>1298910.307562442</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ferry_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>depth</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>l_cargo_straight [m]</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>8.74654837462985</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>EW [N]</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>1298485.307562442</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ferry_crew</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>jet_consumption [kg/(N·s)]</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>2.7e-05</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>3407446264.985502</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>ZFW [N]</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>2188634.464473774</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>altitude_range_WIG [m]</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>943600</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>prop_consumption [kg/J]</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>2.1e-08</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Cd</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>0.001321877371153106</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>h_b</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>0.09263573018439004</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>altitude_range_WOG [m]</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>538000</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>prop_efficiency</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>hull_surface [m²]</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>210.4204947871738</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>1.427664585132139</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>altitude_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Cd0</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02422111472806403</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>take_off_power [W]</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>93133344.13863601</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>WP [N/W]</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>0.09087451023075915</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>altitude_crew</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>oswald_factor</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>take_off_thrust [N]</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>cruise_speed [m/s]</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>115.749</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>V_lof [m/s]</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>64.995</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>3559.80642288087</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>stall_speed_clean [m/s]</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>77.16</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>tfo</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>LD_g</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>16.6018826655351</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>P [W]</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>29215089.07821723</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>stall_speed_takeoff [m/s]</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="E15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>T [N]</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>stall_speed_landing [m/s]</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>n_engines</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>Empennage Design</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>LD</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>23.70191992810363</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>stall_speed_high</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>82.3</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CLmax_clean</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>MTOM [kg]</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>270632.7126739033</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>high_altitude [m]</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>3048</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>CLmax_takeoff</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>745.800921720467</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>cargo_width [m]</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CLmax_landing</t>
-        </is>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>86.35976619470823</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>cargo_height [m]</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>r_float</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>8.635976619470823</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>cargo_length [m]</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>upsweep</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>fuel_economy [L/ton/km]</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>0.1644573947595332</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>cargo_density [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="D23" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="E23" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>General States</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>design_id</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E25" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>kinematic_viscosity [m²/s]</t>
-        </is>
-      </c>
-      <c r="B26" s="3" t="n">
-        <v>1.006e-06</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>rho_water [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>2.454031674527076</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>12.33710945638689</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>4.934843782554757</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>18.50566418458034</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>X_LEMAC [m]</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>21.05644</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>X_LE [m]</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>20.26334010637513</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>9.164709881887404</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>745.800921720467</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>86.35976619470823</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2228,7 +1363,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Design 3</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2238,7 +1373,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Design 3</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -2248,7 +1383,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Design 3</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -2258,7 +1393,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Design 3</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -2278,7 +1413,920 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cruise_altitude [km]</t>
+          <t>cruise_altitude [m]</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>d_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>6.204804790550249</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>2646927.027891309</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>design_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>aircraft_type</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>PROP</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>r_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>3.102402395275125</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>461118.6643351071</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>design_crew</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>wing_type</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>l_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>52.74084071967712</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>fuel_mission [N]</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>435795.1987296298</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ferry_range [m]</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>12038000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>n_wings</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>l_tailcone [m]</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>27.92162155747612</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>fuel_reserve [N]</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>25323.46560547728</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>reserve_range [m]</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>185200</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>n_fuselages</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>l_nose [m]</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>9.307207185825375</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>1296092.186528311</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ferry_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>l_cargo_straight [m]</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>8.74654837462985</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>EW [N]</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>1295667.186528311</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ferry_crew</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jet_consumption [kg/(N·s)]</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>2.7e-05</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Re</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>3407446264.985502</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>ZFW [N]</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>2185808.363556203</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>altitude_range_WIG [m]</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>943600</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>prop_consumption [kg/J]</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>2.1e-08</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0.001321877371153106</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>h_b</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0.09277526293692347</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>altitude_range_WOG [m]</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>538000</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>prop_efficiency</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>hull_surface [m²]</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>210.4204947871738</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>1.427064793454931</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>altitude_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Cd0</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.02315328094641167</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>take_off_power [W]</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>93133344.13863601</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WP [N/W]</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0.09392948775688056</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>altitude_crew</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>oswald_factor</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>take_off_thrust [N]</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cruise_speed [m/s]</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>115.749</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>V_lof [m/s]</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>64.995</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>WS [N/m²]</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>3559.80642288087</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>stall_speed_clean [m/s]</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>77.16</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tfo</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>LD_g</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>16.98040845375636</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>28179936.79197314</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>stall_speed_takeoff [m/s]</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>T [N]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>stall_speed_landing [m/s]</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>n_engines</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>Empennage Design</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>24.23214308284019</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>stall_speed_high</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CLmax_clean</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>MTOM [kg]</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>269819.2688981967</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>high_altitude [m]</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>3048</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CLmax_takeoff</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>743.5592595147021</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cargo_width [m]</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CLmax_landing</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>86.22988226332575</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>cargo_height [m]</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>r_float</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>8.622988226332575</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>cargo_length [m]</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>upsweep</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>0.1625122465512783</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>cargo_density [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>1.228075442628302</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>General States</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>design_id</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>kinematic_viscosity [m²/s]</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1.006e-06</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>rho_water [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>dihedral [deg]</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>viscosity_air [m²/s]</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1.48e-05</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>sweep_x_c [deg]</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>2.454031674527076</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rho_air</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1.225</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>chord_root [m]</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>12.21342606619523</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>chord_tip [m]</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>4.885370426478094</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>y_MAC [m]</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>18.32013909929285</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>21.05644</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>20.27129118145888</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>9.072830792030743</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>730.922103744644</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>85.49398246336662</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="8" max="8"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Requirements</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Inputs</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>General Outputs</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Design Mission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>design_range [m]</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>3704000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>cruise_altitude [m]</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -2298,7 +2346,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2707181.959616246</v>
+        <v>2669083.614040726</v>
       </c>
     </row>
     <row r="3">
@@ -2334,7 +2382,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>500034.1217277198</v>
+        <v>475428.4255377167</v>
       </c>
     </row>
     <row r="4">
@@ -2370,7 +2418,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>475177.4216381638</v>
+        <v>450277.6819258266</v>
       </c>
     </row>
     <row r="5">
@@ -2404,7 +2452,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>24856.70008955605</v>
+        <v>25150.74361189007</v>
       </c>
     </row>
     <row r="6">
@@ -2438,7 +2486,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>1317371.40592891</v>
+        <v>1303916.854888969</v>
       </c>
     </row>
     <row r="7">
@@ -2472,7 +2520,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1316946.40592891</v>
+        <v>1303491.854888969</v>
       </c>
     </row>
     <row r="8">
@@ -2506,7 +2554,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>2207147.837888526</v>
+        <v>2193655.18850301</v>
       </c>
     </row>
     <row r="9">
@@ -2540,7 +2588,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.1146602184967998</v>
+        <v>0.1154756456428767</v>
       </c>
     </row>
     <row r="10">
@@ -2574,7 +2622,7 @@
         </is>
       </c>
       <c r="K10" s="2" t="n">
-        <v>1.348014618278832</v>
+        <v>1.345549746662417</v>
       </c>
     </row>
     <row r="11">
@@ -2592,7 +2640,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02811501719111257</v>
+        <v>0.02320987776139502</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2608,7 +2656,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.08123116348289106</v>
+        <v>0.09375416161734564</v>
       </c>
     </row>
     <row r="12">
@@ -2696,7 +2744,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>15.40938218960205</v>
+        <v>16.9596926268958</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -2704,7 +2752,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>33326888.88774114</v>
+        <v>28468961.46258017</v>
       </c>
     </row>
     <row r="15">
@@ -2763,7 +2811,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>20.77207245022903</v>
+        <v>22.8201101175921</v>
       </c>
     </row>
     <row r="17">
@@ -2789,7 +2837,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>275961.4637733176</v>
+        <v>272077.840371124</v>
       </c>
     </row>
     <row r="18">
@@ -2815,7 +2863,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>760.6317856019537</v>
+        <v>749.9273655990662</v>
       </c>
     </row>
     <row r="19">
@@ -2841,7 +2889,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>87.21420673273097</v>
+        <v>86.59834672781382</v>
       </c>
     </row>
     <row r="20">
@@ -2867,7 +2915,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>8.721420673273098</v>
+        <v>8.659834672781381</v>
       </c>
     </row>
     <row r="21">
@@ -2893,7 +2941,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.1771982585534888</v>
+        <v>0.1679129046739834</v>
       </c>
     </row>
     <row r="22">
@@ -2914,6 +2962,16 @@
         <v>11</v>
       </c>
     </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>1.175600054827848</v>
+      </c>
+    </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
@@ -2925,16 +2983,6 @@
           <t>General States</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2945,13 +2993,15 @@
       <c r="B25" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>0.4</v>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -2965,11 +3015,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="27">
@@ -2983,110 +3033,136 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>viscosity_air [m²/s]</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1.484e-05</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>dihedral [deg]</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E28" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rho_air</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1.225</v>
+      </c>
+      <c r="D29" t="inlineStr">
         <is>
           <t>sweep_x_c [deg]</t>
         </is>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E29" s="2" t="n">
         <v>2.454031674527076</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>12.45917239039014</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>4.983668956156056</v>
+        <v>12.25893671424686</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>18.68875858558521</v>
+        <v>4.903574685698743</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>21.05644</v>
+        <v>18.38840507137029</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>20.25549320347492</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>9.255385204289819</v>
+        <v>20.26836549694127</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>760.6317856019537</v>
+        <v>9.106638702011949</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>87.21420673273097</v>
+        <v>736.3794938831564</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>85.81255699972799</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E38" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3101,7 +3177,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3175,7 +3251,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cruise_altitude [km]</t>
+          <t>cruise_altitude [m]</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -3195,7 +3271,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2725898.387558288</v>
+        <v>2721150.218192705</v>
       </c>
     </row>
     <row r="3">
@@ -3231,7 +3307,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>512122.0676147955</v>
+        <v>509055.477422929</v>
       </c>
     </row>
     <row r="4">
@@ -3267,7 +3343,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>487408.4858193271</v>
+        <v>484305.6699416121</v>
       </c>
     </row>
     <row r="5">
@@ -3301,7 +3377,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>24713.58179546834</v>
+        <v>24749.80748131691</v>
       </c>
     </row>
     <row r="6">
@@ -3335,7 +3411,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>1323981.171555934</v>
+        <v>1322304.340551583</v>
       </c>
     </row>
     <row r="7">
@@ -3369,7 +3445,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1323556.171555934</v>
+        <v>1321879.340551583</v>
       </c>
     </row>
     <row r="8">
@@ -3403,7 +3479,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>2213776.319943493</v>
+        <v>2212094.740769776</v>
       </c>
     </row>
     <row r="9">
@@ -3437,7 +3513,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.08347205837135982</v>
+        <v>0.08354485235901765</v>
       </c>
     </row>
     <row r="10">
@@ -3471,7 +3547,7 @@
         </is>
       </c>
       <c r="K10" s="2" t="n">
-        <v>1.470514842852498</v>
+        <v>1.470145169926236</v>
       </c>
     </row>
     <row r="11">
@@ -3489,7 +3565,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02348417555779338</v>
+        <v>0.02298110575827635</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3505,7 +3581,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.08174918027359299</v>
+        <v>0.08285045328569222</v>
       </c>
     </row>
     <row r="12">
@@ -3593,7 +3669,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>13.05997572107227</v>
+        <v>13.2021471196634</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -3601,7 +3677,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>33344657.13827862</v>
+        <v>32844119.86026673</v>
       </c>
     </row>
     <row r="15">
@@ -3660,7 +3736,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>19.20488814513003</v>
+        <v>19.40907282062873</v>
       </c>
     </row>
     <row r="17">
@@ -3686,7 +3762,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>277869.3565298968</v>
+        <v>277385.3433427833</v>
       </c>
     </row>
     <row r="18">
@@ -3712,7 +3788,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>765.4493908649923</v>
+        <v>764.1160749988813</v>
       </c>
     </row>
     <row r="19">
@@ -3738,7 +3814,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>47.92022717595334</v>
+        <v>47.8784735032002</v>
       </c>
     </row>
     <row r="20">
@@ -3764,7 +3840,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>15.97340905865111</v>
+        <v>15.9594911677334</v>
       </c>
     </row>
     <row r="21">
@@ -3790,7 +3866,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.1817593407397727</v>
+        <v>0.1806022706747688</v>
       </c>
     </row>
     <row r="22">
@@ -3811,7 +3887,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23"/>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>1.260616536384089</v>
+      </c>
+    </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
@@ -3823,16 +3908,6 @@
           <t>General States</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>Design 4</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3843,13 +3918,15 @@
       <c r="B25" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>0.4</v>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Design 4</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -3863,11 +3940,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="27">
@@ -3881,110 +3958,136 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>viscosity_air [m²/s]</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1.48e-05</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>dihedral [deg]</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E28" s="2" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rho_air</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1.225</v>
+      </c>
+      <c r="D29" t="inlineStr">
         <is>
           <t>sweep_x_c [deg]</t>
         </is>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E29" s="2" t="n">
         <v>4.085616779974877</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>22.81915579807302</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>9.127662319229209</v>
+        <v>22.56491680584854</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>10.26862010913286</v>
+        <v>9.025966722339415</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>21.05644</v>
+        <v>10.15421256263184</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>20.32296713506194</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>16.95137287856853</v>
+        <v>20.33113910266916</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>765.4493908649923</v>
+        <v>16.76250962720177</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>47.92022717595334</v>
+        <v>748.4879415686523</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>47.38632529228192</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E38" s="2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance CG Range Calculation and Update Design Files
- Added xcg_OEW and xcg_payload parameters to design JSON files (design2.json, design3.json, design4.json).
- Implemented CGRange class to calculate center of gravity range based on various load cases (OEW, OEW_PAYLOAD, OEW_PAYLOAD_FUEL, OEW_FUEL).
- Updated CG range attributes in the aircraft data structure to include most forward CG and corresponding mission.
- Removed unnecessary print statements from Iteration.py for cleaner output.
- Integrated CGRange calculation into the main execution flow in __main__.py.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -426,990 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="23" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="22" customWidth="1" min="11" max="11"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Requirements</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Inputs</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>General Outputs</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Design Mission</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>design_range [m]</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>3704000</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>cruise_altitude [m]</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>d_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>8.832726010325398</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>MTOW [N]</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2526797.733125615</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>design_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aircraft_type</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>PROP</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>r_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>4.416363005162699</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>383533.5386328679</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>design_crew</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>wing_type</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>l_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>75.07817108776588</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>1253668.146759622</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ferry_range [m]</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>12038000</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>n_wings</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>l_tailcone [m]</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>39.74726704646429</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>EW [N]</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>1253243.146759622</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ferry_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>n_fuselages</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>l_nose [m]</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>13.2490890154881</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>ZFW [N]</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>2143264.194492748</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>reserve_range [m]</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>185200</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>depth</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>l_cargo_straight [m]</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>15.31635142406773</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>h_b</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>0.04748662882282242</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ferry_crew</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>jet_consumption [kg/(N·s)]</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>2.7e-05</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>LD_g</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>16.55882593020626</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>1.751536698492476</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>altitude_range_WIG [m]</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>943600</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>prop_consumption [kg/J]</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>2.1e-08</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>4850602117.146465</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>WP [N/W]</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>0.09385590949149301</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>altitude_range_WOG [m]</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>538000</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>prop_efficiency</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Cd</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>0.00126964877111443</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>altitude_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Cd0</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02434723936958912</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>hull_surface [m²]</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>297.9879596426425</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>3561.173893518813</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>altitude_crew</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>oswald_factor</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>take_off_power [W]</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>61104505.81607803</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>P [W]</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>26922095.22890662</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>cruise_speed [m/s]</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>115.749</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>take_off_thrust [N]</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>T [N]</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>stall_speed_clean [m/s]</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>77.16</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>tfo</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>V_lof [m/s]</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>64.995</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>LD</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>29.00339130070508</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>stall_speed_takeoff [m/s]</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>max_fuel</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>421886.8924961548</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>stall_speed_landing [m/s]</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>n_engines</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>Empennage Design</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>376889.3864231915</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>stall_speed_high</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>82.3</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CLmax_clean</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>6644.152209676395</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>high_altitude [m]</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>3048</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>CLmax_takeoff</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>fuel_mission [N]</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>376889.3864231915</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>cargo_width [m]</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CLmax_landing</t>
-        </is>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>fuel_reserve [N]</t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>6644.152209676395</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>cargo_height [m]</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>r_float</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>MTOM [kg]</t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>257573.6731014898</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>cargo_length [m]</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>upsweep</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>709.5406872445589</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>cargo_density [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>160</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>84.23423812468175</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>xcg_OEW</t>
-        </is>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>8.423423812468174</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>General States</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>xcg_payload</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>fuel_economy [L/ton/km]</t>
-        </is>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>0.1371177552622408</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>design_id</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>1253668.146759622</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>kinematic_viscosity [m²/s]</t>
-        </is>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>1.006e-06</v>
-      </c>
-      <c r="D26" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="E26" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>383533.5386328679</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>rho_water [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>max_fuel</t>
-        </is>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>421886.8924961548</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
-      <c r="K28" s="2" t="n">
-        <v>376889.3864231915</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>6644.152209676395</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>2.454031674527076</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>12.03345745164756</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>4.813382980659023</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>18.05018617747134</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>X_LEMAC [m]</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>21.05644</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>X_LE [m]</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>20.28286059239409</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>8.9391398212239</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>709.5400813789993</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>84.23420216153289</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1433,7 +450,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1443,7 +460,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -1453,7 +470,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -1463,7 +480,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -1487,6 +504,979 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>d_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>8.832726010325398</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>2526797.733806802</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>design_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>aircraft_type</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>PROP</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>r_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>4.416363005162699</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>383533.5390728101</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>design_crew</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>wing_type</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>l_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>75.07817108776588</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>1253668.147000185</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ferry_range [m]</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>12038000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>n_wings</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>l_tailcone [m]</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>39.74726704646429</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>EW [N]</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>1253243.147000185</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ferry_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>n_fuselages</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>l_nose [m]</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>13.2490890154881</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ZFW [N]</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>2143264.194733992</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>reserve_range [m]</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>185200</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>l_cargo_straight [m]</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>15.31635142406773</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>h_b</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0.04748662917987374</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ferry_crew</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jet_consumption [kg/(N·s)]</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>2.7e-05</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>LD_g</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>16.55882593020626</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>1.751536694157919</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>altitude_range_WIG [m]</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>943600</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>prop_consumption [kg/J]</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>2.1e-08</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Re</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>4850602117.146465</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>WP [N/W]</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0.09385590949149301</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>altitude_range_WOG [m]</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>538000</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>prop_efficiency</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0.00126964877111443</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>altitude_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Cd0</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.02434723936958912</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>hull_surface [m²]</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>297.9879596426425</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WS [N/m²]</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>3561.173893518813</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>altitude_crew</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>oswald_factor</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>take_off_power [W]</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>61104505.81607803</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>26922095.23616441</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cruise_speed [m/s]</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>115.749</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>take_off_thrust [N]</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>T [N]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>stall_speed_clean [m/s]</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>77.16</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tfo</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>V_lof [m/s]</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>64.995</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>29.0033912289299</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>stall_speed_takeoff [m/s]</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>421886.8929800912</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>stall_speed_landing [m/s]</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>n_engines</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>Empennage Design</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>376889.3868459184</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>stall_speed_high</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CLmax_clean</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>6644.152226891718</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>high_altitude [m]</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>3048</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CLmax_takeoff</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>fuel_mission [N]</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>376889.3868459184</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cargo_width [m]</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CLmax_landing</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>fuel_reserve [N]</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>6644.152226891718</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>cargo_height [m]</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>r_float</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>MTOM [kg]</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>257573.6731709278</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>cargo_length [m]</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>upsweep</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>709.5406765745053</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>cargo_density [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>xcg_OEW</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>84.23423749132566</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>8.423423749132565</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>General States</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>0.1371177554160349</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>design_id</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>1253668.147000185</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>kinematic_viscosity [m²/s]</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>1.006e-06</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>383533.5390728101</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>rho_water [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>421886.8929800912</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>dihedral [deg]</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>376889.3868459184</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>sweep_x_c [deg]</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>2.454031674527076</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>6644.152226891718</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>chord_root [m]</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>12.03346249876081</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>chord_tip [m]</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>4.813384999504322</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>y_MAC [m]</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>18.05019374814121</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>21.05644</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>20.28286026793681</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>8.939143570508026</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>709.5406765745048</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>84.23423749132563</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="8" max="8"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Requirements</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Inputs</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>General Outputs</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Design Mission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>design_range [m]</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>3704000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>cruise_altitude [m]</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>8</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -1503,7 +1493,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2603249.452963894</v>
+        <v>2603249.387910605</v>
       </c>
     </row>
     <row r="3">
@@ -1539,7 +1529,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>432909.6404852453</v>
+        <v>432909.5984707839</v>
       </c>
     </row>
     <row r="4">
@@ -1575,7 +1565,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1280667.313025685</v>
+        <v>1280667.290051911</v>
       </c>
     </row>
     <row r="5">
@@ -1609,7 +1599,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1280242.313025685</v>
+        <v>1280242.290051911</v>
       </c>
     </row>
     <row r="6">
@@ -1643,7 +1633,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2170339.812478649</v>
+        <v>2170339.789439821</v>
       </c>
     </row>
     <row r="7">
@@ -1677,7 +1667,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.09355038271687469</v>
+        <v>0.09355032286008742</v>
       </c>
     </row>
     <row r="8">
@@ -1711,7 +1701,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.423759080105479</v>
+        <v>1.423759333681073</v>
       </c>
     </row>
     <row r="9">
@@ -1841,7 +1831,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>28646640.80558365</v>
+        <v>28646640.08972517</v>
       </c>
     </row>
     <row r="13">
@@ -1906,7 +1896,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>23.63708119190135</v>
+        <v>23.63708540173361</v>
       </c>
     </row>
     <row r="15">
@@ -1932,7 +1922,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>476200.6045337698</v>
+        <v>476200.5583178623</v>
       </c>
     </row>
     <row r="16">
@@ -1968,7 +1958,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>424348.4436983753</v>
+        <v>424348.4033025702</v>
       </c>
     </row>
     <row r="17">
@@ -1994,7 +1984,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>8561.196786870016</v>
+        <v>8561.195168213628</v>
       </c>
     </row>
     <row r="18">
@@ -2020,7 +2010,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>424348.4436983753</v>
+        <v>424348.4033025702</v>
       </c>
     </row>
     <row r="19">
@@ -2046,7 +2036,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>8561.196786870016</v>
+        <v>8561.195168213628</v>
       </c>
     </row>
     <row r="20">
@@ -2072,7 +2062,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>265366.9167139545</v>
+        <v>265366.9100826305</v>
       </c>
     </row>
     <row r="21">
@@ -2098,7 +2088,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>731.2886565629583</v>
+        <v>731.2895923716698</v>
       </c>
     </row>
     <row r="22">
@@ -2112,11 +2102,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>xcg_OEW</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>1.227309481885543</v>
+        <v>0.45</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2124,17 +2114,25 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>85.51541712246735</v>
+        <v>85.51547183823929</v>
       </c>
     </row>
     <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.55</v>
+      </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>MAC [m]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>8.551541712246735</v>
+        <v>8.55154718382393</v>
       </c>
     </row>
     <row r="24">
@@ -2148,23 +2146,13 @@
           <t>General States</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.1543840398403063</v>
+        <v>0.154384025143734</v>
       </c>
     </row>
     <row r="25">
@@ -2176,13 +2164,15 @@
       <c r="B25" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>0.4</v>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2190,7 +2180,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>1280667.313025685</v>
+        <v>1280667.290051911</v>
       </c>
     </row>
     <row r="26">
@@ -2204,11 +2194,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E26" s="3" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.4</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2216,7 +2206,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>432909.6404852453</v>
+        <v>432909.5984707839</v>
       </c>
     </row>
     <row r="27">
@@ -2230,11 +2220,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>1</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2242,17 +2232,17 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>476200.6045337698</v>
+        <v>476200.5583178623</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>2.454031674527076</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2260,17 +2250,17 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>424348.4436983753</v>
+        <v>424348.4033025702</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>12.21689625881637</v>
+        <v>2.454031674527076</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2278,86 +2268,96 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>8561.196786870016</v>
+        <v>8561.195168213628</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>4.88675850352655</v>
+        <v>12.21649597689135</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>18.32534438822456</v>
+        <v>4.886598390756541</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>21.05644</v>
+        <v>18.32474396533703</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>20.27106809764752</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>9.075408649406448</v>
+        <v>20.27109383005699</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>731.3375155735392</v>
+        <v>9.075111297119291</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>85.51827381171461</v>
+        <v>731.2895923716725</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>85.51547183823945</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E38" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2372,7 +2372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2466,7 +2466,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2655398.509468844</v>
+        <v>2655398.417425396</v>
       </c>
     </row>
     <row r="3">
@@ -2502,7 +2502,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>466589.943962271</v>
+        <v>466589.8845163012</v>
       </c>
     </row>
     <row r="4">
@@ -2538,7 +2538,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1299083.916997104</v>
+        <v>1299083.88449167</v>
       </c>
     </row>
     <row r="5">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1298658.916997104</v>
+        <v>1298658.88449167</v>
       </c>
     </row>
     <row r="6">
@@ -2606,7 +2606,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2188808.565506573</v>
+        <v>2188808.532909095</v>
       </c>
     </row>
     <row r="7">
@@ -2640,7 +2640,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.1157729246623674</v>
+        <v>0.1157728281678391</v>
       </c>
     </row>
     <row r="8">
@@ -2674,7 +2674,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.344658286687761</v>
+        <v>1.344658575433679</v>
       </c>
     </row>
     <row r="9">
@@ -2804,7 +2804,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32689406.32652793</v>
+        <v>32689405.19342281</v>
       </c>
     </row>
     <row r="13">
@@ -2869,7 +2869,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>20.72035345398719</v>
+        <v>20.72035790338339</v>
       </c>
     </row>
     <row r="15">
@@ -2895,7 +2895,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>513248.9383584982</v>
+        <v>513248.8729679313</v>
       </c>
     </row>
     <row r="16">
@@ -2931,7 +2931,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>456737.7799561748</v>
+        <v>456737.7227772949</v>
       </c>
     </row>
     <row r="17">
@@ -2957,7 +2957,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>9852.164006096194</v>
+        <v>9852.161739006231</v>
       </c>
     </row>
     <row r="18">
@@ -2983,7 +2983,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>456737.7799561748</v>
+        <v>456737.7227772949</v>
       </c>
     </row>
     <row r="19">
@@ -3009,7 +3009,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>9852.164006096194</v>
+        <v>9852.161739006231</v>
       </c>
     </row>
     <row r="20">
@@ -3035,7 +3035,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>270682.824614561</v>
+        <v>270682.8152319466</v>
       </c>
     </row>
     <row r="21">
@@ -3061,7 +3061,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>746.0810181822919</v>
+        <v>746.0822618724924</v>
       </c>
     </row>
     <row r="22">
@@ -3087,17 +3087,17 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>86.37598151004084</v>
+        <v>86.3760535028368</v>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>xcg_OEW</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>1.177237829663066</v>
+        <v>0.45</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -3105,7 +3105,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>8.637598151004086</v>
+        <v>8.637605350283678</v>
       </c>
     </row>
     <row r="24">
@@ -3119,13 +3119,21 @@
           <t>General States</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.55</v>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.1661677441368147</v>
+        <v>0.1661677233343195</v>
       </c>
     </row>
     <row r="25">
@@ -3137,23 +3145,13 @@
       <c r="B25" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D25" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>OEW [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>1299083.916997104</v>
+        <v>1299083.88449167</v>
       </c>
     </row>
     <row r="26">
@@ -3165,13 +3163,15 @@
       <c r="B26" s="4" t="n">
         <v>1.006e-06</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.4</v>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3179,7 +3179,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>466589.943962271</v>
+        <v>466589.8845163012</v>
       </c>
     </row>
     <row r="27">
@@ -3193,11 +3193,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.4</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3205,17 +3205,17 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>513248.9383584982</v>
+        <v>513248.8729679313</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>1</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3223,17 +3223,17 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>456737.7799561748</v>
+        <v>456737.7227772949</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>2.454031674527076</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3241,96 +3241,106 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>9852.164006096194</v>
+        <v>9852.161739006231</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>12.33993082307322</v>
+        <v>2.454031674527076</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>4.935972329229287</v>
+        <v>12.33943621468901</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>18.50989623460983</v>
+        <v>4.935774485875602</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>21.05644</v>
+        <v>18.50915432203351</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>20.26315873280244</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>9.16680575428296</v>
+        <v>20.26319052905571</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>746.1420743193388</v>
+        <v>9.166438330911831</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>86.37951576151251</v>
+        <v>746.0822618722547</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>86.37605350282303</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E39" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3345,7 +3355,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3439,7 +3449,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2674226.74656556</v>
+        <v>2674226.592120333</v>
       </c>
     </row>
     <row r="3">
@@ -3475,7 +3485,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>478750.1014388424</v>
+        <v>478750.0016908801</v>
       </c>
     </row>
     <row r="4">
@@ -3511,7 +3521,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1305733.168380152</v>
+        <v>1305733.113837333</v>
       </c>
     </row>
     <row r="5">
@@ -3545,7 +3555,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1305308.168380152</v>
+        <v>1305308.113837333</v>
       </c>
     </row>
     <row r="6">
@@ -3579,7 +3589,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2195476.645126718</v>
+        <v>2195476.590429453</v>
       </c>
     </row>
     <row r="7">
@@ -3613,7 +3623,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.08427472982981841</v>
+        <v>0.08427462970031621</v>
       </c>
     </row>
     <row r="8">
@@ -3647,7 +3657,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.466466636899135</v>
+        <v>1.466467138075632</v>
       </c>
     </row>
     <row r="9">
@@ -3777,7 +3787,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32712581.79734191</v>
+        <v>32712579.90808471</v>
       </c>
     </row>
     <row r="13">
@@ -3842,7 +3852,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>19.15201867366521</v>
+        <v>19.15202521901809</v>
       </c>
     </row>
     <row r="15">
@@ -3868,7 +3878,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>526625.1115827266</v>
+        <v>526625.0018599682</v>
       </c>
     </row>
     <row r="16">
@@ -3904,7 +3914,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>468435.0153135352</v>
+        <v>468434.9193560873</v>
       </c>
     </row>
     <row r="17">
@@ -3930,7 +3940,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>10315.08612530719</v>
+        <v>10315.08233479282</v>
       </c>
     </row>
     <row r="18">
@@ -3956,7 +3966,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>468435.0153135352</v>
+        <v>468434.9193560873</v>
       </c>
     </row>
     <row r="19">
@@ -3982,7 +3992,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>10315.08612530719</v>
+        <v>10315.08233479282</v>
       </c>
     </row>
     <row r="20">
@@ -4008,7 +4018,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>272602.1148384873</v>
+        <v>272602.0990948352</v>
       </c>
     </row>
     <row r="21">
@@ -4034,7 +4044,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>750.9378416827169</v>
+        <v>750.9396261124369</v>
       </c>
     </row>
     <row r="22">
@@ -4060,17 +4070,17 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>47.46381279509845</v>
+        <v>47.46386918843965</v>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>xcg_OEW</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>1.260100167347354</v>
+        <v>0.45</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -4078,7 +4088,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>15.82127093169948</v>
+        <v>15.82128972947988</v>
       </c>
     </row>
     <row r="24">
@@ -4092,13 +4102,21 @@
           <t>General States</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.55</v>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.1704233658464014</v>
+        <v>0.170423330935708</v>
       </c>
     </row>
     <row r="25">
@@ -4110,23 +4128,13 @@
       <c r="B25" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D25" s="1" t="inlineStr">
-        <is>
-          <t>Design 4</t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>OEW [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>1305733.168380152</v>
+        <v>1305733.113837333</v>
       </c>
     </row>
     <row r="26">
@@ -4138,13 +4146,15 @@
       <c r="B26" s="4" t="n">
         <v>1.006e-06</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.4</v>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Design 4</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -4152,7 +4162,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>478750.1014388424</v>
+        <v>478750.0016908801</v>
       </c>
     </row>
     <row r="27">
@@ -4166,11 +4176,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.4</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -4178,17 +4188,17 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>526625.1115827266</v>
+        <v>526625.0018599682</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>5</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -4196,17 +4206,17 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>468435.0153135352</v>
+        <v>468434.9193560873</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>4.085616779974877</v>
+        <v>5</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -4214,96 +4224,106 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>10315.08612530719</v>
+        <v>10315.08233479282</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>22.60294740932848</v>
+        <v>4.085616779974877</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>9.041178963731394</v>
+        <v>22.60184247067595</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>10.17132633419781</v>
+        <v>9.04073698827038</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>21.05644</v>
+        <v>10.17082911180418</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>20.32991669041444</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>16.79076093264402</v>
+        <v>20.3299522062997</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>751.0130504356373</v>
+        <v>16.78994012107356</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>47.4661895595898</v>
+        <v>750.9396261117989</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>47.46386918841949</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E39" s="2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor aircraft data handling and calculations
- Updated ClassIWeightEstimation.py to include Raymers comment for clarity.
- Modified design JSON files (design1.json, design2.json, design3.json, design4.json) to adjust various parameters including xcg_OEW, fuel economy, and added new fields V_h and V_v.
- Enhanced Iteration.py to include Mff in outputs and adjusted fuel economy calculations for design and altitude missions.
- Integrated Empennage class in __main__.py and added tail area calculations based on updated CG range.
- Cleaned up CGRange class to streamline mass component calculations.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -426,7 +426,1016 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="8" max="8"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Requirements</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Inputs</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>General Outputs</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Design Mission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>design_range [m]</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>3704000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>cruise_altitude [m]</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>d_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>8.832726010325398</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>2526797.733806803</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>design_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>aircraft_type</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>PROP</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>r_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>4.416363005162699</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>383533.5390728108</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>design_crew</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>wing_type</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>l_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>75.07817108776588</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>1253668.147000186</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ferry_range [m]</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>12038000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>n_wings</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>l_tailcone [m]</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>39.74726704646429</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>EW [N]</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>1253243.147000186</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ferry_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>n_fuselages</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>l_nose [m]</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>13.2490890154881</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ZFW [N]</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>2143264.194733993</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>reserve_range [m]</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>185200</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>l_cargo_straight [m]</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>15.31635142406773</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>h_b</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0.04748662917987376</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ferry_crew</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jet_consumption [kg/(N·s)]</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>2.7e-05</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>LD_g</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>16.55882593020626</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>1.751536694157918</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>altitude_range_WIG [m]</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>943600</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>prop_consumption [kg/J]</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>2.1e-08</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Re</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>4850602117.146465</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>WP [N/W]</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0.09385590949149301</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>altitude_range_WOG [m]</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>538000</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>prop_efficiency</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0.00126964877111443</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>altitude_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Cd0</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.02434723936958912</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>hull_surface [m²]</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>297.9879596426425</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WS [N/m²]</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>3561.173893518813</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>altitude_crew</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>oswald_factor</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>take_off_power [W]</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>61104505.81607803</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>26922095.23616442</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cruise_speed [m/s]</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>115.749</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>take_off_thrust [N]</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>T [N]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>stall_speed_clean [m/s]</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>77.16</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tfo</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>V_lof [m/s]</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>64.995</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>29.0033912289299</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>stall_speed_takeoff [m/s]</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>421886.892980092</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>stall_speed_landing [m/s]</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>n_engines</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>Empennage Design</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>376889.3868459186</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>stall_speed_high</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CLmax_clean</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>6644.152226892242</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>high_altitude [m]</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>3048</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CLmax_takeoff</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>fuel_mission [N]</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>376889.3868459186</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cargo_width [m]</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CLmax_landing</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>fuel_reserve [N]</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>6644.152226892242</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>cargo_height [m]</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>r_float</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0.8482135970198968</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>cargo_length [m]</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>upsweep</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>MTOM [kg]</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>257573.6731709279</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>cargo_density [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>xcg_OEW</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>709.5406765745048</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>84.23423749132563</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>General States</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>V_h</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>8.423423749132562</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>design_id</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.0838</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>0.06855887770801748</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>kinematic_viscosity [m²/s]</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>1.006e-06</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>1253668.147000186</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>rho_water [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>383533.5390728108</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>421886.892980092</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>376889.3868459186</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>dihedral [deg]</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>6644.152226892242</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>sweep_x_c [deg]</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>2.454031674527076</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0.8405231473353731</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>chord_root [m]</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>12.03346249876081</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>chord_tip [m]</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>4.813384999504324</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>y_MAC [m]</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>18.05019374814121</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>21.05644</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>20.28286026793681</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>8.939143570508028</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>709.5406765745053</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>84.23423749132566</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +1459,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Design 1</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -460,7 +1469,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Design 1</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -470,7 +1479,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Design 1</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -480,7 +1489,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Design 1</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -504,7 +1513,7 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -512,7 +1521,7 @@
         </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>8.832726010325398</v>
+        <v>6.204804790550249</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -520,7 +1529,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2526797.733806802</v>
+        <v>2603249.387910605</v>
       </c>
     </row>
     <row r="3">
@@ -548,7 +1557,7 @@
         </is>
       </c>
       <c r="H3" s="2" t="n">
-        <v>4.416363005162699</v>
+        <v>3.102402395275125</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -556,7 +1565,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>383533.5390728101</v>
+        <v>432909.5984707839</v>
       </c>
     </row>
     <row r="4">
@@ -575,7 +1584,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>LOW</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -584,7 +1593,7 @@
         </is>
       </c>
       <c r="H4" s="2" t="n">
-        <v>75.07817108776588</v>
+        <v>52.74084071967712</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -592,7 +1601,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1253668.147000185</v>
+        <v>1280667.290051911</v>
       </c>
     </row>
     <row r="5">
@@ -618,7 +1627,7 @@
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>39.74726704646429</v>
+        <v>27.92162155747612</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -626,17 +1635,17 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1253243.147000185</v>
+        <v>1280242.290051911</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ferry_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
+          <t>reserve_range [m]</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>185200</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -644,7 +1653,7 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -652,7 +1661,7 @@
         </is>
       </c>
       <c r="H6" s="2" t="n">
-        <v>13.2490890154881</v>
+        <v>9.307207185825375</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -660,17 +1669,17 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2143264.194733992</v>
+        <v>2170339.789439821</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>reserve_range [m]</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>185200</v>
+          <t>ferry_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -678,7 +1687,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -686,7 +1695,7 @@
         </is>
       </c>
       <c r="H7" s="2" t="n">
-        <v>15.31635142406773</v>
+        <v>8.74654837462985</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -694,7 +1703,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.04748662917987374</v>
+        <v>0.0935503228600874</v>
       </c>
     </row>
     <row r="8">
@@ -716,11 +1725,11 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>LD_g</t>
+          <t>Re</t>
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>16.55882593020626</v>
+        <v>3407446264.985502</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -728,7 +1737,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.751536694157919</v>
+        <v>1.423759333681073</v>
       </c>
     </row>
     <row r="9">
@@ -750,11 +1759,11 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Re</t>
+          <t>Cd</t>
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>4850602117.146465</v>
+        <v>0.001321877371153106</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -762,7 +1771,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.09385590949149301</v>
+        <v>0.09087451023075915</v>
       </c>
     </row>
     <row r="10">
@@ -780,15 +1789,15 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.85</v>
+        <v>0.82</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>hull_surface [m²]</t>
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.00126964877111443</v>
+        <v>210.4204947871738</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -811,15 +1820,15 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02434723936958912</v>
+        <v>0.02422111472806403</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>hull_surface [m²]</t>
+          <t>take_off_power [W]</t>
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>297.9879596426425</v>
+        <v>93133344.13863601</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -827,7 +1836,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>3561.173893518813</v>
+        <v>3559.80642288087</v>
       </c>
     </row>
     <row r="12">
@@ -849,11 +1858,8 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>take_off_power [W]</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>61104505.81607803</v>
+          <t>take_off_thrust [N]</t>
+        </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -861,7 +1867,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>26922095.23616441</v>
+        <v>28646640.08972517</v>
       </c>
     </row>
     <row r="13">
@@ -883,8 +1889,11 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>take_off_thrust [N]</t>
-        </is>
+          <t>V_lof [m/s]</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>64.995</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -911,11 +1920,11 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>V_lof [m/s]</t>
+          <t>LD_g</t>
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>64.995</v>
+        <v>16.6018826655351</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -923,7 +1932,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>29.0033912289299</v>
+        <v>23.63708540173361</v>
       </c>
     </row>
     <row r="15">
@@ -949,7 +1958,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>421886.8929800912</v>
+        <v>476200.5583178623</v>
       </c>
     </row>
     <row r="16">
@@ -971,7 +1980,7 @@
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>Design 1</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="H16" s="1" t="inlineStr">
@@ -985,7 +1994,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>376889.3868459184</v>
+        <v>424348.4033025702</v>
       </c>
     </row>
     <row r="17">
@@ -1011,7 +2020,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>6644.152226891718</v>
+        <v>8561.195168213628</v>
       </c>
     </row>
     <row r="18">
@@ -1037,7 +2046,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>376889.3868459184</v>
+        <v>424348.4033025702</v>
       </c>
     </row>
     <row r="19">
@@ -1063,7 +2072,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>6644.152226891718</v>
+        <v>8561.195168213628</v>
       </c>
     </row>
     <row r="20">
@@ -1081,15 +2090,15 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>4.4</v>
+        <v>3.1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>257573.6731709278</v>
+        <v>0.8337041389575658</v>
       </c>
     </row>
     <row r="21">
@@ -1111,11 +2120,11 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>709.5406765745053</v>
+        <v>265366.9100826305</v>
       </c>
     </row>
     <row r="22">
@@ -1133,15 +2142,15 @@
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>84.23423749132566</v>
+        <v>731.2895923716702</v>
       </c>
     </row>
     <row r="23">
@@ -1155,17 +2164,17 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>8.423423749132565</v>
+        <v>85.51547183823932</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Design 1</t>
+          <t>Design 2</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
@@ -1173,13 +2182,21 @@
           <t>General States</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>V_h</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.9</v>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.1371177554160349</v>
+        <v>8.551547183823931</v>
       </c>
     </row>
     <row r="25">
@@ -1189,25 +2206,23 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.0838</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>1253668.147000185</v>
+        <v>0.077192012571867</v>
       </c>
     </row>
     <row r="26">
@@ -1219,21 +2234,13 @@
       <c r="B26" s="4" t="n">
         <v>1.006e-06</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.4</v>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>383533.5390728101</v>
+        <v>1280667.290051911</v>
       </c>
     </row>
     <row r="27">
@@ -1245,1119 +2252,192 @@
       <c r="B27" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>0</v>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>max_fuel</t>
+          <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>421886.8929800912</v>
+        <v>432909.5984707839</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
+          <t>taper_ratio</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>5</v>
+        <v>0.4</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>mission_fuel</t>
+          <t>max_fuel</t>
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>376889.3868459184</v>
+        <v>476200.5583178623</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>2.454031674527076</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>mission_fuel</t>
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>6644.152226891718</v>
+        <v>424348.4033025702</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>12.03346249876081</v>
+        <v>1</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>8561.195168213628</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>4.813384999504322</v>
+        <v>2.454031674527076</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0.8177207555495544</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>18.05019374814121</v>
+        <v>12.21649597689133</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>1720912.57500321</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>21.05644</v>
+        <v>4.886598390756532</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>20.28286026793681</v>
+        <v>18.324743965337</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>8.939143570508026</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>709.5406765745048</v>
+        <v>20.27109383005699</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>84.23423749132563</v>
+        <v>9.075111297119275</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>731.2895923716702</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>85.51547183823932</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="23" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Requirements</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Inputs</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>General Outputs</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Design Mission</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>design_range [m]</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>3704000</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>cruise_altitude [m]</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>d_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>6.204804790550249</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>MTOW [N]</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2603249.387910605</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>design_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aircraft_type</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>PROP</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>r_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>3.102402395275125</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>432909.5984707839</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>design_crew</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>wing_type</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>l_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>52.74084071967712</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>1280667.290051911</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ferry_range [m]</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>12038000</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>n_wings</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>l_tailcone [m]</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>27.92162155747612</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>EW [N]</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>1280242.290051911</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>reserve_range [m]</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>185200</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>n_fuselages</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>l_nose [m]</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>9.307207185825375</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>ZFW [N]</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>2170339.789439821</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ferry_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>depth</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>l_cargo_straight [m]</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>8.74654837462985</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>h_b</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>0.09355032286008742</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ferry_crew</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>jet_consumption [kg/(N·s)]</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>2.7e-05</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>3407446264.985502</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>1.423759333681073</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>altitude_range_WIG [m]</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>943600</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>prop_consumption [kg/J]</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>2.1e-08</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Cd</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>0.001321877371153106</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>WP [N/W]</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>0.09087451023075915</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>altitude_range_WOG [m]</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>538000</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>prop_efficiency</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>hull_surface [m²]</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>210.4204947871738</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>altitude_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Cd0</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02422111472806403</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>take_off_power [W]</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>93133344.13863601</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>3559.80642288087</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>altitude_crew</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>oswald_factor</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>take_off_thrust [N]</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>P [W]</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>28646640.08972517</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>cruise_speed [m/s]</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>115.749</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>V_lof [m/s]</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>64.995</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>T [N]</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>stall_speed_clean [m/s]</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>77.16</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>tfo</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>LD_g</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>16.6018826655351</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>LD</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>23.63708540173361</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>stall_speed_takeoff [m/s]</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>max_fuel</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>476200.5583178623</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>stall_speed_landing [m/s]</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>n_engines</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>Empennage Design</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>424348.4033025702</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>stall_speed_high</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>82.3</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CLmax_clean</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>8561.195168213628</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>high_altitude [m]</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>3048</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>CLmax_takeoff</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>fuel_mission [N]</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>424348.4033025702</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>cargo_width [m]</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CLmax_landing</t>
-        </is>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>fuel_reserve [N]</t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>8561.195168213628</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>cargo_height [m]</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>r_float</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>MTOM [kg]</t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>265366.9100826305</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>cargo_length [m]</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>upsweep</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>731.2895923716698</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>cargo_density [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>160</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>xcg_OEW</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>85.51547183823929</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>xcg_payload</t>
-        </is>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>8.55154718382393</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>General States</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>fuel_economy [L/ton/km]</t>
-        </is>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>0.154384025143734</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>design_id</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>1280667.290051911</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>kinematic_viscosity [m²/s]</t>
-        </is>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>1.006e-06</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>432909.5984707839</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>rho_water [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>max_fuel</t>
-        </is>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>476200.5583178623</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
-      <c r="K28" s="2" t="n">
-        <v>424348.4033025702</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>2.454031674527076</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>8561.195168213628</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>12.21649597689135</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>4.886598390756541</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>18.32474396533703</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>X_LEMAC [m]</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>21.05644</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>X_LE [m]</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>20.27109383005699</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>9.075111297119291</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>731.2895923716725</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>85.51547183823945</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E38" s="2" t="n">
+      <c r="E40" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2372,7 +2452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2466,7 +2546,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2655398.417425396</v>
+        <v>2655398.417425397</v>
       </c>
     </row>
     <row r="3">
@@ -2502,7 +2582,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>466589.8845163012</v>
+        <v>466589.8845163019</v>
       </c>
     </row>
     <row r="4">
@@ -2640,7 +2720,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.1157728281678391</v>
+        <v>0.1157728281678395</v>
       </c>
     </row>
     <row r="8">
@@ -2674,7 +2754,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.344658575433679</v>
+        <v>1.344658575433678</v>
       </c>
     </row>
     <row r="9">
@@ -2804,7 +2884,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32689405.19342281</v>
+        <v>32689405.19342282</v>
       </c>
     </row>
     <row r="13">
@@ -2869,7 +2949,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>20.72035790338339</v>
+        <v>20.72035790338338</v>
       </c>
     </row>
     <row r="15">
@@ -2895,7 +2975,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>513248.8729679313</v>
+        <v>513248.8729679321</v>
       </c>
     </row>
     <row r="16">
@@ -2931,7 +3011,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>456737.7227772949</v>
+        <v>456737.7227772951</v>
       </c>
     </row>
     <row r="17">
@@ -2957,7 +3037,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>9852.161739006231</v>
+        <v>9852.161739006755</v>
       </c>
     </row>
     <row r="18">
@@ -2983,7 +3063,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>456737.7227772949</v>
+        <v>456737.7227772951</v>
       </c>
     </row>
     <row r="19">
@@ -3009,7 +3089,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>9852.161739006231</v>
+        <v>9852.161739006755</v>
       </c>
     </row>
     <row r="20">
@@ -3031,11 +3111,11 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>270682.8152319466</v>
+        <v>0.8242862986381174</v>
       </c>
     </row>
     <row r="21">
@@ -3057,11 +3137,11 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>746.0822618724924</v>
+        <v>270682.8152319467</v>
       </c>
     </row>
     <row r="22">
@@ -3083,11 +3163,11 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>86.3760535028368</v>
+        <v>746.0822618724875</v>
       </c>
     </row>
     <row r="23">
@@ -3101,11 +3181,11 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>8.637605350283678</v>
+        <v>86.37605350283651</v>
       </c>
     </row>
     <row r="24">
@@ -3129,11 +3209,11 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.1661677233343195</v>
+        <v>8.63760535028365</v>
       </c>
     </row>
     <row r="25">
@@ -3145,13 +3225,21 @@
       <c r="B25" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>V_h</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.9</v>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>1299083.88449167</v>
+        <v>0.08308386166715977</v>
       </c>
     </row>
     <row r="26">
@@ -3163,23 +3251,21 @@
       <c r="B26" s="4" t="n">
         <v>1.006e-06</v>
       </c>
-      <c r="D26" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="E26" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.0838</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>466589.8845163012</v>
+        <v>1299083.88449167</v>
       </c>
     </row>
     <row r="27">
@@ -3191,156 +3277,194 @@
       <c r="B27" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0.4</v>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>466589.8845163019</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
           <t>max_fuel</t>
         </is>
       </c>
-      <c r="K27" s="2" t="n">
-        <v>513248.8729679313</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
       <c r="K28" s="2" t="n">
-        <v>456737.7227772949</v>
+        <v>513248.8729679321</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
+          <t>taper_ratio</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>mission_fuel</t>
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>9852.161739006231</v>
+        <v>456737.7227772951</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>2.454031674527076</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>9852.161739006755</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>12.33943621468901</v>
+        <v>1</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0.8026824433780242</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>4.935774485875602</v>
+        <v>2.454031674527076</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>1733790.843393344</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>18.50915432203351</v>
+        <v>12.33943621469093</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>21.05644</v>
+        <v>4.935774485876372</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>20.26319052905571</v>
+        <v>18.50915432203639</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>9.166438330911831</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>746.0822618722547</v>
+        <v>20.26319052905558</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>86.37605350282303</v>
+        <v>9.166438330913261</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="inlineStr">
         <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>746.0822618724875</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>86.37605350283651</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E41" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3355,7 +3479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3449,7 +3573,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2674226.592120333</v>
+        <v>2674226.592120334</v>
       </c>
     </row>
     <row r="3">
@@ -3485,7 +3609,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>478750.0016908801</v>
+        <v>478750.0016908805</v>
       </c>
     </row>
     <row r="4">
@@ -3623,7 +3747,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.08427462970031621</v>
+        <v>0.08427462970031709</v>
       </c>
     </row>
     <row r="8">
@@ -3657,7 +3781,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.466467138075632</v>
+        <v>1.466467138075628</v>
       </c>
     </row>
     <row r="9">
@@ -3787,7 +3911,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32712579.90808471</v>
+        <v>32712579.90808472</v>
       </c>
     </row>
     <row r="13">
@@ -3852,7 +3976,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>19.15202521901809</v>
+        <v>19.15202521901804</v>
       </c>
     </row>
     <row r="15">
@@ -3878,7 +4002,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>526625.0018599682</v>
+        <v>526625.0018599686</v>
       </c>
     </row>
     <row r="16">
@@ -3914,7 +4038,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>468434.9193560873</v>
+        <v>468434.919356088</v>
       </c>
     </row>
     <row r="17">
@@ -3940,7 +4064,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>10315.08233479282</v>
+        <v>10315.08233479253</v>
       </c>
     </row>
     <row r="18">
@@ -3966,7 +4090,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>468434.9193560873</v>
+        <v>468434.919356088</v>
       </c>
     </row>
     <row r="19">
@@ -3992,7 +4116,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>10315.08233479282</v>
+        <v>10315.08233479253</v>
       </c>
     </row>
     <row r="20">
@@ -4014,11 +4138,11 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>272602.0990948352</v>
+        <v>0.8209762766171245</v>
       </c>
     </row>
     <row r="21">
@@ -4040,11 +4164,11 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>750.9396261124369</v>
+        <v>272602.0990948352</v>
       </c>
     </row>
     <row r="22">
@@ -4066,11 +4190,11 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>47.46386918843965</v>
+        <v>750.9396261124215</v>
       </c>
     </row>
     <row r="23">
@@ -4084,11 +4208,11 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>15.82128972947988</v>
+        <v>47.46386918843916</v>
       </c>
     </row>
     <row r="24">
@@ -4112,11 +4236,11 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.170423330935708</v>
+        <v>15.82128972947972</v>
       </c>
     </row>
     <row r="25">
@@ -4128,13 +4252,21 @@
       <c r="B25" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>V_h</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.9</v>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>1305733.113837333</v>
+        <v>0.08521166546785409</v>
       </c>
     </row>
     <row r="26">
@@ -4146,23 +4278,21 @@
       <c r="B26" s="4" t="n">
         <v>1.006e-06</v>
       </c>
-      <c r="D26" s="1" t="inlineStr">
-        <is>
-          <t>Design 4</t>
-        </is>
-      </c>
-      <c r="E26" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.0838</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>478750.0016908801</v>
+        <v>1305733.113837333</v>
       </c>
     </row>
     <row r="27">
@@ -4174,156 +4304,194 @@
       <c r="B27" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0.4</v>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>478750.0016908805</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>Design 4</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
           <t>max_fuel</t>
         </is>
       </c>
-      <c r="K27" s="2" t="n">
-        <v>526625.0018599682</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
       <c r="K28" s="2" t="n">
-        <v>468434.9193560873</v>
+        <v>526625.0018599686</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
+          <t>taper_ratio</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>5</v>
+        <v>0.4</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>mission_fuel</t>
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>10315.08233479282</v>
+        <v>468434.919356088</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>4.085616779974877</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>10315.08233479253</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>22.60184247067595</v>
+        <v>5</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0.7940574299257867</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>9.04073698827038</v>
+        <v>4.085616779974877</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>1744319.451377081</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>10.17082911180418</v>
+        <v>22.60184247068532</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>21.05644</v>
+        <v>9.040736988274128</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>20.3299522062997</v>
+        <v>10.17082911180839</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>16.78994012107356</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>750.9396261117989</v>
+        <v>20.3299522062994</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>47.46386918841949</v>
+        <v>16.78994012108052</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="inlineStr">
         <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>750.9396261124215</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>47.46386918843916</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E41" s="2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ferry crew values across design files
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -444,7 +444,7 @@
     <col width="23" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2526797.733806803</v>
+        <v>2526797.733806802</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>383533.5390728108</v>
+        <v>383533.5390728101</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1253668.147000186</v>
+        <v>1253668.147000185</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1253243.147000186</v>
+        <v>1253243.147000185</v>
       </c>
     </row>
     <row r="6">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2143264.194733993</v>
+        <v>2143264.194733992</v>
       </c>
     </row>
     <row r="7">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.04748662917987376</v>
+        <v>0.04748662917987374</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.751536694157918</v>
+        <v>1.751536694157919</v>
       </c>
     </row>
     <row r="9">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>26922095.23616442</v>
+        <v>26922095.23616441</v>
       </c>
     </row>
     <row r="13">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>421886.892980092</v>
+        <v>421886.8929800912</v>
       </c>
     </row>
     <row r="16">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>376889.3868459186</v>
+        <v>376889.3868459184</v>
       </c>
     </row>
     <row r="17">
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>6644.152226892242</v>
+        <v>6644.152226891718</v>
       </c>
     </row>
     <row r="18">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>376889.3868459186</v>
+        <v>376889.3868459184</v>
       </c>
     </row>
     <row r="19">
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>6644.152226892242</v>
+        <v>6644.152226891718</v>
       </c>
     </row>
     <row r="20">
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>0.8482135970198968</v>
+        <v>0.8482135970198971</v>
       </c>
     </row>
     <row r="21">
@@ -1115,7 +1115,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>257573.6731709279</v>
+        <v>257573.6731709278</v>
       </c>
     </row>
     <row r="22">
@@ -1141,7 +1141,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>709.5406765745048</v>
+        <v>709.5406765745053</v>
       </c>
     </row>
     <row r="23">
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>84.23423749132563</v>
+        <v>84.23423749132566</v>
       </c>
     </row>
     <row r="24">
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>8.423423749132562</v>
+        <v>8.423423749132565</v>
       </c>
     </row>
     <row r="25">
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>0.06855887770801748</v>
+        <v>0.06855887770801745</v>
       </c>
     </row>
     <row r="26">
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>1253668.147000186</v>
+        <v>1253668.147000185</v>
       </c>
     </row>
     <row r="27">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>383533.5390728108</v>
+        <v>383533.5390728101</v>
       </c>
     </row>
     <row r="28">
@@ -1277,7 +1277,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>421886.892980092</v>
+        <v>421886.8929800912</v>
       </c>
     </row>
     <row r="29">
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>376889.3868459186</v>
+        <v>376889.3868459184</v>
       </c>
     </row>
     <row r="30">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="K30" s="2" t="n">
-        <v>6644.152226892242</v>
+        <v>6644.152226891718</v>
       </c>
     </row>
     <row r="31">
@@ -1351,7 +1351,7 @@
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>4.813384999504324</v>
+        <v>4.813384999504322</v>
       </c>
     </row>
     <row r="34">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>8.939143570508028</v>
+        <v>8.939143570508026</v>
       </c>
     </row>
     <row r="38">
@@ -1401,7 +1401,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>709.5406765745053</v>
+        <v>709.5406765745048</v>
       </c>
     </row>
     <row r="39">
@@ -1411,7 +1411,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>84.23423749132566</v>
+        <v>84.23423749132563</v>
       </c>
     </row>
     <row r="40">
@@ -1713,7 +1713,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2863,7 +2863,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -2929,11 +2929,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Cl_alpha</t>
+          <t>tfo</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>5</v>
+        <v>0.001</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -2963,11 +2963,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>tfo</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0.001</v>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -2989,11 +2989,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>0</v>
+          <t>n_engines</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8</v>
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
@@ -3025,11 +3025,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>n_engines</t>
+          <t>CLmax_clean</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -3051,11 +3051,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CLmax_clean</t>
+          <t>CLmax_takeoff</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CLmax_takeoff</t>
+          <t>CLmax_landing</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>CLmax_landing</t>
+          <t>r_float</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3129,11 +3129,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>r_float</t>
+          <t>upsweep</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>1.5</v>
+        <v>11</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -3155,11 +3155,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>upsweep</t>
+          <t>xcg_OEW</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>11</v>
+        <v>0.45</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -3173,11 +3173,11 @@
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>xcg_OEW</t>
+          <t>xcg_payload</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.45</v>
+        <v>0.55</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -3201,11 +3201,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>xcg_payload</t>
+          <t>V_h</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.55</v>
+        <v>0.9</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -3227,11 +3227,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>V_h</t>
+          <t>V_v</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.9</v>
+        <v>0.0838</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -3251,14 +3251,6 @@
       <c r="B26" s="4" t="n">
         <v>1.006e-06</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>V_v</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.0838</v>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
           <t>OEW [N]</t>
@@ -3277,6 +3269,16 @@
       <c r="B27" s="2" t="n">
         <v>1000</v>
       </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
       <c r="J27" t="inlineStr">
         <is>
           <t>total_fuel [N]</t>
@@ -3287,15 +3289,13 @@
       </c>
     </row>
     <row r="28">
-      <c r="D28" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="E28" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.4</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3309,11 +3309,11 @@
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>0.4</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3327,11 +3327,11 @@
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E30" s="3" t="n">
-        <v>0</v>
+          <t>dihedral [deg]</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3345,11 +3345,11 @@
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>1</v>
+        <v>2.454031674527076</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3363,11 +3363,11 @@
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>2.454031674527076</v>
+        <v>12.33943621469093</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3381,90 +3381,80 @@
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>12.33943621469093</v>
+        <v>4.935774485876372</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>4.935774485876372</v>
+        <v>18.50915432203639</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>18.50915432203639</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>21.05644</v>
+        <v>20.26319052905558</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>20.26319052905558</v>
+        <v>9.166438330913261</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>9.166438330913261</v>
+        <v>746.0822618724875</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>746.0822618724875</v>
+        <v>86.37605350283651</v>
       </c>
     </row>
     <row r="40">
       <c r="D40" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>aspect_ratio</t>
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>86.37605350283651</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E41" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3757,7 +3747,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update design parameters and calculations across multiple design files
- Adjusted aerodynamic coefficients (Cd0) in design2.json, design3.json, and design4.json for improved accuracy.
- Modified various design metrics including MTOW, total fuel, OEW, and fuel economy in design2.json, design3.json, and design4.json to reflect updated calculations.
- Updated ferry and altitude performance metrics in design3.json and design4.json to enhance mission profiles.
- Corrected wing design parameters in all design files to ensure consistency with new aerodynamic data.
- Removed redundant fuel mission and reserve fuel outputs in Iteration.py to streamline data handling.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,13 +438,13 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2574437.066356279</v>
+        <v>2524434.530168885</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>414301.2515731714</v>
+        <v>382007.271465351</v>
       </c>
     </row>
     <row r="4">
@@ -588,11 +588,11 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>fuel_mission [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>388403.4960463954</v>
+        <v>1252833.574173365</v>
       </c>
     </row>
     <row r="5">
@@ -622,11 +622,11 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>fuel_reserve [N]</t>
+          <t>EW [N]</t>
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>25897.75552677596</v>
+        <v>1252408.574173365</v>
       </c>
     </row>
     <row r="6">
@@ -656,11 +656,11 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>ZFW [N]</t>
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>1270492.127716752</v>
+        <v>2142427.258703534</v>
       </c>
     </row>
     <row r="7">
@@ -690,11 +690,11 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>EW [N]</t>
+          <t>h_b</t>
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1270067.127716752</v>
+        <v>0.04750885085416576</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -720,15 +720,15 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>16.79397971338663</v>
+        <v>16.70488891980677</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ZFW [N]</t>
+          <t>k</t>
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>2160135.814783108</v>
+        <v>1.751267021153337</v>
       </c>
     </row>
     <row r="9">
@@ -758,11 +758,11 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>h_b</t>
+          <t>WP [N/W]</t>
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.04704521330223214</v>
+        <v>0.09507857087882329</v>
       </c>
     </row>
     <row r="10">
@@ -792,11 +792,8 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>1.756933311801416</v>
+          <t>TW</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -814,7 +811,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02367017989497004</v>
+        <v>0.02392332955096443</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -822,15 +819,15 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>297.9879596426425</v>
+        <v>141.2696827920026</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>WP [N/W]</t>
+          <t>WS [N/m²]</t>
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.09582402833754056</v>
+        <v>3561.173893518813</v>
       </c>
     </row>
     <row r="12">
@@ -856,12 +853,15 @@
         </is>
       </c>
       <c r="H12" s="2" t="n">
-        <v>61104505.81607803</v>
+        <v>28968332.02305043</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>TW</t>
-        </is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>26551035.70484091</v>
       </c>
     </row>
     <row r="13">
@@ -888,11 +888,8 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>3561.173893518813</v>
+          <t>T [N]</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -922,11 +919,11 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>P [W]</t>
+          <t>LD</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>26866299.72690997</v>
+        <v>29.25472105728739</v>
       </c>
     </row>
     <row r="15">
@@ -948,8 +945,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>T [N]</t>
-        </is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>420207.9986118862</v>
       </c>
     </row>
     <row r="16">
@@ -981,11 +981,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>mission_fuel</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>29.50590239616616</v>
+        <v>375422.8595370818</v>
       </c>
     </row>
     <row r="17">
@@ -1007,11 +1007,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>262429.8742463078</v>
+        <v>6584.411928269255</v>
       </c>
     </row>
     <row r="18">
@@ -1033,11 +1033,11 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>722.9181004124157</v>
+        <v>0.8486761027469408</v>
       </c>
     </row>
     <row r="19">
@@ -1059,11 +1059,11 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>fuel_mission [N]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>85.02459058486643</v>
+        <v>375422.8595632432</v>
       </c>
     </row>
     <row r="20">
@@ -1077,19 +1077,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>r_float</t>
+          <t>CL_hydro</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>4.4</v>
+        <v>0.5</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>fuel_reserve [N]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>8.502459058486643</v>
+        <v>6584.411929335445</v>
       </c>
     </row>
     <row r="21">
@@ -1103,19 +1103,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>upsweep</t>
+          <t>r_float</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>11</v>
+        <v>4.4</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.1448394220378516</v>
+        <v>257332.7757562574</v>
       </c>
     </row>
     <row r="22">
@@ -1129,11 +1129,37 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>upsweep</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>1.453895622250116</v>
+        <v>11</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>708.8770741477267</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xcg_OEW</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>84.19483797405437</v>
       </c>
     </row>
     <row r="24">
@@ -1147,15 +1173,21 @@
           <t>General States</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>8.419483797405437</v>
       </c>
     </row>
     <row r="25">
@@ -1169,11 +1201,19 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>taper_ratio</t>
+          <t>V_h</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.4</v>
+        <v>0.9</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>0.06829210589132233</v>
       </c>
     </row>
     <row r="26">
@@ -1187,11 +1227,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>0</v>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.0838</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>1252833.574173365</v>
       </c>
     </row>
     <row r="27">
@@ -1205,11 +1253,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
+          <t>k</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>5</v>
+        <v>1.751274668032127</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>382007.271465351</v>
       </c>
     </row>
     <row r="28">
@@ -1221,110 +1277,186 @@
       <c r="B28" s="3" t="n">
         <v>1.484e-05</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>2.454031674527076</v>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>420207.9986118862</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>rho_air</t>
+          <t>rho_air [kg/m³]</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>1.225</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>12.06448415554899</v>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>375422.8595370818</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>taper_ratio</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>4.825793662219597</v>
+        <v>0.4</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>6584.411928269255</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>18.09672623332349</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0.841402256178446</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>21.05644</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>20.28086601857185</v>
+        <v>2.454031674527076</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>8.962188229836395</v>
+        <v>12.02783399629348</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>713.203711903514</v>
+        <v>4.811133598517394</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>84.45138908884293</v>
+        <v>18.04175099444022</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>21.05644</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>20.28322210023828</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>8.934962397246588</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>708.8770741477269</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>84.19483797405438</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E42" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1339,7 +1471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1433,7 +1565,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2646927.027891309</v>
+        <v>2597048.611488787</v>
       </c>
     </row>
     <row r="3">
@@ -1469,7 +1601,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>461118.6643351071</v>
+        <v>428904.846598424</v>
       </c>
     </row>
     <row r="4">
@@ -1501,11 +1633,11 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>fuel_mission [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>435795.1987296298</v>
+        <v>1278477.466278875</v>
       </c>
     </row>
     <row r="5">
@@ -1535,11 +1667,11 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>fuel_reserve [N]</t>
+          <t>EW [N]</t>
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>25323.46560547728</v>
+        <v>1278052.466278875</v>
       </c>
     </row>
     <row r="6">
@@ -1569,11 +1701,11 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>ZFW [N]</t>
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>1296092.186528311</v>
+        <v>2168143.764890363</v>
       </c>
     </row>
     <row r="7">
@@ -1591,7 +1723,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1603,11 +1735,11 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>EW [N]</t>
+          <t>h_b</t>
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1295667.186528311</v>
+        <v>0.09366193778912307</v>
       </c>
     </row>
     <row r="8">
@@ -1617,7 +1749,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1637,11 +1769,11 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ZFW [N]</t>
+          <t>k</t>
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>2185808.363556203</v>
+        <v>1.423286944126012</v>
       </c>
     </row>
     <row r="9">
@@ -1671,11 +1803,11 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>h_b</t>
+          <t>WP [N/W]</t>
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.09277526293692347</v>
+        <v>0.09323812173756052</v>
       </c>
     </row>
     <row r="10">
@@ -1701,15 +1833,12 @@
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>210.4204947871738</v>
+        <v>70.13639222689177</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>1.427064793454931</v>
+          <t>TW</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -1727,7 +1856,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02315328094641167</v>
+        <v>0.02338881420110402</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1735,15 +1864,15 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>93133344.13863601</v>
+        <v>31042778.22612376</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>WP [N/W]</t>
+          <t>WS [N/m²]</t>
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.09392948775688056</v>
+        <v>3559.80642288087</v>
       </c>
     </row>
     <row r="12">
@@ -1770,8 +1899,11 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>TW</t>
-        </is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>27853935.31198279</v>
       </c>
     </row>
     <row r="13">
@@ -1801,11 +1933,8 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>3559.80642288087</v>
+          <t>T [N]</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1831,15 +1960,15 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.98040845375636</v>
+        <v>16.89469288882871</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>P [W]</t>
+          <t>LD</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>28179936.79197314</v>
+        <v>24.04599581368848</v>
       </c>
     </row>
     <row r="15">
@@ -1861,8 +1990,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>T [N]</t>
-        </is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>471795.3312582664</v>
       </c>
     </row>
     <row r="16">
@@ -1894,11 +2026,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>mission_fuel</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>24.23214308284019</v>
+        <v>420498.0342925607</v>
       </c>
     </row>
     <row r="17">
@@ -1920,11 +2052,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>269819.2688981967</v>
+        <v>8406.812305863306</v>
       </c>
     </row>
     <row r="18">
@@ -1946,11 +2078,11 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>743.5592595147021</v>
+        <v>0.8348491265427067</v>
       </c>
     </row>
     <row r="19">
@@ -1972,11 +2104,11 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>86.22988226332575</v>
+        <v>264734.8227817316</v>
       </c>
     </row>
     <row r="20">
@@ -1990,19 +2122,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>r_float</t>
+          <t>CL_hydro</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>3.1</v>
+        <v>0.5</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>8.622988226332575</v>
+        <v>729.5477065258664</v>
       </c>
     </row>
     <row r="21">
@@ -2016,19 +2148,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>upsweep</t>
+          <t>r_float</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>11</v>
+        <v>3.1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.1625122465512783</v>
+        <v>85.41356487852889</v>
       </c>
     </row>
     <row r="22">
@@ -2042,11 +2174,37 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>upsweep</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>1.228075442628302</v>
+        <v>11</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>8.541356487852889</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xcg_OEW</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0.07649160288323889</v>
       </c>
     </row>
     <row r="24">
@@ -2060,15 +2218,21 @@
           <t>General States</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>1278477.466278875</v>
       </c>
     </row>
     <row r="25">
@@ -2082,11 +2246,19 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>taper_ratio</t>
+          <t>V_h</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.4</v>
+        <v>0.9</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>428904.846598424</v>
       </c>
     </row>
     <row r="26">
@@ -2100,11 +2272,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>0</v>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.0838</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>471795.3312582664</v>
       </c>
     </row>
     <row r="27">
@@ -2118,11 +2298,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
+          <t>k</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1</v>
+        <v>1.423294502805824</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>420498.0342925607</v>
       </c>
     </row>
     <row r="28">
@@ -2134,110 +2322,178 @@
       <c r="B28" s="3" t="n">
         <v>1.48e-05</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>2.454031674527076</v>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>8406.812305863306</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>rho_air</t>
+          <t>rho_air [kg/m³]</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>1.225</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>12.21342606619523</v>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0.8198004069149908</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>taper_ratio</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>4.885370426478094</v>
+        <v>0.4</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>1720912.57500321</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>18.32013909929285</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>21.05644</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>20.27129118145888</v>
+        <v>2.454031674527076</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>9.072830792030743</v>
+        <v>12.20193783979032</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>730.922103744644</v>
+        <v>4.880775135916128</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>85.49398246336662</v>
+        <v>18.30290675968548</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>21.05644</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>20.2720297102992</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>9.064296680987093</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>729.5477065259233</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>85.41356487853223</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E42" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2252,7 +2508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2346,7 +2602,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2669083.614040726</v>
+        <v>2618435.421524607</v>
       </c>
     </row>
     <row r="3">
@@ -2382,7 +2638,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>475428.4255377167</v>
+        <v>442717.4503287238</v>
       </c>
     </row>
     <row r="4">
@@ -2414,11 +2670,11 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>fuel_mission [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>450277.6819258266</v>
+        <v>1286030.285774358</v>
       </c>
     </row>
     <row r="5">
@@ -2448,11 +2704,11 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>fuel_reserve [N]</t>
+          <t>EW [N]</t>
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>25150.74361189007</v>
+        <v>1285605.285774358</v>
       </c>
     </row>
     <row r="6">
@@ -2482,11 +2738,11 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>ZFW [N]</t>
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>1303916.854888969</v>
+        <v>2175717.971195883</v>
       </c>
     </row>
     <row r="7">
@@ -2504,7 +2760,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -2516,11 +2772,11 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>EW [N]</t>
+          <t>h_b</t>
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1303491.854888969</v>
+        <v>0.1162669240453023</v>
       </c>
     </row>
     <row r="8">
@@ -2546,15 +2802,15 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>4850602117.146465</v>
+        <v>4837280592.753655</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ZFW [N]</t>
+          <t>k</t>
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>2193655.18850301</v>
+        <v>1.34318527219474</v>
       </c>
     </row>
     <row r="9">
@@ -2580,15 +2836,15 @@
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.00126964877111443</v>
+        <v>0.001270043469758956</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>h_b</t>
+          <t>WP [N/W]</t>
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.1154756456428767</v>
+        <v>0.09301989426111927</v>
       </c>
     </row>
     <row r="10">
@@ -2614,15 +2870,12 @@
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>358.3025367334438</v>
+        <v>69.21817427258117</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>1.345549746662417</v>
+          <t>TW</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -2640,7 +2893,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02320987776139502</v>
+        <v>0.02337930126140052</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2648,15 +2901,15 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>76160445.50231826</v>
+        <v>14596596.60224672</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>WP [N/W]</t>
+          <t>WS [N/m²]</t>
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.09375416161734564</v>
+        <v>3539.60038145072</v>
       </c>
     </row>
     <row r="12">
@@ -2666,7 +2919,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -2683,8 +2936,11 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>TW</t>
-        </is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>28149198.00031495</v>
       </c>
     </row>
     <row r="13">
@@ -2710,15 +2966,12 @@
         </is>
       </c>
       <c r="H13" s="2" t="n">
-        <v>64.995</v>
+        <v>64.8165</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>3559.122838225619</v>
+          <t>T [N]</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -2732,11 +2985,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Cl_alpha</t>
+          <t>tfo</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>5</v>
+        <v>0.001</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -2744,15 +2997,15 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.9596926268958</v>
+        <v>16.89812972912173</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>P [W]</t>
+          <t>LD</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>28468961.46258017</v>
+        <v>22.69731897979241</v>
       </c>
     </row>
     <row r="15">
@@ -2762,20 +3015,23 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>61.9</v>
+        <v>61.73</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>tfo</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0.001</v>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>T [N]</t>
-        </is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>486989.1953615962</v>
       </c>
     </row>
     <row r="16">
@@ -2785,15 +3041,15 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>61.9</v>
+        <v>61.73</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v>0</v>
+          <t>n_engines</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8</v>
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
@@ -2807,11 +3063,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>mission_fuel</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>22.8201101175921</v>
+        <v>433778.962629226</v>
       </c>
     </row>
     <row r="17">
@@ -2825,19 +3081,19 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>n_engines</t>
+          <t>CLmax_clean</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>272077.840371124</v>
+        <v>8938.48769949784</v>
       </c>
     </row>
     <row r="18">
@@ -2851,19 +3107,19 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CLmax_clean</t>
+          <t>CLmax_takeoff</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>749.9273655990662</v>
+        <v>0.8309229065993357</v>
       </c>
     </row>
     <row r="19">
@@ -2877,7 +3133,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CLmax_takeoff</t>
+          <t>CLmax_landing</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
@@ -2885,11 +3141,11 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>86.59834672781382</v>
+        <v>266914.9257415501</v>
       </c>
     </row>
     <row r="20">
@@ -2903,19 +3159,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>CLmax_landing</t>
+          <t>CL_hydro</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>8.659834672781381</v>
+        <v>739.754531400354</v>
       </c>
     </row>
     <row r="21">
@@ -2937,11 +3193,11 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.1679129046739834</v>
+        <v>86.00898391449314</v>
       </c>
     </row>
     <row r="22">
@@ -2961,15 +3217,31 @@
       <c r="E22" s="2" t="n">
         <v>11</v>
       </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>8.600898391449315</v>
+      </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>xcg_OEW</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>1.175600054827848</v>
+        <v>0.45</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0.07890749882900248</v>
       </c>
     </row>
     <row r="24">
@@ -2983,6 +3255,22 @@
           <t>General States</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>1286030.285774358</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2993,15 +3281,21 @@
       <c r="B25" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D25" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>V_h</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>442717.4503287238</v>
       </c>
     </row>
     <row r="26">
@@ -3015,11 +3309,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>taper_ratio</t>
+          <t>V_v</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.4</v>
+        <v>0.0838</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>486989.1953615962</v>
       </c>
     </row>
     <row r="27">
@@ -3033,11 +3335,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="4" t="n">
-        <v>0</v>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1.175466862781727</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>433778.962629226</v>
       </c>
     </row>
     <row r="28">
@@ -3049,120 +3359,178 @@
       <c r="B28" s="3" t="n">
         <v>1.484e-05</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>1</v>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>8938.48769949784</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>rho_air</t>
+          <t>rho_air [kg/m³]</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>1.225</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>2.454031674527076</v>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0.8144958966029898</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>taper_ratio</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>12.25893671424686</v>
+        <v>0.4</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>1733790.843393344</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>4.903574685698743</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>18.38840507137029</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>21.05644</v>
+        <v>2.454031674527076</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>20.26836549694127</v>
+        <v>12.28699770230961</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>9.106638702011949</v>
+        <v>4.914799080923845</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>736.3794938831564</v>
+        <v>18.43049655346442</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>85.81255699972799</v>
+        <v>21.05644</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>20.2665615762801</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>9.127484007429995</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>739.7545314291519</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>86.00898391616727</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E42" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3177,7 +3545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3189,7 +3557,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -3271,7 +3639,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2721150.218192705</v>
+        <v>2671601.222731665</v>
       </c>
     </row>
     <row r="3">
@@ -3307,7 +3675,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>509055.477422929</v>
+        <v>477054.4151611172</v>
       </c>
     </row>
     <row r="4">
@@ -3339,11 +3707,11 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>fuel_mission [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>484305.6699416121</v>
+        <v>1304805.956347816</v>
       </c>
     </row>
     <row r="5">
@@ -3373,11 +3741,11 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>fuel_reserve [N]</t>
+          <t>EW [N]</t>
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>24749.80748131691</v>
+        <v>1304380.956347816</v>
       </c>
     </row>
     <row r="6">
@@ -3407,11 +3775,11 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>ZFW [N]</t>
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>1322304.340551583</v>
+        <v>2194546.807570548</v>
       </c>
     </row>
     <row r="7">
@@ -3441,11 +3809,11 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>EW [N]</t>
+          <t>h_b</t>
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1321879.340551583</v>
+        <v>0.08431602766458843</v>
       </c>
     </row>
     <row r="8">
@@ -3455,7 +3823,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -3475,11 +3843,11 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ZFW [N]</t>
+          <t>k</t>
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>2212094.740769776</v>
+        <v>1.466260010108539</v>
       </c>
     </row>
     <row r="9">
@@ -3509,11 +3877,11 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>h_b</t>
+          <t>WP [N/W]</t>
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.08354485235901765</v>
+        <v>0.08235589165771251</v>
       </c>
     </row>
     <row r="10">
@@ -3539,15 +3907,12 @@
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>101.5868044236281</v>
+        <v>48.16011913363723</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>1.470145169926236</v>
+          <t>TW</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -3565,7 +3930,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02298110575827635</v>
+        <v>0.02320536089523409</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3573,15 +3938,15 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>20831081.52820842</v>
+        <v>9875567.735130826</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>WP [N/W]</t>
+          <t>WS [N/m²]</t>
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.08285045328569222</v>
+        <v>3561.173893518813</v>
       </c>
     </row>
     <row r="12">
@@ -3608,8 +3973,11 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>TW</t>
-        </is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>32439709.76400051</v>
       </c>
     </row>
     <row r="13">
@@ -3639,11 +4007,8 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>3561.173893518813</v>
+          <t>T [N]</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -3669,15 +4034,15 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>13.2021471196634</v>
+        <v>13.13819989259041</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>P [W]</t>
+          <t>LD</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>32844119.86026673</v>
+        <v>19.26401710731762</v>
       </c>
     </row>
     <row r="15">
@@ -3699,8 +4064,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>T [N]</t>
-        </is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>524759.8566772289</v>
       </c>
     </row>
     <row r="16">
@@ -3732,11 +4100,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>mission_fuel</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>19.40907282062873</v>
+        <v>466803.7826471954</v>
       </c>
     </row>
     <row r="17">
@@ -3758,11 +4126,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>277385.3433427833</v>
+        <v>10250.63251392171</v>
       </c>
     </row>
     <row r="18">
@@ -3784,11 +4152,11 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>764.1160749988813</v>
+        <v>0.8214350214013836</v>
       </c>
     </row>
     <row r="19">
@@ -3810,11 +4178,11 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>47.8784735032002</v>
+        <v>272334.4773426774</v>
       </c>
     </row>
     <row r="20">
@@ -3836,11 +4204,11 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>15.9594911677334</v>
+        <v>750.2024058959332</v>
       </c>
     </row>
     <row r="21">
@@ -3854,19 +4222,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>r_float</t>
+          <t>CL_hydro</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.1806022706747688</v>
+        <v>47.44056510717173</v>
       </c>
     </row>
     <row r="22">
@@ -3880,21 +4248,37 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>upsweep</t>
+          <t>r_float</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>11</v>
+        <v>1.5</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>15.81352170239058</v>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>upsweep</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>1.260616536384089</v>
+        <v>11</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0.08491495002281096</v>
       </c>
     </row>
     <row r="24">
@@ -3908,6 +4292,22 @@
           <t>General States</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xcg_OEW</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>1304805.956347816</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3918,15 +4318,21 @@
       <c r="B25" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D25" s="1" t="inlineStr">
-        <is>
-          <t>Design 4</t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>477054.4151611172</v>
       </c>
     </row>
     <row r="26">
@@ -3940,11 +4346,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>taper_ratio</t>
+          <t>V_h</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.4</v>
+        <v>0.9</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>max_fuel</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>524759.8566772289</v>
       </c>
     </row>
     <row r="27">
@@ -3958,11 +4372,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E27" s="4" t="n">
-        <v>0</v>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.0838</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>mission_fuel</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>466803.7826471954</v>
       </c>
     </row>
     <row r="28">
@@ -3976,118 +4398,186 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
+          <t>k</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>5</v>
+        <v>1.466271510318843</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>10250.63251392171</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>rho_air</t>
+          <t>rho_air [kg/m³]</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>1.225</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>4.085616779974877</v>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0.7948787038329889</v>
       </c>
     </row>
     <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>22.56491680584854</v>
+      <c r="D30" s="1" t="inlineStr">
+        <is>
+          <t>Design 4</t>
+        </is>
+      </c>
+      <c r="E30" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>1744319.451377081</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>taper_ratio</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>9.025966722339415</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>10.15421256263184</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>21.05644</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>20.33113910266916</v>
+        <v>4.085616779974877</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>16.76250962720177</v>
+        <v>22.59074529030858</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>748.4879415686523</v>
+        <v>9.036298116123431</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>47.38632529228192</v>
+        <v>10.16583538063886</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>21.05644</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>20.33030890138294</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>16.78169650137209</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>750.2024059742508</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>47.44056510964801</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="D43" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E43" s="2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update design parameters across multiple JSON files to improve performance metrics
- Increased propeller efficiency and adjusted drag coefficients in design2.json, design3.json, and design4.json.
- Modified various weight and fuel parameters to reflect updated calculations in design2.json, design3.json, and design4.json.
- Fine-tuned aerodynamic characteristics such as wing design and center of gravity ranges in design2.json, design3.json, and design4.json.
- Adjusted take-off power and thrust values for better alignment with performance expectations in design3.json and design4.json.
- Ensured consistency in fuel economy and reserve fuel calculations across all design files.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2524434.530168885</v>
+        <v>2630224.648699611</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>382007.271465351</v>
+        <v>450331.4854738481</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1252833.574173365</v>
+        <v>1290193.688577064</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1252408.574173365</v>
+        <v>1289768.688577064</v>
       </c>
     </row>
     <row r="6">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2142427.258703534</v>
+        <v>2179893.163225763</v>
       </c>
     </row>
     <row r="7">
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.04750885085416576</v>
+        <v>0.06008755531464779</v>
       </c>
     </row>
     <row r="8">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>16.70488891980677</v>
+        <v>13.08369566255592</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.751267021153337</v>
+        <v>1.623799771135969</v>
       </c>
     </row>
     <row r="9">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.09507857087882329</v>
+        <v>0.08193335381292005</v>
       </c>
     </row>
     <row r="10">
@@ -784,7 +784,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>Cd_water</t>
         </is>
       </c>
       <c r="H10" s="2" t="n">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02392332955096443</v>
+        <v>0.02339910199117188</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>141.2696827920026</v>
+        <v>154.2858147484878</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -853,7 +853,7 @@
         </is>
       </c>
       <c r="H12" s="2" t="n">
-        <v>28968332.02305043</v>
+        <v>31637380.50337056</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>26551035.70484091</v>
+        <v>32102001.52071466</v>
       </c>
     </row>
     <row r="13">
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>29.25472105728739</v>
+        <v>21.24530202247096</v>
       </c>
     </row>
     <row r="15">
@@ -945,11 +945,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>max_fuel</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>420207.9986118862</v>
+        <v>495364.634021233</v>
       </c>
     </row>
     <row r="16">
@@ -981,11 +981,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>mission_fuel</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>375422.8595370818</v>
+        <v>441100.8727192185</v>
       </c>
     </row>
     <row r="17">
@@ -1005,13 +1005,21 @@
       <c r="E17" s="2" t="n">
         <v>1.5</v>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>S_h [m²]</t>
+        </is>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>224.7087640222175</v>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>6584.411928269255</v>
+        <v>9230.612754629576</v>
       </c>
     </row>
     <row r="18">
@@ -1031,13 +1039,21 @@
       <c r="E18" s="2" t="n">
         <v>1.7</v>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>S_v [m²]</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>125.5372961670788</v>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8486761027469408</v>
+        <v>0.8287859230212549</v>
       </c>
     </row>
     <row r="19">
@@ -1057,13 +1073,21 @@
       <c r="E19" s="2" t="n">
         <v>1.7</v>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>l_h [m]</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>32.82058871597789</v>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>fuel_mission [N]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>375422.8595632432</v>
+        <v>268116.6818246291</v>
       </c>
     </row>
     <row r="20">
@@ -1083,13 +1107,21 @@
       <c r="E20" s="2" t="n">
         <v>0.5</v>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>l_v [m]</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>32.82058871597789</v>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>fuel_reserve [N]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>6584.411929335445</v>
+        <v>738.5836039870164</v>
       </c>
     </row>
     <row r="21">
@@ -1107,15 +1139,15 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>4.4</v>
+        <v>3</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>257332.7757562574</v>
+        <v>66.56952473859265</v>
       </c>
     </row>
     <row r="22">
@@ -1135,13 +1167,23 @@
       <c r="E22" s="2" t="n">
         <v>11</v>
       </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="H22" s="1" t="inlineStr">
+        <is>
+          <t>CG Range</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>708.8770741477267</v>
+        <v>11.09492078976544</v>
       </c>
     </row>
     <row r="23">
@@ -1153,13 +1195,21 @@
       <c r="E23" s="2" t="n">
         <v>0.4</v>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>most_aft_cg [m]</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>34.7497652630114</v>
+      </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>84.19483797405437</v>
+        <v>0.08023940669366764</v>
       </c>
     </row>
     <row r="24">
@@ -1181,13 +1231,23 @@
       <c r="E24" s="2" t="n">
         <v>0.55</v>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>most_aft_mission</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ALTITUDE_OEW_PAYLOAD</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>8.419483797405437</v>
+        <v>1290193.688577064</v>
       </c>
     </row>
     <row r="25">
@@ -1207,13 +1267,21 @@
       <c r="E25" s="2" t="n">
         <v>0.9</v>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>most_forward_cg [m]</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>29.08041911622887</v>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>0.06829210589132233</v>
+        <v>450331.4854738481</v>
       </c>
     </row>
     <row r="26">
@@ -1233,13 +1301,23 @@
       <c r="E26" s="2" t="n">
         <v>0.0838</v>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>most_forward_mission</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>DESIGN_OEW_FUEL</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>1252833.574173365</v>
+        <v>495364.634021233</v>
       </c>
     </row>
     <row r="27">
@@ -1257,15 +1335,15 @@
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1.751274668032127</v>
+        <v>1.605242456062792</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>382007.271465351</v>
+        <v>441100.8727192185</v>
       </c>
     </row>
     <row r="28">
@@ -1279,11 +1357,11 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>max_fuel</t>
+          <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>420207.9986118862</v>
+        <v>9230.612754629576</v>
       </c>
     </row>
     <row r="29">
@@ -1307,11 +1385,11 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>mission_fuel</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>375422.8595370818</v>
+        <v>0.8056775067428494</v>
       </c>
     </row>
     <row r="30">
@@ -1323,14 +1401,6 @@
       <c r="E30" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K30" s="2" t="n">
-        <v>6584.411928269255</v>
-      </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
@@ -1341,14 +1411,6 @@
       <c r="E31" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Mff</t>
-        </is>
-      </c>
-      <c r="K31" s="2" t="n">
-        <v>0.841402256178446</v>
-      </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
@@ -1367,7 +1429,7 @@
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>2.454031674527076</v>
+        <v>4.085616779974877</v>
       </c>
     </row>
     <row r="34">
@@ -1377,7 +1439,7 @@
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>12.02783399629348</v>
+        <v>15.84988684272195</v>
       </c>
     </row>
     <row r="35">
@@ -1387,7 +1449,7 @@
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>4.811133598517394</v>
+        <v>6.339954737088782</v>
       </c>
     </row>
     <row r="36">
@@ -1397,7 +1459,7 @@
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>18.04175099444022</v>
+        <v>14.26489815844976</v>
       </c>
     </row>
     <row r="37">
@@ -1417,7 +1479,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>20.28322210023828</v>
+        <v>20.03751870296788</v>
       </c>
     </row>
     <row r="39">
@@ -1427,7 +1489,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>8.934962397246588</v>
+        <v>11.77420165459345</v>
       </c>
     </row>
     <row r="40">
@@ -1437,7 +1499,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>708.8770741477269</v>
+        <v>738.5836040056462</v>
       </c>
     </row>
     <row r="41">
@@ -1447,7 +1509,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>84.19483797405438</v>
+        <v>66.56952473943221</v>
       </c>
     </row>
     <row r="42">
@@ -1457,7 +1519,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1466,6 +1528,1121 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="27" customWidth="1" min="8" max="8"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Requirements</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Inputs</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>General Outputs</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Design Mission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>design_range [m]</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>3704000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>cruise_altitude [m]</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>d_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>6.204804790550249</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>2585106.105313952</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>design_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>aircraft_type</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>PROP</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>r_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>3.102402395275125</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>421191.8166952552</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>design_crew</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>wing_type</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>l_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>52.74084071967712</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>1274259.932513383</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ferry_range [m]</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>12038000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>n_wings</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>l_tailcone [m]</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>27.92162155747612</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>EW [N]</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>1273834.932513383</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>reserve_range [m]</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>185200</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>n_fuselages</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>l_nose [m]</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>9.307207185825375</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ZFW [N]</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>2163914.288618697</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ferry_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>l_cargo_straight [m]</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>8.74654837462985</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>h_b</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0.09387803518272897</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ferry_crew</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jet_consumption [kg/(N·s)]</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>2.7e-05</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Re</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>3407446264.985502</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>1.422374919554507</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>altitude_range_WIG [m]</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>943600</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>prop_consumption [kg/J]</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>2.1e-08</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Cd_water</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0.001321877371153106</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>WP [N/W]</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0.09647518482443268</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>altitude_range_WOG [m]</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>538000</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>prop_efficiency</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>hull_surface [m²]</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>224.1641870825653</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>altitude_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Cd0</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.02344655710840882</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>take_off_power [W]</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>47857314.10082371</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WS [N/m²]</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>3559.80642288087</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>altitude_crew</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>oswald_factor</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>take_off_thrust [N]</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>26795554.83639006</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cruise_speed [m/s]</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>115.749</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>V_lof [m/s]</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>64.995</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>T [N]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>stall_speed_clean [m/s]</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>77.16</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tfo</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>LD_g</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>16.87387639850711</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>24.00097858489925</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>stall_speed_takeoff [m/s]</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>max_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>463310.9983647808</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>stall_speed_landing [m/s]</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>n_engines</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>Empennage Design</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>mission_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>413082.8798527136</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>stall_speed_high</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CLmax_clean</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>S_h [m²]</t>
+        </is>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>244.7440899719453</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>8108.936842541618</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>high_altitude [m]</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>3048</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CLmax_takeoff</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>S_v [m²]</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>227.8839415516557</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0.8370698147246444</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cargo_width [m]</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CLmax_landing</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>l_h [m]</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>22.91452403750576</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>MTOM [kg]</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>263517.4419280277</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>cargo_height [m]</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>CL_hydro</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>l_v [m]</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>22.91452403750576</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>726.1928875453634</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>cargo_length [m]</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>r_float</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>3.102402395275125</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>85.21695180803896</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>cargo_density [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>upsweep</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="H22" s="1" t="inlineStr">
+        <is>
+          <t>CG Range</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>8.521695180803896</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xcg_OEW</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>most_aft_cg [m]</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>24.55223261020365</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0.07514273320377675</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>General States</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>most_aft_mission</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ALTITUDE_OEW_PAYLOAD_FUEL</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>1274259.932513383</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>design_id</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>V_h</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>most_forward_cg [m]</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>21.09633628787085</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>421191.8166952552</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>kinematic_viscosity [m²/s]</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1.006e-06</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.0838</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>most_forward_mission</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>DESIGN_OEW</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>max_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>463310.9983647808</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>rho_water [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1.226101000048545</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>mission_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>413082.8798527136</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>viscosity_air [m²/s]</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1.48e-05</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>8108.936842541618</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rho_air [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1.225</v>
+      </c>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0.823842794974096</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>1720912.57500321</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>dihedral [deg]</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>sweep_x_c [deg]</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>2.454031674527076</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>chord_root [m]</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>12.20193783978984</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>chord_tip [m]</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>4.880775135915937</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>y_MAC [m]</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>18.30290675968476</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>21.05644</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>20.27202971029923</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>9.06429668098674</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>729.5477065258664</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>85.41356487852889</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1495,7 +2672,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 3</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1505,7 +2682,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -1515,7 +2692,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 3</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -1525,7 +2702,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 3</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -1549,7 +2726,7 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -1557,7 +2734,7 @@
         </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>6.204804790550249</v>
+        <v>8.832726010325398</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -1565,7 +2742,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2597048.611488787</v>
+        <v>2605660.308783418</v>
       </c>
     </row>
     <row r="3">
@@ -1593,7 +2770,7 @@
         </is>
       </c>
       <c r="H3" s="2" t="n">
-        <v>3.102402395275125</v>
+        <v>4.416363005162699</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -1601,7 +2778,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>428904.846598424</v>
+        <v>434466.6841037282</v>
       </c>
     </row>
     <row r="4">
@@ -1629,7 +2806,7 @@
         </is>
       </c>
       <c r="H4" s="2" t="n">
-        <v>52.74084071967712</v>
+        <v>75.07817108776588</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -1637,7 +2814,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1278477.466278875</v>
+        <v>1281518.714370907</v>
       </c>
     </row>
     <row r="5">
@@ -1663,7 +2840,7 @@
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>27.92162155747612</v>
+        <v>39.74726704646429</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -1671,7 +2848,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1278052.466278875</v>
+        <v>1281093.714370907</v>
       </c>
     </row>
     <row r="6">
@@ -1689,7 +2866,7 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1697,7 +2874,7 @@
         </is>
       </c>
       <c r="H6" s="2" t="n">
-        <v>9.307207185825375</v>
+        <v>13.2490890154881</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1705,7 +2882,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2168143.764890363</v>
+        <v>2171193.62467969</v>
       </c>
     </row>
     <row r="7">
@@ -1723,7 +2900,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1731,7 +2908,7 @@
         </is>
       </c>
       <c r="H7" s="2" t="n">
-        <v>8.74654837462985</v>
+        <v>15.31635142406773</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1739,7 +2916,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.09366193778912307</v>
+        <v>0.1165515941021191</v>
       </c>
     </row>
     <row r="8">
@@ -1765,7 +2942,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>3407446264.985502</v>
+        <v>4837280592.753655</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1773,7 +2950,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.423286944126012</v>
+        <v>1.34234114146773</v>
       </c>
     </row>
     <row r="9">
@@ -1799,7 +2976,7 @@
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.001321877371153106</v>
+        <v>0.001270043469758956</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1807,7 +2984,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.09323812173756052</v>
+        <v>0.09623828153247972</v>
       </c>
     </row>
     <row r="10">
@@ -1825,7 +3002,7 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.82</v>
+        <v>0.85</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1833,7 +3010,7 @@
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>70.13639222689177</v>
+        <v>227.1273881588691</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1856,7 +3033,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02338881420110402</v>
+        <v>0.02344053599430469</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1864,7 +3041,7 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>31042778.22612376</v>
+        <v>46205736.73514064</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1872,7 +3049,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>3559.80642288087</v>
+        <v>3539.60038145072</v>
       </c>
     </row>
     <row r="12">
@@ -1903,7 +3080,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>27853935.31198279</v>
+        <v>27075091.81680501</v>
       </c>
     </row>
     <row r="13">
@@ -1929,7 +3106,7 @@
         </is>
       </c>
       <c r="H13" s="2" t="n">
-        <v>64.995</v>
+        <v>64.8165</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1960,7 +3137,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.89469288882871</v>
+        <v>16.87604343537927</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1968,7 +3145,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>24.04599581368848</v>
+        <v>22.65340740850599</v>
       </c>
     </row>
     <row r="15">
@@ -1978,7 +3155,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>61.9</v>
+        <v>61.73</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1988,13 +3165,21 @@
       <c r="E15" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Cd_water</t>
+        </is>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0.001270043469758956</v>
+      </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>max_fuel</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>471795.3312582664</v>
+        <v>477913.352514101</v>
       </c>
     </row>
     <row r="16">
@@ -2004,7 +3189,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>61.9</v>
+        <v>61.73</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -2014,23 +3199,13 @@
       <c r="E16" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>Design 2</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>Empennage Design</t>
-        </is>
-      </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>mission_fuel</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>420498.0342925607</v>
+        <v>425845.5147107402</v>
       </c>
     </row>
     <row r="17">
@@ -2050,13 +3225,23 @@
       <c r="E17" s="2" t="n">
         <v>1.5</v>
       </c>
+      <c r="G17" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="H17" s="1" t="inlineStr">
+        <is>
+          <t>Empennage Design</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>8406.812305863306</v>
+        <v>8621.169392987969</v>
       </c>
     </row>
     <row r="18">
@@ -2076,13 +3261,21 @@
       <c r="E18" s="2" t="n">
         <v>1.7</v>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>S_h [m²]</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>186.9548079677261</v>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8348491265427067</v>
+        <v>0.8332604282149961</v>
       </c>
     </row>
     <row r="19">
@@ -2102,13 +3295,21 @@
       <c r="E19" s="2" t="n">
         <v>1.7</v>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>S_v [m²]</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>174.0756989743939</v>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>264734.8227817316</v>
+        <v>265612.6716394922</v>
       </c>
     </row>
     <row r="20">
@@ -2128,13 +3329,21 @@
       <c r="E20" s="2" t="n">
         <v>0.5</v>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>l_h [m]</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>30.62931767049474</v>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>S [m²]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>729.5477065258664</v>
+        <v>736.1453350695695</v>
       </c>
     </row>
     <row r="21">
@@ -2152,7 +3361,15 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>3.1</v>
+        <v>4.416363005162699</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>l_v [m]</t>
+        </is>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>30.62931767049474</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2160,7 +3377,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>85.41356487852889</v>
+        <v>85.79891229319691</v>
       </c>
     </row>
     <row r="22">
@@ -2186,7 +3403,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>8.541356487852889</v>
+        <v>8.57989122931969</v>
       </c>
     </row>
     <row r="23">
@@ -2196,7 +3413,17 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.4</v>
+        <v>0.45</v>
+      </c>
+      <c r="G23" s="1" t="inlineStr">
+        <is>
+          <t>Design 3</t>
+        </is>
+      </c>
+      <c r="H23" s="1" t="inlineStr">
+        <is>
+          <t>CG Range</t>
+        </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2204,13 +3431,13 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.07649160288323889</v>
+        <v>0.0774643478551897</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 3</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
@@ -2226,13 +3453,21 @@
       <c r="E24" s="2" t="n">
         <v>0.55</v>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>most_aft_cg [m]</t>
+        </is>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>36.94103630849455</v>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>OEW [N]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1278477.466278875</v>
+        <v>1281518.714370907</v>
       </c>
     </row>
     <row r="25">
@@ -2242,7 +3477,7 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -2252,13 +3487,23 @@
       <c r="E25" s="2" t="n">
         <v>0.9</v>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>most_aft_mission</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>ALTITUDE_OEW_PAYLOAD</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>428904.846598424</v>
+        <v>434466.6841037282</v>
       </c>
     </row>
     <row r="26">
@@ -2278,13 +3523,21 @@
       <c r="E26" s="2" t="n">
         <v>0.0838</v>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>most_forward_cg [m]</t>
+        </is>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>31.47020801445873</v>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>max_fuel</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>471795.3312582664</v>
+        <v>477913.352514101</v>
       </c>
     </row>
     <row r="27">
@@ -2302,15 +3555,25 @@
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1.423294502805824</v>
+        <v>1.174470038720226</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>most_forward_mission</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>DESIGN_OEW_FUEL</t>
+        </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>mission_fuel</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>420498.0342925607</v>
+        <v>425845.5147107402</v>
       </c>
     </row>
     <row r="28">
@@ -2320,7 +3583,7 @@
         </is>
       </c>
       <c r="B28" s="3" t="n">
-        <v>1.48e-05</v>
+        <v>1.484e-05</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2328,7 +3591,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>8406.812305863306</v>
+        <v>8621.169392987969</v>
       </c>
     </row>
     <row r="29">
@@ -2342,7 +3605,7 @@
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 3</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr">
@@ -2356,7 +3619,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8198004069149908</v>
+        <v>0.8186888779158671</v>
       </c>
     </row>
     <row r="30">
@@ -2374,7 +3637,7 @@
         </is>
       </c>
       <c r="K30" s="2" t="n">
-        <v>1720912.57500321</v>
+        <v>1733790.843393344</v>
       </c>
     </row>
     <row r="31">
@@ -2414,7 +3677,7 @@
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>12.20193783979032</v>
+        <v>12.28699770207048</v>
       </c>
     </row>
     <row r="35">
@@ -2424,7 +3687,7 @@
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>4.880775135916128</v>
+        <v>4.914799080828193</v>
       </c>
     </row>
     <row r="36">
@@ -2434,7 +3697,7 @@
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>18.30290675968548</v>
+        <v>18.43049655310572</v>
       </c>
     </row>
     <row r="37">
@@ -2454,7 +3717,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>20.2720297102992</v>
+        <v>20.26656157629547</v>
       </c>
     </row>
     <row r="39">
@@ -2464,7 +3727,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>9.064296680987093</v>
+        <v>9.127484007252358</v>
       </c>
     </row>
     <row r="40">
@@ -2474,7 +3737,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>729.5477065259233</v>
+        <v>739.7545314003578</v>
       </c>
     </row>
     <row r="41">
@@ -2484,1044 +3747,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>85.41356487853223</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="23" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Requirements</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Inputs</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>General Outputs</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Design Mission</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>design_range [m]</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>3704000</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>cruise_altitude [m]</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>d_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>8.832726010325398</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>MTOW [N]</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2618435.421524607</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>design_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aircraft_type</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>PROP</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>r_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>4.416363005162699</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>442717.4503287238</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>design_crew</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>wing_type</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>l_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>75.07817108776588</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>1286030.285774358</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ferry_range [m]</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>12038000</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>n_wings</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>l_tailcone [m]</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>39.74726704646429</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>EW [N]</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>1285605.285774358</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>reserve_range [m]</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>185200</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>n_fuselages</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>l_nose [m]</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>13.2490890154881</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>ZFW [N]</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>2175717.971195883</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ferry_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>depth</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>l_cargo_straight [m]</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>15.31635142406773</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>h_b</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>0.1162669240453023</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ferry_crew</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>jet_consumption [kg/(N·s)]</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>2.7e-05</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>4837280592.753655</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>1.34318527219474</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>altitude_range_WIG [m]</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>943600</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>prop_consumption [kg/J]</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>2.1e-08</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Cd</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>0.001270043469758956</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>WP [N/W]</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>0.09301989426111927</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>altitude_range_WOG [m]</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>538000</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>prop_efficiency</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>hull_surface [m²]</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>69.21817427258117</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>altitude_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Cd0</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02337930126140052</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>take_off_power [W]</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>14596596.60224672</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>3539.60038145072</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>altitude_crew</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>170</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>oswald_factor</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>take_off_thrust [N]</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>P [W]</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>28149198.00031495</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>cruise_speed [m/s]</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>115.749</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>V_lof [m/s]</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>64.8165</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>T [N]</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>stall_speed_clean [m/s]</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>77.16</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>tfo</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>LD_g</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>16.89812972912173</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>LD</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>22.69731897979241</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>stall_speed_takeoff [m/s]</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>61.73</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="E15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>max_fuel</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>486989.1953615962</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>stall_speed_landing [m/s]</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>61.73</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>n_engines</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>Empennage Design</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>433778.962629226</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>stall_speed_high</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>82.3</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CLmax_clean</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>8938.48769949784</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>high_altitude [m]</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>3048</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>CLmax_takeoff</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Mff</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>0.8309229065993357</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>cargo_width [m]</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CLmax_landing</t>
-        </is>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>MTOM [kg]</t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>266914.9257415501</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>cargo_height [m]</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>CL_hydro</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>739.754531400354</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>cargo_length [m]</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>r_float</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>86.00898391449314</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>cargo_density [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>160</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>upsweep</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>8.600898391449315</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>xcg_OEW</t>
-        </is>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>fuel_economy [L/ton/km]</t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>0.07890749882900248</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>General States</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>xcg_payload</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>1286030.285774358</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>design_id</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>V_h</t>
-        </is>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>442717.4503287238</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>kinematic_viscosity [m²/s]</t>
-        </is>
-      </c>
-      <c r="B26" s="3" t="n">
-        <v>1.006e-06</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>V_v</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.0838</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>max_fuel</t>
-        </is>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>486989.1953615962</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>rho_water [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>1.175466862781727</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>mission_fuel</t>
-        </is>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>433778.962629226</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>viscosity_air [m²/s]</t>
-        </is>
-      </c>
-      <c r="B28" s="3" t="n">
-        <v>1.484e-05</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K28" s="2" t="n">
-        <v>8938.48769949784</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>rho_air [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="n">
-        <v>1.225</v>
-      </c>
-      <c r="D29" s="1" t="inlineStr">
-        <is>
-          <t>Design 3</t>
-        </is>
-      </c>
-      <c r="E29" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Mff</t>
-        </is>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>0.8144958966029898</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>MTOW [N]</t>
-        </is>
-      </c>
-      <c r="K30" s="2" t="n">
-        <v>1733790.843393344</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E31" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>2.454031674527076</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>12.28699770230961</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>4.914799080923845</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>18.43049655346442</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>X_LEMAC [m]</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>21.05644</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>X_LE [m]</t>
-        </is>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>20.2665615762801</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>9.127484007429995</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>739.7545314291519</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>86.00898391616727</v>
+        <v>86.00898391449336</v>
       </c>
     </row>
     <row r="42">
@@ -3557,7 +3783,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -3639,7 +3865,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2671601.222731665</v>
+        <v>2671601.222731659</v>
       </c>
     </row>
     <row r="3">
@@ -3675,7 +3901,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>477054.4151611172</v>
+        <v>477054.4151611131</v>
       </c>
     </row>
     <row r="4">
@@ -3711,7 +3937,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1304805.956347816</v>
+        <v>1304805.956347814</v>
       </c>
     </row>
     <row r="5">
@@ -3745,7 +3971,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1304380.956347816</v>
+        <v>1304380.956347814</v>
       </c>
     </row>
     <row r="6">
@@ -3779,7 +4005,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2194546.807570548</v>
+        <v>2194546.807570545</v>
       </c>
     </row>
     <row r="7">
@@ -3813,7 +4039,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.08431602766458843</v>
+        <v>0.08431602766458753</v>
       </c>
     </row>
     <row r="8">
@@ -3847,7 +4073,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.466260010108539</v>
+        <v>1.466260010108543</v>
       </c>
     </row>
     <row r="9">
@@ -3869,7 +4095,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>Cd_water</t>
         </is>
       </c>
       <c r="H9" s="2" t="n">
@@ -3881,7 +4107,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.08235589165771251</v>
+        <v>0.08235589165771333</v>
       </c>
     </row>
     <row r="10">
@@ -3907,7 +4133,7 @@
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>48.16011913363723</v>
+        <v>50.9373226662635</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -3930,7 +4156,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02320536089523409</v>
+        <v>0.02320536089523371</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3938,7 +4164,7 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>9875567.735130826</v>
+        <v>10445052.65531117</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -3977,7 +4203,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32439709.76400051</v>
+        <v>32439709.76400011</v>
       </c>
     </row>
     <row r="13">
@@ -4034,7 +4260,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>13.13819989259041</v>
+        <v>13.13819989259052</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -4042,7 +4268,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>19.26401710731762</v>
+        <v>19.26401710731784</v>
       </c>
     </row>
     <row r="15">
@@ -4064,11 +4290,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>max_fuel</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>524759.8566772289</v>
+        <v>524759.8566772245</v>
       </c>
     </row>
     <row r="16">
@@ -4100,11 +4326,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>mission_fuel</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>466803.7826471954</v>
+        <v>466803.7826471923</v>
       </c>
     </row>
     <row r="17">
@@ -4124,13 +4350,21 @@
       <c r="E17" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>S_h [m²]</t>
+        </is>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>348.4123905193871</v>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>10250.63251392171</v>
+        <v>10250.63251392083</v>
       </c>
     </row>
     <row r="18">
@@ -4150,13 +4384,21 @@
       <c r="E18" s="2" t="n">
         <v>1.5</v>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>S_v [m²]</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>97.32319441841544</v>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8214350214013836</v>
+        <v>0.8214350214013847</v>
       </c>
     </row>
     <row r="19">
@@ -4176,13 +4418,21 @@
       <c r="E19" s="2" t="n">
         <v>1.7</v>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>l_h [m]</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>30.64474202029018</v>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>272334.4773426774</v>
+        <v>272334.4773426767</v>
       </c>
     </row>
     <row r="20">
@@ -4202,13 +4452,21 @@
       <c r="E20" s="2" t="n">
         <v>1.7</v>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>l_v [m]</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>30.64474202029018</v>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>S [m²]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>750.2024058959332</v>
+        <v>750.2024058959494</v>
       </c>
     </row>
     <row r="21">
@@ -4234,7 +4492,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>47.44056510717173</v>
+        <v>47.44056510717223</v>
       </c>
     </row>
     <row r="22">
@@ -4254,13 +4512,23 @@
       <c r="E22" s="2" t="n">
         <v>1.5</v>
       </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>Design 4</t>
+        </is>
+      </c>
+      <c r="H22" s="1" t="inlineStr">
+        <is>
+          <t>CG Range</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr">
         <is>
           <t>MAC [m]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>15.81352170239058</v>
+        <v>15.81352170239075</v>
       </c>
     </row>
     <row r="23">
@@ -4272,13 +4540,21 @@
       <c r="E23" s="2" t="n">
         <v>11</v>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>most_aft_cg [m]</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>36.92561195869911</v>
+      </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.08491495002281096</v>
+        <v>0.08491495002281038</v>
       </c>
     </row>
     <row r="24">
@@ -4300,13 +4576,23 @@
       <c r="E24" s="2" t="n">
         <v>0.45</v>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>most_aft_mission</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ALTITUDE_OEW_PAYLOAD</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>OEW [N]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1304805.956347816</v>
+        <v>1304805.956347814</v>
       </c>
     </row>
     <row r="25">
@@ -4326,13 +4612,21 @@
       <c r="E25" s="2" t="n">
         <v>0.55</v>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>most_forward_cg [m]</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>32.40212780415207</v>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>477054.4151611172</v>
+        <v>477054.4151611131</v>
       </c>
     </row>
     <row r="26">
@@ -4352,13 +4646,23 @@
       <c r="E26" s="2" t="n">
         <v>0.9</v>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>most_forward_mission</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>DESIGN_OEW_FUEL</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>max_fuel</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>524759.8566772289</v>
+        <v>524759.8566772245</v>
       </c>
     </row>
     <row r="27">
@@ -4380,11 +4684,11 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>mission_fuel</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>466803.7826471954</v>
+        <v>466803.7826471923</v>
       </c>
     </row>
     <row r="28">
@@ -4410,7 +4714,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>10250.63251392171</v>
+        <v>10250.63251392083</v>
       </c>
     </row>
     <row r="29">
@@ -4428,7 +4732,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.7948787038329889</v>
+        <v>0.7948786627699523</v>
       </c>
     </row>
     <row r="30">
@@ -4498,7 +4802,7 @@
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>22.59074529030858</v>
+        <v>22.59074528912964</v>
       </c>
     </row>
     <row r="36">
@@ -4508,7 +4812,7 @@
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>9.036298116123431</v>
+        <v>9.036298115651858</v>
       </c>
     </row>
     <row r="37">
@@ -4518,7 +4822,7 @@
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>10.16583538063886</v>
+        <v>10.16583538010834</v>
       </c>
     </row>
     <row r="38">
@@ -4538,7 +4842,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>20.33030890138294</v>
+        <v>20.33030890142084</v>
       </c>
     </row>
     <row r="40">
@@ -4548,7 +4852,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>16.78169650137209</v>
+        <v>16.78169650049631</v>
       </c>
     </row>
     <row r="41">
@@ -4558,7 +4862,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>750.2024059742508</v>
+        <v>750.2024058959494</v>
       </c>
     </row>
     <row r="42">
@@ -4568,7 +4872,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>47.44056510964801</v>
+        <v>47.44056510717223</v>
       </c>
     </row>
     <row r="43">

</xml_diff>

<commit_message>
Refactor Cd0 estimation and update design data
- Updated tail_wet method in Cd0Estimation.py to use empennage surface areas.
- Modified Cd0 values in design JSON files to reflect new calculations.
- Adjusted various design parameters across multiple design JSON files for accuracy.
- Enhanced AircraftIteration class to correctly assign 'k' value based on mission type.
- Refactored main function to iterate over all mission types for Cd0 estimation.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -438,13 +438,13 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2630224.648699609</v>
+        <v>2650876.583481097</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>450331.4854738471</v>
+        <v>463669.4723415911</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1290193.688577062</v>
+        <v>1297486.984556024</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1289768.688577062</v>
+        <v>1297061.984556024</v>
       </c>
     </row>
     <row r="6">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2179893.163225762</v>
+        <v>2187207.111139506</v>
       </c>
     </row>
     <row r="7">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.06008755531464768</v>
+        <v>0.05985318932693635</v>
       </c>
     </row>
     <row r="8">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>13.08369566255593</v>
+        <v>12.42619345649818</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.62379977113597</v>
+        <v>1.625794215105503</v>
       </c>
     </row>
     <row r="9">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.08193335381292018</v>
+        <v>0.07676623795780944</v>
       </c>
     </row>
     <row r="10">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02339910199117182</v>
+        <v>0.02594082812541138</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32102001.52071457</v>
+        <v>34531802.703918</v>
       </c>
     </row>
     <row r="13">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>21.245302022471</v>
+        <v>20.2024334373566</v>
       </c>
     </row>
     <row r="15">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>495364.6340212318</v>
+        <v>510036.4195757503</v>
       </c>
     </row>
     <row r="16">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>441100.8727192181</v>
+        <v>453928.7344860725</v>
       </c>
     </row>
     <row r="17">
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>240.7046751102362</v>
+        <v>240.7046751102366</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>9230.612754628994</v>
+        <v>9740.737855518644</v>
       </c>
     </row>
     <row r="18">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>134.4736784949187</v>
+        <v>134.4736784949189</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8287859230212551</v>
+        <v>0.8250882461933756</v>
       </c>
     </row>
     <row r="19">
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>30.63951259439536</v>
+        <v>30.63951259439532</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>268116.6818246288</v>
+        <v>270221.8739532208</v>
       </c>
     </row>
     <row r="20">
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.63951259439536</v>
+        <v>30.63951259439532</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>738.5836039870188</v>
+        <v>744.3790437215927</v>
       </c>
     </row>
     <row r="21">
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>66.56952473859276</v>
+        <v>66.83018975230847</v>
       </c>
     </row>
     <row r="22">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>11.09492078976546</v>
+        <v>11.13836495871808</v>
       </c>
     </row>
     <row r="23">
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>36.93084138459393</v>
+        <v>36.93084138459397</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.08023940669366754</v>
+        <v>0.08257288658677123</v>
       </c>
     </row>
     <row r="24">
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1290193.688577062</v>
+        <v>1297486.984556024</v>
       </c>
     </row>
     <row r="25">
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="H25" s="2" t="n">
-        <v>31.79288673099522</v>
+        <v>33.78517698949464</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1281,7 +1281,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>450331.4854738471</v>
+        <v>463669.4723415911</v>
       </c>
     </row>
     <row r="26">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>DESIGN_OEW_FUEL</t>
+          <t>DESIGN_OEW</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>495364.6340212318</v>
+        <v>510036.4195757503</v>
       </c>
     </row>
     <row r="27">
@@ -1343,7 +1343,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>441100.8727192181</v>
+        <v>453928.7344860725</v>
       </c>
     </row>
     <row r="28">
@@ -1369,7 +1369,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>9230.612754628994</v>
+        <v>9740.737855518644</v>
       </c>
     </row>
     <row r="29">
@@ -1395,7 +1395,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8056774888768197</v>
+        <v>0.7989301431583113</v>
       </c>
     </row>
     <row r="30">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>21.05644</v>
+        <v>30.03126843510636</v>
       </c>
     </row>
     <row r="41">
@@ -1507,7 +1507,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>20.03751870298073</v>
+        <v>29.01234713808708</v>
       </c>
     </row>
     <row r="42">
@@ -2146,7 +2146,7 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>243.0584944865134</v>
+        <v>243.1178115077496</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>226.3144648663313</v>
+        <v>226.3696956038824</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2214,7 +2214,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>22.91446344560504</v>
+        <v>22.90887266759338</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2248,7 +2248,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>22.91446344560504</v>
+        <v>22.90887266759338</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2336,7 +2336,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>24.55229320210437</v>
+        <v>24.55788398011603</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2530,7 +2530,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8238427162961426</v>
+        <v>0.8238427162976993</v>
       </c>
     </row>
     <row r="30">
@@ -2650,7 +2650,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>21.05644</v>
+        <v>21.09633628787085</v>
       </c>
     </row>
     <row r="42">
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>20.2738353405413</v>
+        <v>20.31373162841215</v>
       </c>
     </row>
     <row r="43">
@@ -3333,7 +3333,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>185.6057148332545</v>
+        <v>185.6057148332636</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>172.8195433669636</v>
+        <v>172.8195433669721</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -3401,7 +3401,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.62643959261036</v>
+        <v>30.62643959260885</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3435,7 +3435,7 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>30.62643959261036</v>
+        <v>30.62643959260885</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>36.94391438637893</v>
+        <v>36.94391438638043</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -3595,7 +3595,7 @@
         </is>
       </c>
       <c r="H26" s="2" t="n">
-        <v>31.49295374709665</v>
+        <v>33.78517698949464</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3630,7 +3630,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>DESIGN_OEW_FUEL</t>
+          <t>DESIGN_OEW</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -3691,7 +3691,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8186888149662509</v>
+        <v>0.8186888149672051</v>
       </c>
     </row>
     <row r="30">
@@ -3811,7 +3811,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>21.05644</v>
+        <v>30.03126843510636</v>
       </c>
     </row>
     <row r="42">
@@ -3821,7 +3821,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>20.26849080547514</v>
+        <v>29.24331924058149</v>
       </c>
     </row>
     <row r="43">
@@ -3890,7 +3890,7 @@
     <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="23" customWidth="1" min="8" max="8"/>
+    <col width="27" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
     <col width="21" customWidth="1" min="11" max="11"/>
@@ -3969,7 +3969,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2671601.222731658</v>
+        <v>2671601.222731657</v>
       </c>
     </row>
     <row r="3">
@@ -4005,7 +4005,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>477054.4151611137</v>
+        <v>477054.4151611129</v>
       </c>
     </row>
     <row r="4">
@@ -4041,7 +4041,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1304805.956347813</v>
+        <v>1304805.956347812</v>
       </c>
     </row>
     <row r="5">
@@ -4075,7 +4075,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1304380.956347813</v>
+        <v>1304380.956347812</v>
       </c>
     </row>
     <row r="6">
@@ -4143,7 +4143,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.08431602766458754</v>
+        <v>0.08431602766458753</v>
       </c>
     </row>
     <row r="8">
@@ -4307,7 +4307,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32439709.76400011</v>
+        <v>32439709.7640001</v>
       </c>
     </row>
     <row r="13">
@@ -4398,7 +4398,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>524759.8566772251</v>
+        <v>524759.8566772243</v>
       </c>
     </row>
     <row r="16">
@@ -4434,7 +4434,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>466803.7826471922</v>
+        <v>466803.7826471921</v>
       </c>
     </row>
     <row r="17">
@@ -4460,7 +4460,7 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>348.4123905193982</v>
+        <v>350.1374236528796</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -4468,7 +4468,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>10250.63251392142</v>
+        <v>10250.63251392083</v>
       </c>
     </row>
     <row r="18">
@@ -4494,7 +4494,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>97.32319441841854</v>
+        <v>97.80505367370436</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -4502,7 +4502,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8214350214013845</v>
+        <v>0.8214350214013847</v>
       </c>
     </row>
     <row r="19">
@@ -4528,7 +4528,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>30.6447420202892</v>
+        <v>30.49376359930098</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -4536,7 +4536,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>272334.4773426767</v>
+        <v>272334.4773426765</v>
       </c>
     </row>
     <row r="20">
@@ -4562,7 +4562,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.6447420202892</v>
+        <v>30.49376359930098</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -4570,7 +4570,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>750.202405895949</v>
+        <v>750.2024058959493</v>
       </c>
     </row>
     <row r="21">
@@ -4632,7 +4632,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>15.81352170239074</v>
+        <v>15.81352170239075</v>
       </c>
     </row>
     <row r="23">
@@ -4650,7 +4650,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>36.92561195870009</v>
+        <v>37.07659037968831</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -4658,7 +4658,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.08491495002281038</v>
+        <v>0.08491495002281035</v>
       </c>
     </row>
     <row r="24">
@@ -4687,7 +4687,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>ALTITUDE_OEW_PAYLOAD</t>
+          <t>ALTITUDE_OEW_PAYLOAD_FUEL</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -4696,7 +4696,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1304805.956347813</v>
+        <v>1304805.956347812</v>
       </c>
     </row>
     <row r="25">
@@ -4722,7 +4722,7 @@
         </is>
       </c>
       <c r="H25" s="2" t="n">
-        <v>32.40212780415207</v>
+        <v>33.78517698949464</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -4730,7 +4730,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>477054.4151611137</v>
+        <v>477054.4151611129</v>
       </c>
     </row>
     <row r="26">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>DESIGN_OEW_FUEL</t>
+          <t>DESIGN_OEW</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -4766,7 +4766,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>524759.8566772251</v>
+        <v>524759.8566772243</v>
       </c>
     </row>
     <row r="27">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>466803.7826471922</v>
+        <v>466803.7826471921</v>
       </c>
     </row>
     <row r="28">
@@ -4818,7 +4818,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>10250.63251392142</v>
+        <v>10250.63251392083</v>
       </c>
     </row>
     <row r="29">
@@ -4844,7 +4844,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.7948786627141319</v>
+        <v>0.7948786627141348</v>
       </c>
     </row>
     <row r="30">
@@ -4955,7 +4955,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>9.036298115651856</v>
+        <v>9.036298115651855</v>
       </c>
     </row>
     <row r="41">
@@ -4975,7 +4975,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>21.05644</v>
+        <v>30.03126843510636</v>
       </c>
     </row>
     <row r="43">
@@ -4985,7 +4985,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>20.33030890142084</v>
+        <v>29.30513733652719</v>
       </c>
     </row>
     <row r="44">
@@ -5005,7 +5005,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>750.2024058959493</v>
+        <v>750.202405895949</v>
       </c>
     </row>
     <row r="46">

</xml_diff>

<commit_message>
Update aircraft design parameters and calculations
- Adjusted drag coefficient (Cd0) values in design2.json, design3.json, and design4.json for improved aerodynamic accuracy.
- Modified vertical and horizontal center of gravity (xcg) parameters in design2.json, design3.json, and design4.json to reflect updated configurations.
- Increased mass fractions for wing and fuselage in design2.json, design3.json, and design4.json to account for structural changes.
- Revised various performance metrics including MTOW, total fuel, OEW, and fuel economy across all design files to enhance overall aircraft performance.
- Updated the Iteration.py script to include maximum lift-to-drag ratio (LD) calculations in the outputs for design, ferry, and altitude scenarios.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -438,7 +438,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2650876.583481097</v>
+        <v>2535043.010301131</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>463669.4723415911</v>
+        <v>388858.7248612563</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1297486.984556024</v>
+        <v>1256579.992429574</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1297061.984556024</v>
+        <v>1256154.992429574</v>
       </c>
     </row>
     <row r="6">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2187207.111139506</v>
+        <v>2146184.285439875</v>
       </c>
     </row>
     <row r="7">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.05985318932693635</v>
+        <v>0.04740934087046762</v>
       </c>
     </row>
     <row r="8">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>12.42619345649818</v>
+        <v>16.0696979793025</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.625794215105503</v>
+        <v>1.752476118452925</v>
       </c>
     </row>
     <row r="9">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.07676623795780944</v>
+        <v>0.08975876618484213</v>
       </c>
     </row>
     <row r="10">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02594082812541138</v>
+        <v>0.02585195421099691</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>34531802.703918</v>
+        <v>28242845.99768967</v>
       </c>
     </row>
     <row r="13">
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>20.2024334373566</v>
+        <v>28.16176193947887</v>
       </c>
     </row>
     <row r="15">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>510036.4195757503</v>
+        <v>427744.597347382</v>
       </c>
     </row>
     <row r="16">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>453928.7344860725</v>
+        <v>382006.368650084</v>
       </c>
     </row>
     <row r="17">
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>240.7046751102366</v>
+        <v>166.7313236276682</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>9740.737855518644</v>
+        <v>6852.356211172359</v>
       </c>
     </row>
     <row r="18">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>134.4736784949189</v>
+        <v>149.6658822681303</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8250882461933756</v>
+        <v>0.8466066558708742</v>
       </c>
     </row>
     <row r="19">
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>30.63951259439532</v>
+        <v>30.61860656663953</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>270221.8739532208</v>
+        <v>258414.170265151</v>
       </c>
     </row>
     <row r="20">
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.63951259439532</v>
+        <v>30.61860656663953</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>744.3790437215927</v>
+        <v>711.8559966653349</v>
       </c>
     </row>
     <row r="21">
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>66.83018975230847</v>
+        <v>84.37155899148331</v>
       </c>
     </row>
     <row r="22">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>11.13836495871808</v>
+        <v>8.437155899148332</v>
       </c>
     </row>
     <row r="23">
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>36.93084138459397</v>
+        <v>36.95174741234976</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.08257288658677123</v>
+        <v>0.06948969333188471</v>
       </c>
     </row>
     <row r="24">
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1297486.984556024</v>
+        <v>1256579.992429574</v>
       </c>
     </row>
     <row r="25">
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.0838</v>
+        <v>0.083867</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="H25" s="2" t="n">
-        <v>33.78517698949464</v>
+        <v>33.6303205104692</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1281,7 +1281,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>463669.4723415911</v>
+        <v>388858.7248612563</v>
       </c>
     </row>
     <row r="26">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>DESIGN_OEW</t>
+          <t>DESIGN_OEW_FUEL</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>510036.4195757503</v>
+        <v>427744.597347382</v>
       </c>
     </row>
     <row r="27">
@@ -1343,7 +1343,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>453928.7344860725</v>
+        <v>382006.368650084</v>
       </c>
     </row>
     <row r="28">
@@ -1369,7 +1369,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>9740.737855518644</v>
+        <v>6852.356211172359</v>
       </c>
     </row>
     <row r="29">
@@ -1395,7 +1395,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.7989301431583113</v>
+        <v>0.8374736970559907</v>
       </c>
     </row>
     <row r="30">
@@ -1407,6 +1407,14 @@
       <c r="E30" s="2" t="n">
         <v>0.08</v>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>28.16176193947887</v>
+      </c>
     </row>
     <row r="32">
       <c r="D32" s="1" t="inlineStr">
@@ -1457,7 +1465,7 @@
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>4.085616779974877</v>
+        <v>2.454031674527076</v>
       </c>
     </row>
     <row r="37">
@@ -1467,7 +1475,7 @@
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>15.84988684252209</v>
+        <v>12.0530379738033</v>
       </c>
     </row>
     <row r="38">
@@ -1477,7 +1485,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>6.339954737008835</v>
+        <v>4.821215189521321</v>
       </c>
     </row>
     <row r="39">
@@ -1487,7 +1495,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>14.26489815826988</v>
+        <v>18.07955696070495</v>
       </c>
     </row>
     <row r="40">
@@ -1497,7 +1505,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>30.03126843510636</v>
+        <v>28.95682619287017</v>
       </c>
     </row>
     <row r="41">
@@ -1507,7 +1515,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>29.01234713808708</v>
+        <v>28.18198803741139</v>
       </c>
     </row>
     <row r="42">
@@ -1517,7 +1525,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>11.77420165444498</v>
+        <v>8.953685351968167</v>
       </c>
     </row>
     <row r="43">
@@ -1527,7 +1535,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>738.5836039870188</v>
+        <v>711.8510495499273</v>
       </c>
     </row>
     <row r="44">
@@ -1537,7 +1545,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>66.56952473859276</v>
+        <v>84.37126581662309</v>
       </c>
     </row>
     <row r="45">
@@ -1547,7 +1555,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1576,10 +1584,10 @@
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="27" customWidth="1" min="8" max="8"/>
+    <col width="23" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1655,7 +1663,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2585106.105315377</v>
+        <v>2610442.412995288</v>
       </c>
     </row>
     <row r="3">
@@ -1691,7 +1699,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>421191.8166961765</v>
+        <v>437555.191008916</v>
       </c>
     </row>
     <row r="4">
@@ -1727,7 +1735,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1274259.932513885</v>
+        <v>1283207.529573377</v>
       </c>
     </row>
     <row r="5">
@@ -1761,7 +1769,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1273834.932513885</v>
+        <v>1282782.529573377</v>
       </c>
     </row>
     <row r="6">
@@ -1795,7 +1803,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2163914.288619201</v>
+        <v>2172887.221986372</v>
       </c>
     </row>
     <row r="7">
@@ -1829,7 +1837,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.09387803518307419</v>
+        <v>0.09342134021245534</v>
       </c>
     </row>
     <row r="8">
@@ -1863,7 +1871,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.422374919553053</v>
+        <v>1.424306358628104</v>
       </c>
     </row>
     <row r="9">
@@ -1897,7 +1905,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.09647518482399101</v>
+        <v>0.08665443614762731</v>
       </c>
     </row>
     <row r="10">
@@ -1946,7 +1954,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02344655710855558</v>
+        <v>0.02707970372361656</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1993,7 +2001,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>26795554.83652751</v>
+        <v>30124740.6254892</v>
       </c>
     </row>
     <row r="13">
@@ -2050,7 +2058,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.8738763984543</v>
+        <v>15.70118567185378</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -2058,7 +2066,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>24.00097858479959</v>
+        <v>22.36329859042182</v>
       </c>
     </row>
     <row r="15">
@@ -2084,7 +2092,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>463310.9983657943</v>
+        <v>481310.7101098076</v>
       </c>
     </row>
     <row r="16">
@@ -2120,7 +2128,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>413082.8798535989</v>
+        <v>428815.146324671</v>
       </c>
     </row>
     <row r="17">
@@ -2146,7 +2154,7 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>243.1178115077496</v>
+        <v>245.2699382238973</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2154,7 +2162,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>8108.93684257759</v>
+        <v>8740.04468424496</v>
       </c>
     </row>
     <row r="18">
@@ -2180,7 +2188,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>226.3696956038824</v>
+        <v>228.3735647018066</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2188,7 +2196,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8370698147243778</v>
+        <v>0.832382745227138</v>
       </c>
     </row>
     <row r="19">
@@ -2214,7 +2222,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>22.90887266759338</v>
+        <v>23.04539858668156</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2222,7 +2230,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>263517.441928173</v>
+        <v>266100.1440362169</v>
       </c>
     </row>
     <row r="20">
@@ -2248,7 +2256,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>22.90887266759338</v>
+        <v>23.04539858668156</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2256,7 +2264,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>726.1928875400224</v>
+        <v>733.3103037384867</v>
       </c>
     </row>
     <row r="21">
@@ -2282,7 +2290,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>85.21695180772558</v>
+        <v>85.63353920856517</v>
       </c>
     </row>
     <row r="22">
@@ -2318,7 +2326,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>8.521695180772559</v>
+        <v>8.563353920856516</v>
       </c>
     </row>
     <row r="23">
@@ -2336,7 +2344,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>24.55788398011603</v>
+        <v>24.42135806102785</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2344,7 +2352,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.0751427332039378</v>
+        <v>0.07800454510606263</v>
       </c>
     </row>
     <row r="24">
@@ -2373,7 +2381,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>ALTITUDE_OEW_PAYLOAD_FUEL</t>
+          <t>ALTITUDE_OEW_PAYLOAD</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2382,7 +2390,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1274259.932513885</v>
+        <v>1283207.529573377</v>
       </c>
     </row>
     <row r="25">
@@ -2400,7 +2408,7 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.0838</v>
+        <v>0.083867</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -2416,7 +2424,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>421191.8166961765</v>
+        <v>437555.191008916</v>
       </c>
     </row>
     <row r="26">
@@ -2452,7 +2460,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>463310.9983657943</v>
+        <v>481310.7101098076</v>
       </c>
     </row>
     <row r="27">
@@ -2478,7 +2486,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>413082.8798535989</v>
+        <v>428815.146324671</v>
       </c>
     </row>
     <row r="28">
@@ -2504,7 +2512,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>8108.93684257759</v>
+        <v>8740.04468424496</v>
       </c>
     </row>
     <row r="29">
@@ -2530,7 +2538,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8238427162976993</v>
+        <v>0.8153246717564306</v>
       </c>
     </row>
     <row r="30">
@@ -2540,7 +2548,7 @@
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2558,7 +2566,15 @@
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>22.36329859042182</v>
       </c>
     </row>
     <row r="33">
@@ -2620,7 +2636,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>12.17385025824651</v>
+        <v>12.23387312081413</v>
       </c>
     </row>
     <row r="39">
@@ -2630,7 +2646,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>4.869540103298605</v>
+        <v>4.893549248325652</v>
       </c>
     </row>
     <row r="40">
@@ -2640,7 +2656,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>18.26077538736977</v>
+        <v>18.35080968122119</v>
       </c>
     </row>
     <row r="41">
@@ -2650,7 +2666,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>21.09633628787085</v>
+        <v>20.00577388395828</v>
       </c>
     </row>
     <row r="42">
@@ -2660,7 +2676,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>20.31373162841215</v>
+        <v>19.21931061190594</v>
       </c>
     </row>
     <row r="43">
@@ -2670,7 +2686,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>9.043431620411695</v>
+        <v>9.08802003260478</v>
       </c>
     </row>
     <row r="44">
@@ -2680,7 +2696,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>726.1928875400224</v>
+        <v>733.371492527274</v>
       </c>
     </row>
     <row r="45">
@@ -2690,7 +2706,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>85.21695180772558</v>
+        <v>85.63711184569888</v>
       </c>
     </row>
     <row r="46">
@@ -2726,7 +2742,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -2808,7 +2824,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2605660.308785691</v>
+        <v>2622957.14200784</v>
       </c>
     </row>
     <row r="3">
@@ -2844,7 +2860,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>434466.6841051969</v>
+        <v>445637.789224964</v>
       </c>
     </row>
     <row r="4">
@@ -2880,7 +2896,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1281518.714371709</v>
+        <v>1287627.145640868</v>
       </c>
     </row>
     <row r="5">
@@ -2914,7 +2930,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1281093.714371709</v>
+        <v>1287202.145640868</v>
       </c>
     </row>
     <row r="6">
@@ -2948,7 +2964,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2171193.624680494</v>
+        <v>2177319.352782876</v>
       </c>
     </row>
     <row r="7">
@@ -2982,7 +2998,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.1165515941027839</v>
+        <v>0.1161666644374126</v>
       </c>
     </row>
     <row r="8">
@@ -3016,7 +3032,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.342341141465762</v>
+        <v>1.343483387947545</v>
       </c>
     </row>
     <row r="9">
@@ -3050,7 +3066,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.09623828153181459</v>
+        <v>0.08980979329635373</v>
       </c>
     </row>
     <row r="10">
@@ -3099,7 +3115,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02344053599452553</v>
+        <v>0.02572776629574262</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3146,7 +3162,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>27075091.81701575</v>
+        <v>29205691.78188201</v>
       </c>
     </row>
     <row r="13">
@@ -3203,7 +3219,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.87604343529977</v>
+        <v>16.10843550119909</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -3211,7 +3227,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>22.65340740836607</v>
+        <v>21.64141550168546</v>
       </c>
     </row>
     <row r="15">
@@ -3245,7 +3261,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>477913.3525157166</v>
+        <v>490201.5681474604</v>
       </c>
     </row>
     <row r="16">
@@ -3271,7 +3287,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>425845.514712152</v>
+        <v>436587.1783089098</v>
       </c>
     </row>
     <row r="17">
@@ -3307,7 +3323,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>8621.169393044955</v>
+        <v>9050.610916054167</v>
       </c>
     </row>
     <row r="18">
@@ -3333,7 +3349,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>185.6057148332636</v>
+        <v>187.4330750456031</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -3341,7 +3357,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8332604282145779</v>
+        <v>0.8301010023809104</v>
       </c>
     </row>
     <row r="19">
@@ -3367,7 +3383,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>172.8195433669721</v>
+        <v>174.5210187646838</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -3375,7 +3391,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>265612.6716397239</v>
+        <v>267375.8554544179</v>
       </c>
     </row>
     <row r="20">
@@ -3401,7 +3417,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.62643959260885</v>
+        <v>30.63033313524951</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3409,7 +3425,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>736.1453350611716</v>
+        <v>741.03199779522</v>
       </c>
     </row>
     <row r="21">
@@ -3435,7 +3451,7 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>30.62643959260885</v>
+        <v>30.63033313524951</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -3443,7 +3459,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>85.79891229270751</v>
+        <v>86.08321542526278</v>
       </c>
     </row>
     <row r="22">
@@ -3469,7 +3485,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>8.579891229270752</v>
+        <v>8.608321542526278</v>
       </c>
     </row>
     <row r="23">
@@ -3497,7 +3513,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.07746434785544652</v>
+        <v>0.07941833336582084</v>
       </c>
     </row>
     <row r="24">
@@ -3525,7 +3541,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>36.94391438638043</v>
+        <v>36.94002084373978</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -3533,7 +3549,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1281518.714371709</v>
+        <v>1287627.145640868</v>
       </c>
     </row>
     <row r="25">
@@ -3551,7 +3567,7 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.0838</v>
+        <v>0.083867</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -3569,7 +3585,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>434466.6841051969</v>
+        <v>445637.789224964</v>
       </c>
     </row>
     <row r="26">
@@ -3595,7 +3611,7 @@
         </is>
       </c>
       <c r="H26" s="2" t="n">
-        <v>33.78517698949464</v>
+        <v>33.63463057823858</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3603,7 +3619,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>477913.3525157166</v>
+        <v>490201.5681474604</v>
       </c>
     </row>
     <row r="27">
@@ -3630,7 +3646,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>DESIGN_OEW</t>
+          <t>DESIGN_OEW_FUEL</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -3639,7 +3655,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>425845.514712152</v>
+        <v>436587.1783089098</v>
       </c>
     </row>
     <row r="28">
@@ -3665,7 +3681,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>8621.169393044955</v>
+        <v>9050.610916054167</v>
       </c>
     </row>
     <row r="29">
@@ -3691,7 +3707,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8186888149672051</v>
+        <v>0.8130244787342943</v>
       </c>
     </row>
     <row r="30">
@@ -3701,7 +3717,7 @@
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3719,7 +3735,15 @@
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>21.64141550168546</v>
       </c>
     </row>
     <row r="33">
@@ -3781,7 +3805,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>12.25698747038679</v>
+        <v>12.29760219641277</v>
       </c>
     </row>
     <row r="39">
@@ -3791,7 +3815,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>4.902794988154715</v>
+        <v>4.919040878565108</v>
       </c>
     </row>
     <row r="40">
@@ -3801,7 +3825,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>18.38548120558018</v>
+        <v>18.44640329461915</v>
       </c>
     </row>
     <row r="41">
@@ -3811,7 +3835,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>30.03126843510636</v>
+        <v>28.93502503931185</v>
       </c>
     </row>
     <row r="42">
@@ -3821,7 +3845,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>29.24331924058149</v>
+        <v>28.14446489811388</v>
       </c>
     </row>
     <row r="43">
@@ -3831,7 +3855,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>9.105190692287326</v>
+        <v>9.135361631620913</v>
       </c>
     </row>
     <row r="44">
@@ -3841,7 +3865,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>736.1453350611716</v>
+        <v>741.0319969279589</v>
       </c>
     </row>
     <row r="45">
@@ -3851,7 +3875,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>85.79891229270751</v>
+        <v>86.08321537488936</v>
       </c>
     </row>
     <row r="46">
@@ -3890,7 +3914,7 @@
     <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="27" customWidth="1" min="8" max="8"/>
+    <col width="23" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
     <col width="21" customWidth="1" min="11" max="11"/>
@@ -3969,7 +3993,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2671601.222731657</v>
+        <v>2700961.475400982</v>
       </c>
     </row>
     <row r="3">
@@ -4005,7 +4029,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>477054.4151611129</v>
+        <v>496016.6416391923</v>
       </c>
     </row>
     <row r="4">
@@ -4041,7 +4065,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1304805.956347812</v>
+        <v>1315174.622286388</v>
       </c>
     </row>
     <row r="5">
@@ -4075,7 +4099,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1304380.956347812</v>
+        <v>1314749.622286388</v>
       </c>
     </row>
     <row r="6">
@@ -4109,7 +4133,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2194546.807570545</v>
+        <v>2204944.83376179</v>
       </c>
     </row>
     <row r="7">
@@ -4143,7 +4167,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.08431602766458753</v>
+        <v>0.08385649659017519</v>
       </c>
     </row>
     <row r="8">
@@ -4177,7 +4201,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.466260010108543</v>
+        <v>1.468568290239539</v>
       </c>
     </row>
     <row r="9">
@@ -4211,7 +4235,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.08235589165771333</v>
+        <v>0.07590230305533839</v>
       </c>
     </row>
     <row r="10">
@@ -4260,7 +4284,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02320536089523372</v>
+        <v>0.02639956891071301</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -4307,7 +4331,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>32439709.7640001</v>
+        <v>35584710.43272272</v>
       </c>
     </row>
     <row r="13">
@@ -4364,7 +4388,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>13.13819989259052</v>
+        <v>12.31775640184354</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -4372,7 +4396,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>19.26401710731783</v>
+        <v>18.08946645864251</v>
       </c>
     </row>
     <row r="15">
@@ -4398,7 +4422,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>524759.8566772243</v>
+        <v>545618.3058031115</v>
       </c>
     </row>
     <row r="16">
@@ -4434,7 +4458,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>466803.7826471921</v>
+        <v>485047.0515637147</v>
       </c>
     </row>
     <row r="17">
@@ -4460,7 +4484,7 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>350.1374236528796</v>
+        <v>354.1396874821904</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -4468,7 +4492,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>10250.63251392083</v>
+        <v>10969.59007547755</v>
       </c>
     </row>
     <row r="18">
@@ -4494,7 +4518,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>97.80505367370436</v>
+        <v>98.92301937002517</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -4502,7 +4526,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8214350214013847</v>
+        <v>0.8163555288897432</v>
       </c>
     </row>
     <row r="19">
@@ -4528,7 +4552,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>30.49376359930098</v>
+        <v>30.65149497925002</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -4536,7 +4560,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>272334.4773426765</v>
+        <v>275327.3675230358</v>
       </c>
     </row>
     <row r="20">
@@ -4562,7 +4586,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.49376359930098</v>
+        <v>30.65149497925002</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -4570,7 +4594,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>750.2024058959493</v>
+        <v>758.4471076824697</v>
       </c>
     </row>
     <row r="21">
@@ -4596,7 +4620,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>47.44056510717223</v>
+        <v>47.70053797440244</v>
       </c>
     </row>
     <row r="22">
@@ -4632,7 +4656,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>15.81352170239075</v>
+        <v>15.90017932480081</v>
       </c>
     </row>
     <row r="23">
@@ -4650,7 +4674,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>37.07659037968831</v>
+        <v>36.91885899973926</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -4658,7 +4682,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.08491495002281035</v>
+        <v>0.08823353124662627</v>
       </c>
     </row>
     <row r="24">
@@ -4687,7 +4711,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>ALTITUDE_OEW_PAYLOAD_FUEL</t>
+          <t>ALTITUDE_OEW_PAYLOAD</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -4696,7 +4720,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1304805.956347812</v>
+        <v>1315174.622286388</v>
       </c>
     </row>
     <row r="25">
@@ -4730,7 +4754,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>477054.4151611129</v>
+        <v>496016.6416391923</v>
       </c>
     </row>
     <row r="26">
@@ -4748,7 +4772,7 @@
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.0838</v>
+        <v>0.083867</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -4766,7 +4790,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>524759.8566772243</v>
+        <v>545618.3058031115</v>
       </c>
     </row>
     <row r="27">
@@ -4792,7 +4816,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>466803.7826471921</v>
+        <v>485047.0515637147</v>
       </c>
     </row>
     <row r="28">
@@ -4818,7 +4842,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>10250.63251392083</v>
+        <v>10969.59007547755</v>
       </c>
     </row>
     <row r="29">
@@ -4844,7 +4868,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.7948786627141348</v>
+        <v>0.7858151769334533</v>
       </c>
     </row>
     <row r="30">
@@ -4872,7 +4896,15 @@
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>18.08946645864251</v>
       </c>
     </row>
     <row r="32">
@@ -4882,7 +4914,7 @@
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="33"/>
@@ -4945,7 +4977,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>22.59074528912964</v>
+        <v>22.7155257137488</v>
       </c>
     </row>
     <row r="40">
@@ -4955,7 +4987,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>9.036298115651855</v>
+        <v>9.086210285499522</v>
       </c>
     </row>
     <row r="41">
@@ -4965,7 +4997,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>10.16583538010834</v>
+        <v>10.22198657118696</v>
       </c>
     </row>
     <row r="42">
@@ -4975,7 +5007,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>30.03126843510636</v>
+        <v>28.00634157148075</v>
       </c>
     </row>
     <row r="43">
@@ -4985,7 +5017,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>29.30513733652719</v>
+        <v>27.27619967353882</v>
       </c>
     </row>
     <row r="44">
@@ -4995,7 +5027,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>16.7816965004963</v>
+        <v>16.8743905302134</v>
       </c>
     </row>
     <row r="45">
@@ -5005,7 +5037,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>750.202405895949</v>
+        <v>758.5128094244151</v>
       </c>
     </row>
     <row r="46">
@@ -5015,7 +5047,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>47.44056510717223</v>
+        <v>47.70260399887248</v>
       </c>
     </row>
     <row r="47">

</xml_diff>

<commit_message>
Update design parameters and calculations in JSON files and PayloadRange.py
- Adjusted aerodynamic coefficients (Cd0) in design2.json, design3.json, and design4.json for improved accuracy.
- Modified lift-to-drag ratios (LD_g) in design2.json and design3.json to reflect updated calculations.
- Updated various weight and fuel metrics in design2.json, design3.json, and design4.json, including MTOW, total fuel, and mission fuel.
- Corrected wing design parameters in design2.json, design3.json, and design4.json for better aerodynamic performance.
- Changed the fuel extraction logic in PayloadRange.py to use 'mission_fuel' instead of 'total_fuel' for more accurate range calculations.
- Added reserve fuel extraction in PayloadRange.py to account for fuel reserves in range calculations.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 1 Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 2 Data" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 3 Data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 4 Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Design 1 Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Design 2 Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Design 3 Data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Design 4 Data" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,17 +18,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -43,7 +55,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -53,17 +72,50 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -142,10 +194,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -183,69 +235,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -269,54 +323,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -326,7 +379,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -335,7 +388,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -344,7 +397,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -352,10 +405,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -384,7 +437,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -397,13 +450,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -438,7 +490,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -448,42 +500,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>Requirements</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Inputs</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>General Outputs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="12" t="inlineStr">
         <is>
           <t>Design Mission</t>
         </is>
@@ -495,7 +547,7 @@
           <t>design_range [m]</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="13" t="n">
         <v>3704000</v>
       </c>
       <c r="D2" t="inlineStr">
@@ -503,7 +555,7 @@
           <t>cruise_altitude [m]</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="13" t="n">
         <v>4</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -511,7 +563,7 @@
           <t>d_fuselage [m]</t>
         </is>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="13" t="n">
         <v>8.832726010325398</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -519,8 +571,8 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K2" s="2" t="n">
-        <v>2630224.648699611</v>
+      <c r="K2" s="13" t="n">
+        <v>2630224.648699607</v>
       </c>
     </row>
     <row r="3">
@@ -529,7 +581,7 @@
           <t>design_payload [kg]</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D3" t="inlineStr">
@@ -547,7 +599,7 @@
           <t>r_fuselage [m]</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="13" t="n">
         <v>4.416363005162699</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -555,8 +607,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K3" s="2" t="n">
-        <v>450331.4854738481</v>
+      <c r="K3" s="13" t="n">
+        <v>450331.4854738463</v>
       </c>
     </row>
     <row r="4">
@@ -565,7 +617,7 @@
           <t>design_crew</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D4" t="inlineStr">
@@ -583,7 +635,7 @@
           <t>l_fuselage [m]</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="13" t="n">
         <v>75.07817108776588</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -591,8 +643,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K4" s="2" t="n">
-        <v>1290193.688577064</v>
+      <c r="K4" s="13" t="n">
+        <v>1290193.688577061</v>
       </c>
     </row>
     <row r="5">
@@ -601,7 +653,7 @@
           <t>ferry_range [m]</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="13" t="n">
         <v>12038000</v>
       </c>
       <c r="D5" t="inlineStr">
@@ -609,7 +661,7 @@
           <t>n_wings</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
@@ -617,7 +669,7 @@
           <t>l_tailcone [m]</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="13" t="n">
         <v>39.74726704646429</v>
       </c>
       <c r="J5" t="inlineStr">
@@ -625,8 +677,8 @@
           <t>EW [N]</t>
         </is>
       </c>
-      <c r="K5" s="2" t="n">
-        <v>1289768.688577064</v>
+      <c r="K5" s="13" t="n">
+        <v>1289768.688577061</v>
       </c>
     </row>
     <row r="6">
@@ -635,7 +687,7 @@
           <t>ferry_payload [kg]</t>
         </is>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="14" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
@@ -643,7 +695,7 @@
           <t>n_fuselages</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
@@ -651,7 +703,7 @@
           <t>l_nose [m]</t>
         </is>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="13" t="n">
         <v>13.2490890154881</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -659,8 +711,8 @@
           <t>ZFW [N]</t>
         </is>
       </c>
-      <c r="K6" s="2" t="n">
-        <v>2179893.163225763</v>
+      <c r="K6" s="13" t="n">
+        <v>2179893.163225761</v>
       </c>
     </row>
     <row r="7">
@@ -669,7 +721,7 @@
           <t>reserve_range [m]</t>
         </is>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="13" t="n">
         <v>185200</v>
       </c>
       <c r="D7" t="inlineStr">
@@ -677,7 +729,7 @@
           <t>depth</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="13" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" t="inlineStr">
@@ -685,7 +737,7 @@
           <t>l_cargo_straight [m]</t>
         </is>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="13" t="n">
         <v>15.31635142406773</v>
       </c>
       <c r="J7" t="inlineStr">
@@ -693,8 +745,8 @@
           <t>h_b</t>
         </is>
       </c>
-      <c r="K7" s="2" t="n">
-        <v>0.06008755531464779</v>
+      <c r="K7" s="13" t="n">
+        <v>0.06008755531464749</v>
       </c>
     </row>
     <row r="8">
@@ -703,7 +755,7 @@
           <t>ferry_crew</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="13" t="n">
         <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
@@ -711,7 +763,7 @@
           <t>jet_consumption [kg/(N·s)]</t>
         </is>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="15" t="n">
         <v>2.7e-05</v>
       </c>
       <c r="G8" t="inlineStr">
@@ -719,16 +771,16 @@
           <t>LD_g</t>
         </is>
       </c>
-      <c r="H8" s="2" t="n">
-        <v>13.08369566255592</v>
+      <c r="H8" s="13" t="n">
+        <v>13.08369566255597</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>k</t>
         </is>
       </c>
-      <c r="K8" s="2" t="n">
-        <v>1.623799771135969</v>
+      <c r="K8" s="13" t="n">
+        <v>1.623799771135971</v>
       </c>
     </row>
     <row r="9">
@@ -737,7 +789,7 @@
           <t>altitude_range_WIG [m]</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="13" t="n">
         <v>943600</v>
       </c>
       <c r="D9" t="inlineStr">
@@ -745,7 +797,7 @@
           <t>prop_consumption [kg/J]</t>
         </is>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="15" t="n">
         <v>2.1e-08</v>
       </c>
       <c r="G9" t="inlineStr">
@@ -753,7 +805,7 @@
           <t>Re</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="13" t="n">
         <v>4850602117.146465</v>
       </c>
       <c r="J9" t="inlineStr">
@@ -761,8 +813,8 @@
           <t>WP [N/W]</t>
         </is>
       </c>
-      <c r="K9" s="2" t="n">
-        <v>0.08193335381292005</v>
+      <c r="K9" s="13" t="n">
+        <v>0.08193335381292044</v>
       </c>
     </row>
     <row r="10">
@@ -771,7 +823,7 @@
           <t>altitude_range_WOG [m]</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="13" t="n">
         <v>538000</v>
       </c>
       <c r="D10" t="inlineStr">
@@ -779,7 +831,7 @@
           <t>prop_efficiency</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G10" t="inlineStr">
@@ -787,7 +839,7 @@
           <t>Cd_water</t>
         </is>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="13" t="n">
         <v>0.00126964877111443</v>
       </c>
       <c r="J10" t="inlineStr">
@@ -802,7 +854,7 @@
           <t>altitude_payload [kg]</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D11" t="inlineStr">
@@ -810,15 +862,15 @@
           <t>Cd0</t>
         </is>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02339910199117188</v>
+      <c r="E11" s="13" t="n">
+        <v>0.02339910199117171</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>hull_surface [m²]</t>
         </is>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="13" t="n">
         <v>154.2858147484878</v>
       </c>
       <c r="J11" t="inlineStr">
@@ -826,7 +878,7 @@
           <t>WS [N/m²]</t>
         </is>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="13" t="n">
         <v>3561.173893518813</v>
       </c>
     </row>
@@ -836,7 +888,7 @@
           <t>altitude_crew</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D12" t="inlineStr">
@@ -844,7 +896,7 @@
           <t>oswald_factor</t>
         </is>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G12" t="inlineStr">
@@ -852,7 +904,7 @@
           <t>take_off_power [W]</t>
         </is>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="H12" s="13" t="n">
         <v>31637380.50337056</v>
       </c>
       <c r="J12" t="inlineStr">
@@ -860,8 +912,8 @@
           <t>P [W]</t>
         </is>
       </c>
-      <c r="K12" s="2" t="n">
-        <v>32102001.52071466</v>
+      <c r="K12" s="13" t="n">
+        <v>32102001.52071445</v>
       </c>
     </row>
     <row r="13">
@@ -870,7 +922,7 @@
           <t>cruise_speed [m/s]</t>
         </is>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="13" t="n">
         <v>115.749</v>
       </c>
       <c r="D13" t="inlineStr">
@@ -878,7 +930,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="13" t="n">
         <v>6</v>
       </c>
       <c r="G13" t="inlineStr">
@@ -898,7 +950,7 @@
           <t>stall_speed_clean [m/s]</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="13" t="n">
         <v>77.16</v>
       </c>
       <c r="D14" t="inlineStr">
@@ -906,7 +958,7 @@
           <t>tfo</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="13" t="n">
         <v>0.001</v>
       </c>
       <c r="G14" t="inlineStr">
@@ -914,7 +966,7 @@
           <t>V_lof [m/s]</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="13" t="n">
         <v>64.995</v>
       </c>
       <c r="J14" t="inlineStr">
@@ -922,8 +974,8 @@
           <t>LD</t>
         </is>
       </c>
-      <c r="K14" s="2" t="n">
-        <v>21.24530202247096</v>
+      <c r="K14" s="13" t="n">
+        <v>21.24530202247108</v>
       </c>
     </row>
     <row r="15">
@@ -932,7 +984,7 @@
           <t>stall_speed_takeoff [m/s]</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="13" t="n">
         <v>61.9</v>
       </c>
       <c r="D15" t="inlineStr">
@@ -940,7 +992,7 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="14" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
@@ -948,8 +1000,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K15" s="2" t="n">
-        <v>495364.634021233</v>
+      <c r="K15" s="13" t="n">
+        <v>495364.6340212309</v>
       </c>
     </row>
     <row r="16">
@@ -958,7 +1010,7 @@
           <t>stall_speed_landing [m/s]</t>
         </is>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="13" t="n">
         <v>61.9</v>
       </c>
       <c r="D16" t="inlineStr">
@@ -966,15 +1018,15 @@
           <t>n_engines</t>
         </is>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="G16" s="1" t="inlineStr">
+      <c r="G16" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="H16" s="1" t="inlineStr">
+      <c r="H16" s="12" t="inlineStr">
         <is>
           <t>Empennage Design</t>
         </is>
@@ -984,8 +1036,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K16" s="2" t="n">
-        <v>441100.8727192185</v>
+      <c r="K16" s="13" t="n">
+        <v>445721.0545815718</v>
       </c>
     </row>
     <row r="17">
@@ -994,7 +1046,7 @@
           <t>stall_speed_high</t>
         </is>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="13" t="n">
         <v>82.3</v>
       </c>
       <c r="D17" t="inlineStr">
@@ -1002,7 +1054,7 @@
           <t>CLmax_clean</t>
         </is>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="13" t="n">
         <v>1.5</v>
       </c>
       <c r="G17" t="inlineStr">
@@ -1010,16 +1062,16 @@
           <t>S_h [m²]</t>
         </is>
       </c>
-      <c r="H17" s="2" t="n">
-        <v>224.7087640222175</v>
+      <c r="H17" s="13" t="n">
+        <v>224.7087642558615</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>9230.612754629576</v>
+      <c r="K17" s="13" t="n">
+        <v>4610.430892274482</v>
       </c>
     </row>
     <row r="18">
@@ -1028,7 +1080,7 @@
           <t>high_altitude [m]</t>
         </is>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="13" t="n">
         <v>3048</v>
       </c>
       <c r="D18" t="inlineStr">
@@ -1036,7 +1088,7 @@
           <t>CLmax_takeoff</t>
         </is>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G18" t="inlineStr">
@@ -1044,16 +1096,16 @@
           <t>S_v [m²]</t>
         </is>
       </c>
-      <c r="H18" s="2" t="n">
-        <v>125.5372961670788</v>
+      <c r="H18" s="13" t="n">
+        <v>125.5372962976079</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
-      <c r="K18" s="2" t="n">
-        <v>0.8287859230212549</v>
+      <c r="K18" s="13" t="n">
+        <v>0.8287859230212553</v>
       </c>
     </row>
     <row r="19">
@@ -1062,7 +1114,7 @@
           <t>cargo_width [m]</t>
         </is>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="13" t="n">
         <v>3.5</v>
       </c>
       <c r="D19" t="inlineStr">
@@ -1070,7 +1122,7 @@
           <t>CLmax_landing</t>
         </is>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G19" t="inlineStr">
@@ -1078,16 +1130,16 @@
           <t>l_h [m]</t>
         </is>
       </c>
-      <c r="H19" s="2" t="n">
-        <v>32.82058871597789</v>
+      <c r="H19" s="13" t="n">
+        <v>32.82058867861615</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>MTOM [kg]</t>
         </is>
       </c>
-      <c r="K19" s="2" t="n">
-        <v>268116.6818246291</v>
+      <c r="K19" s="13" t="n">
+        <v>268116.6818246287</v>
       </c>
     </row>
     <row r="20">
@@ -1096,7 +1148,7 @@
           <t>cargo_height [m]</t>
         </is>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="13" t="n">
         <v>4</v>
       </c>
       <c r="D20" t="inlineStr">
@@ -1104,7 +1156,7 @@
           <t>CL_hydro</t>
         </is>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="13" t="n">
         <v>0.5</v>
       </c>
       <c r="G20" t="inlineStr">
@@ -1112,16 +1164,16 @@
           <t>l_v [m]</t>
         </is>
       </c>
-      <c r="H20" s="2" t="n">
-        <v>32.82058871597789</v>
+      <c r="H20" s="13" t="n">
+        <v>32.82058867861615</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="K20" s="2" t="n">
-        <v>738.5836039870164</v>
+      <c r="K20" s="13" t="n">
+        <v>738.5836039870237</v>
       </c>
     </row>
     <row r="21">
@@ -1130,7 +1182,7 @@
           <t>cargo_length [m]</t>
         </is>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="13" t="n">
         <v>7.32</v>
       </c>
       <c r="D21" t="inlineStr">
@@ -1138,7 +1190,7 @@
           <t>r_float</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="13" t="n">
         <v>3</v>
       </c>
       <c r="J21" t="inlineStr">
@@ -1146,8 +1198,8 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="K21" s="2" t="n">
-        <v>66.56952473859265</v>
+      <c r="K21" s="13" t="n">
+        <v>66.56952473859297</v>
       </c>
     </row>
     <row r="22">
@@ -1156,7 +1208,7 @@
           <t>cargo_density [kg/m³]</t>
         </is>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="13" t="n">
         <v>160</v>
       </c>
       <c r="D22" t="inlineStr">
@@ -1164,15 +1216,15 @@
           <t>upsweep</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="G22" s="1" t="inlineStr">
+      <c r="G22" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="H22" s="1" t="inlineStr">
+      <c r="H22" s="12" t="inlineStr">
         <is>
           <t>CG Range</t>
         </is>
@@ -1182,8 +1234,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="K22" s="2" t="n">
-        <v>11.09492078976544</v>
+      <c r="K22" s="13" t="n">
+        <v>11.0949207897655</v>
       </c>
     </row>
     <row r="23">
@@ -1192,7 +1244,7 @@
           <t>xcg_OEW</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="E23" s="13" t="n">
         <v>0.4</v>
       </c>
       <c r="G23" t="inlineStr">
@@ -1200,25 +1252,25 @@
           <t>most_aft_cg [m]</t>
         </is>
       </c>
-      <c r="H23" s="2" t="n">
-        <v>34.7497652630114</v>
+      <c r="H23" s="13" t="n">
+        <v>34.74976530037313</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
-      <c r="K23" s="2" t="n">
-        <v>0.08023940669366764</v>
+      <c r="K23" s="13" t="n">
+        <v>0.08107985085141033</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="B24" s="1" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t>General States</t>
         </is>
@@ -1228,7 +1280,7 @@
           <t>xcg_payload</t>
         </is>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="13" t="n">
         <v>0.55</v>
       </c>
       <c r="G24" t="inlineStr">
@@ -1246,8 +1298,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K24" s="2" t="n">
-        <v>1290193.688577064</v>
+      <c r="K24" s="13" t="n">
+        <v>1290193.688577061</v>
       </c>
     </row>
     <row r="25">
@@ -1256,7 +1308,7 @@
           <t>design_id</t>
         </is>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="13" t="n">
         <v>1</v>
       </c>
       <c r="D25" t="inlineStr">
@@ -1264,7 +1316,7 @@
           <t>V_h</t>
         </is>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="G25" t="inlineStr">
@@ -1272,16 +1324,16 @@
           <t>most_forward_cg [m]</t>
         </is>
       </c>
-      <c r="H25" s="2" t="n">
-        <v>29.08041911622887</v>
+      <c r="H25" s="13" t="n">
+        <v>29.08041911616586</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K25" s="2" t="n">
-        <v>450331.4854738481</v>
+      <c r="K25" s="13" t="n">
+        <v>450331.4854738463</v>
       </c>
     </row>
     <row r="26">
@@ -1290,7 +1342,7 @@
           <t>kinematic_viscosity [m²/s]</t>
         </is>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="15" t="n">
         <v>1.006e-06</v>
       </c>
       <c r="D26" t="inlineStr">
@@ -1298,7 +1350,7 @@
           <t>V_v</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="13" t="n">
         <v>0.0838</v>
       </c>
       <c r="G26" t="inlineStr">
@@ -1316,8 +1368,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K26" s="2" t="n">
-        <v>495364.634021233</v>
+      <c r="K26" s="13" t="n">
+        <v>495364.6340212309</v>
       </c>
     </row>
     <row r="27">
@@ -1326,7 +1378,7 @@
           <t>rho_water [kg/m³]</t>
         </is>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="13" t="n">
         <v>1000</v>
       </c>
       <c r="D27" t="inlineStr">
@@ -1334,16 +1386,16 @@
           <t>k</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
-        <v>1.605242456062792</v>
+      <c r="E27" s="13" t="n">
+        <v>1.605243221150477</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K27" s="2" t="n">
-        <v>441100.8727192185</v>
+      <c r="K27" s="13" t="n">
+        <v>445721.0545815718</v>
       </c>
     </row>
     <row r="28">
@@ -1352,7 +1404,7 @@
           <t>viscosity_air [m²/s]</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="15" t="n">
         <v>1.484e-05</v>
       </c>
       <c r="J28" t="inlineStr">
@@ -1360,8 +1412,8 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K28" s="2" t="n">
-        <v>9230.612754629576</v>
+      <c r="K28" s="13" t="n">
+        <v>4610.430892274482</v>
       </c>
     </row>
     <row r="29">
@@ -1370,15 +1422,15 @@
           <t>rho_air [kg/m³]</t>
         </is>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="13" t="n">
         <v>1.225</v>
       </c>
-      <c r="D29" s="1" t="inlineStr">
+      <c r="D29" s="12" t="inlineStr">
         <is>
           <t>Design 1</t>
         </is>
       </c>
-      <c r="E29" s="1" t="inlineStr">
+      <c r="E29" s="12" t="inlineStr">
         <is>
           <t>Wing Design</t>
         </is>
@@ -1388,8 +1440,8 @@
           <t>Mff</t>
         </is>
       </c>
-      <c r="K29" s="2" t="n">
-        <v>0.8056775067428494</v>
+      <c r="K29" s="13" t="n">
+        <v>0.8056775116690675</v>
       </c>
     </row>
     <row r="30">
@@ -1398,7 +1450,7 @@
           <t>taper_ratio</t>
         </is>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="E30" s="13" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -1408,7 +1460,7 @@
           <t>sweep_c_4 [deg]</t>
         </is>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1418,7 +1470,7 @@
           <t>dihedral [deg]</t>
         </is>
       </c>
-      <c r="E32" s="2" t="n">
+      <c r="E32" s="13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1428,7 +1480,7 @@
           <t>sweep_x_c [deg]</t>
         </is>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="13" t="n">
         <v>4.085616779974877</v>
       </c>
     </row>
@@ -1438,8 +1490,8 @@
           <t>chord_root [m]</t>
         </is>
       </c>
-      <c r="E34" s="2" t="n">
-        <v>15.84988684272195</v>
+      <c r="E34" s="13" t="n">
+        <v>15.84988684220103</v>
       </c>
     </row>
     <row r="35">
@@ -1448,8 +1500,8 @@
           <t>chord_tip [m]</t>
         </is>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>6.339954737088782</v>
+      <c r="E35" s="13" t="n">
+        <v>6.339954736880411</v>
       </c>
     </row>
     <row r="36">
@@ -1458,8 +1510,8 @@
           <t>y_MAC [m]</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>14.26489815844976</v>
+      <c r="E36" s="13" t="n">
+        <v>14.26489815798092</v>
       </c>
     </row>
     <row r="37">
@@ -1468,7 +1520,7 @@
           <t>X_LEMAC [m]</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="13" t="n">
         <v>21.05644</v>
       </c>
     </row>
@@ -1478,8 +1530,8 @@
           <t>X_LE [m]</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>20.03751870296788</v>
+      <c r="E38" s="13" t="n">
+        <v>20.03751870300136</v>
       </c>
     </row>
     <row r="39">
@@ -1488,8 +1540,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>11.77420165459345</v>
+      <c r="E39" s="13" t="n">
+        <v>11.77420165420648</v>
       </c>
     </row>
     <row r="40">
@@ -1498,8 +1550,8 @@
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>738.5836040056462</v>
+      <c r="E40" s="13" t="n">
+        <v>738.583603957097</v>
       </c>
     </row>
     <row r="41">
@@ -1508,8 +1560,8 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>66.56952473943221</v>
+      <c r="E41" s="13" t="n">
+        <v>66.56952473724431</v>
       </c>
     </row>
     <row r="42">
@@ -1518,7 +1570,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="13" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1555,42 +1607,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>Requirements</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Inputs</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>General Outputs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="12" t="inlineStr">
         <is>
           <t>Design Mission</t>
         </is>
@@ -1602,7 +1654,7 @@
           <t>design_range [m]</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="13" t="n">
         <v>3704000</v>
       </c>
       <c r="D2" t="inlineStr">
@@ -1610,7 +1662,7 @@
           <t>cruise_altitude [m]</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="13" t="n">
         <v>8</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -1618,7 +1670,7 @@
           <t>d_fuselage [m]</t>
         </is>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="13" t="n">
         <v>6.204804790550249</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -1626,8 +1678,8 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K2" s="2" t="n">
-        <v>2585106.105313952</v>
+      <c r="K2" s="13" t="n">
+        <v>2585106.105315377</v>
       </c>
     </row>
     <row r="3">
@@ -1636,7 +1688,7 @@
           <t>design_payload [kg]</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D3" t="inlineStr">
@@ -1654,7 +1706,7 @@
           <t>r_fuselage [m]</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="13" t="n">
         <v>3.102402395275125</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -1662,8 +1714,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K3" s="2" t="n">
-        <v>421191.8166952552</v>
+      <c r="K3" s="13" t="n">
+        <v>421191.8166961765</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1724,7 @@
           <t>design_crew</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D4" t="inlineStr">
@@ -1690,7 +1742,7 @@
           <t>l_fuselage [m]</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="13" t="n">
         <v>52.74084071967712</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -1698,8 +1750,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K4" s="2" t="n">
-        <v>1274259.932513383</v>
+      <c r="K4" s="13" t="n">
+        <v>1274259.932513885</v>
       </c>
     </row>
     <row r="5">
@@ -1708,7 +1760,7 @@
           <t>ferry_range [m]</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="13" t="n">
         <v>12038000</v>
       </c>
       <c r="D5" t="inlineStr">
@@ -1716,7 +1768,7 @@
           <t>n_wings</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
@@ -1724,7 +1776,7 @@
           <t>l_tailcone [m]</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="13" t="n">
         <v>27.92162155747612</v>
       </c>
       <c r="J5" t="inlineStr">
@@ -1732,8 +1784,8 @@
           <t>EW [N]</t>
         </is>
       </c>
-      <c r="K5" s="2" t="n">
-        <v>1273834.932513383</v>
+      <c r="K5" s="13" t="n">
+        <v>1273834.932513885</v>
       </c>
     </row>
     <row r="6">
@@ -1742,7 +1794,7 @@
           <t>reserve_range [m]</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="13" t="n">
         <v>185200</v>
       </c>
       <c r="D6" t="inlineStr">
@@ -1750,7 +1802,7 @@
           <t>n_fuselages</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="13" t="n">
         <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
@@ -1758,7 +1810,7 @@
           <t>l_nose [m]</t>
         </is>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="13" t="n">
         <v>9.307207185825375</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -1766,8 +1818,8 @@
           <t>ZFW [N]</t>
         </is>
       </c>
-      <c r="K6" s="2" t="n">
-        <v>2163914.288618697</v>
+      <c r="K6" s="13" t="n">
+        <v>2163914.288619201</v>
       </c>
     </row>
     <row r="7">
@@ -1776,7 +1828,7 @@
           <t>ferry_payload [kg]</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="14" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
@@ -1784,7 +1836,7 @@
           <t>depth</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="13" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" t="inlineStr">
@@ -1792,7 +1844,7 @@
           <t>l_cargo_straight [m]</t>
         </is>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="13" t="n">
         <v>8.74654837462985</v>
       </c>
       <c r="J7" t="inlineStr">
@@ -1800,8 +1852,8 @@
           <t>h_b</t>
         </is>
       </c>
-      <c r="K7" s="2" t="n">
-        <v>0.09387803518272897</v>
+      <c r="K7" s="13" t="n">
+        <v>0.09387803518307419</v>
       </c>
     </row>
     <row r="8">
@@ -1810,7 +1862,7 @@
           <t>ferry_crew</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="13" t="n">
         <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
@@ -1818,7 +1870,7 @@
           <t>jet_consumption [kg/(N·s)]</t>
         </is>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="15" t="n">
         <v>2.7e-05</v>
       </c>
       <c r="G8" t="inlineStr">
@@ -1826,7 +1878,7 @@
           <t>Re</t>
         </is>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="13" t="n">
         <v>3407446264.985502</v>
       </c>
       <c r="J8" t="inlineStr">
@@ -1834,8 +1886,8 @@
           <t>k</t>
         </is>
       </c>
-      <c r="K8" s="2" t="n">
-        <v>1.422374919554507</v>
+      <c r="K8" s="13" t="n">
+        <v>1.422374919553053</v>
       </c>
     </row>
     <row r="9">
@@ -1844,7 +1896,7 @@
           <t>altitude_range_WIG [m]</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="13" t="n">
         <v>943600</v>
       </c>
       <c r="D9" t="inlineStr">
@@ -1852,7 +1904,7 @@
           <t>prop_consumption [kg/J]</t>
         </is>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="15" t="n">
         <v>2.1e-08</v>
       </c>
       <c r="G9" t="inlineStr">
@@ -1860,7 +1912,7 @@
           <t>Cd_water</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="13" t="n">
         <v>0.001321877371153106</v>
       </c>
       <c r="J9" t="inlineStr">
@@ -1868,8 +1920,8 @@
           <t>WP [N/W]</t>
         </is>
       </c>
-      <c r="K9" s="2" t="n">
-        <v>0.09647518482443268</v>
+      <c r="K9" s="13" t="n">
+        <v>0.09647518482399101</v>
       </c>
     </row>
     <row r="10">
@@ -1878,7 +1930,7 @@
           <t>altitude_range_WOG [m]</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="13" t="n">
         <v>538000</v>
       </c>
       <c r="D10" t="inlineStr">
@@ -1886,7 +1938,7 @@
           <t>prop_efficiency</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G10" t="inlineStr">
@@ -1894,7 +1946,7 @@
           <t>hull_surface [m²]</t>
         </is>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="13" t="n">
         <v>224.1641870825653</v>
       </c>
       <c r="J10" t="inlineStr">
@@ -1909,7 +1961,7 @@
           <t>altitude_payload [kg]</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D11" t="inlineStr">
@@ -1917,15 +1969,15 @@
           <t>Cd0</t>
         </is>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02344655710840882</v>
+      <c r="E11" s="13" t="n">
+        <v>0.02344655710855558</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>take_off_power [W]</t>
         </is>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="13" t="n">
         <v>47857314.10082371</v>
       </c>
       <c r="J11" t="inlineStr">
@@ -1933,7 +1985,7 @@
           <t>WS [N/m²]</t>
         </is>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="13" t="n">
         <v>3559.80642288087</v>
       </c>
     </row>
@@ -1943,7 +1995,7 @@
           <t>altitude_crew</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D12" t="inlineStr">
@@ -1951,7 +2003,7 @@
           <t>oswald_factor</t>
         </is>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G12" t="inlineStr">
@@ -1964,8 +2016,8 @@
           <t>P [W]</t>
         </is>
       </c>
-      <c r="K12" s="2" t="n">
-        <v>26795554.83639006</v>
+      <c r="K12" s="13" t="n">
+        <v>26795554.83652751</v>
       </c>
     </row>
     <row r="13">
@@ -1974,7 +2026,7 @@
           <t>cruise_speed [m/s]</t>
         </is>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="13" t="n">
         <v>115.749</v>
       </c>
       <c r="D13" t="inlineStr">
@@ -1982,7 +2034,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="13" t="n">
         <v>10</v>
       </c>
       <c r="G13" t="inlineStr">
@@ -1990,7 +2042,7 @@
           <t>V_lof [m/s]</t>
         </is>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="13" t="n">
         <v>64.995</v>
       </c>
       <c r="J13" t="inlineStr">
@@ -2005,7 +2057,7 @@
           <t>stall_speed_clean [m/s]</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="13" t="n">
         <v>77.16</v>
       </c>
       <c r="D14" t="inlineStr">
@@ -2013,7 +2065,7 @@
           <t>tfo</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="13" t="n">
         <v>0.001</v>
       </c>
       <c r="G14" t="inlineStr">
@@ -2021,16 +2073,16 @@
           <t>LD_g</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
-        <v>16.87387639850711</v>
+      <c r="H14" s="13" t="n">
+        <v>16.8738763984543</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>LD</t>
         </is>
       </c>
-      <c r="K14" s="2" t="n">
-        <v>24.00097858489925</v>
+      <c r="K14" s="13" t="n">
+        <v>24.00097858479959</v>
       </c>
     </row>
     <row r="15">
@@ -2039,7 +2091,7 @@
           <t>stall_speed_takeoff [m/s]</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="13" t="n">
         <v>61.9</v>
       </c>
       <c r="D15" t="inlineStr">
@@ -2047,7 +2099,7 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="14" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
@@ -2055,8 +2107,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K15" s="2" t="n">
-        <v>463310.9983647808</v>
+      <c r="K15" s="13" t="n">
+        <v>463310.9983657943</v>
       </c>
     </row>
     <row r="16">
@@ -2065,7 +2117,7 @@
           <t>stall_speed_landing [m/s]</t>
         </is>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="13" t="n">
         <v>61.9</v>
       </c>
       <c r="D16" t="inlineStr">
@@ -2073,15 +2125,15 @@
           <t>n_engines</t>
         </is>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="G16" s="1" t="inlineStr">
+      <c r="G16" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="H16" s="1" t="inlineStr">
+      <c r="H16" s="12" t="inlineStr">
         <is>
           <t>Empennage Design</t>
         </is>
@@ -2091,8 +2143,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K16" s="2" t="n">
-        <v>413082.8798527136</v>
+      <c r="K16" s="13" t="n">
+        <v>417141.1395492081</v>
       </c>
     </row>
     <row r="17">
@@ -2101,7 +2153,7 @@
           <t>stall_speed_high</t>
         </is>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="13" t="n">
         <v>82.3</v>
       </c>
       <c r="D17" t="inlineStr">
@@ -2109,7 +2161,7 @@
           <t>CLmax_clean</t>
         </is>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="13" t="n">
         <v>1.5</v>
       </c>
       <c r="G17" t="inlineStr">
@@ -2117,16 +2169,16 @@
           <t>S_h [m²]</t>
         </is>
       </c>
-      <c r="H17" s="2" t="n">
-        <v>244.7440899719453</v>
+      <c r="H17" s="13" t="n">
+        <v>243.0584944865134</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>8108.936842541618</v>
+      <c r="K17" s="13" t="n">
+        <v>4050.677146968432</v>
       </c>
     </row>
     <row r="18">
@@ -2135,7 +2187,7 @@
           <t>high_altitude [m]</t>
         </is>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="13" t="n">
         <v>3048</v>
       </c>
       <c r="D18" t="inlineStr">
@@ -2143,7 +2195,7 @@
           <t>CLmax_takeoff</t>
         </is>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G18" t="inlineStr">
@@ -2151,16 +2203,16 @@
           <t>S_v [m²]</t>
         </is>
       </c>
-      <c r="H18" s="2" t="n">
-        <v>227.8839415516557</v>
+      <c r="H18" s="13" t="n">
+        <v>226.3144648663313</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
-      <c r="K18" s="2" t="n">
-        <v>0.8370698147246444</v>
+      <c r="K18" s="13" t="n">
+        <v>0.8370698147243778</v>
       </c>
     </row>
     <row r="19">
@@ -2169,7 +2221,7 @@
           <t>cargo_width [m]</t>
         </is>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="13" t="n">
         <v>3.5</v>
       </c>
       <c r="D19" t="inlineStr">
@@ -2177,7 +2229,7 @@
           <t>CLmax_landing</t>
         </is>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G19" t="inlineStr">
@@ -2185,16 +2237,16 @@
           <t>l_h [m]</t>
         </is>
       </c>
-      <c r="H19" s="2" t="n">
-        <v>22.91452403750576</v>
+      <c r="H19" s="13" t="n">
+        <v>22.91446344560504</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>MTOM [kg]</t>
         </is>
       </c>
-      <c r="K19" s="2" t="n">
-        <v>263517.4419280277</v>
+      <c r="K19" s="13" t="n">
+        <v>263517.441928173</v>
       </c>
     </row>
     <row r="20">
@@ -2203,7 +2255,7 @@
           <t>cargo_height [m]</t>
         </is>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="13" t="n">
         <v>4</v>
       </c>
       <c r="D20" t="inlineStr">
@@ -2211,7 +2263,7 @@
           <t>CL_hydro</t>
         </is>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="13" t="n">
         <v>0.5</v>
       </c>
       <c r="G20" t="inlineStr">
@@ -2219,16 +2271,16 @@
           <t>l_v [m]</t>
         </is>
       </c>
-      <c r="H20" s="2" t="n">
-        <v>22.91452403750576</v>
+      <c r="H20" s="13" t="n">
+        <v>22.91446344560504</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="K20" s="2" t="n">
-        <v>726.1928875453634</v>
+      <c r="K20" s="13" t="n">
+        <v>726.1928875400224</v>
       </c>
     </row>
     <row r="21">
@@ -2237,7 +2289,7 @@
           <t>cargo_length [m]</t>
         </is>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="13" t="n">
         <v>7.32</v>
       </c>
       <c r="D21" t="inlineStr">
@@ -2245,7 +2297,7 @@
           <t>r_float</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="13" t="n">
         <v>3.102402395275125</v>
       </c>
       <c r="J21" t="inlineStr">
@@ -2253,8 +2305,8 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="K21" s="2" t="n">
-        <v>85.21695180803896</v>
+      <c r="K21" s="13" t="n">
+        <v>85.21695180772558</v>
       </c>
     </row>
     <row r="22">
@@ -2263,7 +2315,7 @@
           <t>cargo_density [kg/m³]</t>
         </is>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="13" t="n">
         <v>160</v>
       </c>
       <c r="D22" t="inlineStr">
@@ -2271,15 +2323,15 @@
           <t>upsweep</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="G22" s="1" t="inlineStr">
+      <c r="G22" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="H22" s="1" t="inlineStr">
+      <c r="H22" s="12" t="inlineStr">
         <is>
           <t>CG Range</t>
         </is>
@@ -2289,8 +2341,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="K22" s="2" t="n">
-        <v>8.521695180803896</v>
+      <c r="K22" s="13" t="n">
+        <v>8.521695180772559</v>
       </c>
     </row>
     <row r="23">
@@ -2299,7 +2351,7 @@
           <t>xcg_OEW</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="E23" s="13" t="n">
         <v>0.4</v>
       </c>
       <c r="G23" t="inlineStr">
@@ -2307,25 +2359,25 @@
           <t>most_aft_cg [m]</t>
         </is>
       </c>
-      <c r="H23" s="2" t="n">
-        <v>24.55223261020365</v>
+      <c r="H23" s="13" t="n">
+        <v>24.55229320210437</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
-      <c r="K23" s="2" t="n">
-        <v>0.07514273320377675</v>
+      <c r="K23" s="13" t="n">
+        <v>0.07588095969661533</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="B24" s="1" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t>General States</t>
         </is>
@@ -2335,7 +2387,7 @@
           <t>xcg_payload</t>
         </is>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="13" t="n">
         <v>0.55</v>
       </c>
       <c r="G24" t="inlineStr">
@@ -2353,8 +2405,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K24" s="2" t="n">
-        <v>1274259.932513383</v>
+      <c r="K24" s="13" t="n">
+        <v>1274259.932513885</v>
       </c>
     </row>
     <row r="25">
@@ -2363,7 +2415,7 @@
           <t>design_id</t>
         </is>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D25" t="inlineStr">
@@ -2371,7 +2423,7 @@
           <t>V_h</t>
         </is>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="G25" t="inlineStr">
@@ -2379,7 +2431,7 @@
           <t>most_forward_cg [m]</t>
         </is>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="H25" s="13" t="n">
         <v>21.09633628787085</v>
       </c>
       <c r="J25" t="inlineStr">
@@ -2387,8 +2439,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K25" s="2" t="n">
-        <v>421191.8166952552</v>
+      <c r="K25" s="13" t="n">
+        <v>421191.8166961765</v>
       </c>
     </row>
     <row r="26">
@@ -2397,7 +2449,7 @@
           <t>kinematic_viscosity [m²/s]</t>
         </is>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="15" t="n">
         <v>1.006e-06</v>
       </c>
       <c r="D26" t="inlineStr">
@@ -2405,7 +2457,7 @@
           <t>V_v</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="13" t="n">
         <v>0.0838</v>
       </c>
       <c r="G26" t="inlineStr">
@@ -2423,8 +2475,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K26" s="2" t="n">
-        <v>463310.9983647808</v>
+      <c r="K26" s="13" t="n">
+        <v>463310.9983657943</v>
       </c>
     </row>
     <row r="27">
@@ -2433,7 +2485,7 @@
           <t>rho_water [kg/m³]</t>
         </is>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="13" t="n">
         <v>1000</v>
       </c>
       <c r="D27" t="inlineStr">
@@ -2441,7 +2493,7 @@
           <t>k</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E27" s="13" t="n">
         <v>1.226101000048545</v>
       </c>
       <c r="J27" t="inlineStr">
@@ -2449,8 +2501,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K27" s="2" t="n">
-        <v>413082.8798527136</v>
+      <c r="K27" s="13" t="n">
+        <v>417141.1395492081</v>
       </c>
     </row>
     <row r="28">
@@ -2459,7 +2511,7 @@
           <t>viscosity_air [m²/s]</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="15" t="n">
         <v>1.48e-05</v>
       </c>
       <c r="J28" t="inlineStr">
@@ -2467,8 +2519,8 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K28" s="2" t="n">
-        <v>8108.936842541618</v>
+      <c r="K28" s="13" t="n">
+        <v>4050.677146968432</v>
       </c>
     </row>
     <row r="29">
@@ -2477,15 +2529,15 @@
           <t>rho_air [kg/m³]</t>
         </is>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="13" t="n">
         <v>1.225</v>
       </c>
-      <c r="D29" s="1" t="inlineStr">
+      <c r="D29" s="12" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="E29" s="1" t="inlineStr">
+      <c r="E29" s="12" t="inlineStr">
         <is>
           <t>Wing Design</t>
         </is>
@@ -2495,8 +2547,8 @@
           <t>Mff</t>
         </is>
       </c>
-      <c r="K29" s="2" t="n">
-        <v>0.823842794974096</v>
+      <c r="K29" s="13" t="n">
+        <v>0.8238427162961426</v>
       </c>
     </row>
     <row r="30">
@@ -2505,7 +2557,7 @@
           <t>taper_ratio</t>
         </is>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="E30" s="13" t="n">
         <v>0.4</v>
       </c>
       <c r="J30" t="inlineStr">
@@ -2513,7 +2565,7 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="K30" s="13" t="n">
         <v>1720912.57500321</v>
       </c>
     </row>
@@ -2523,7 +2575,7 @@
           <t>sweep_c_4 [deg]</t>
         </is>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2533,7 +2585,7 @@
           <t>dihedral [deg]</t>
         </is>
       </c>
-      <c r="E32" s="2" t="n">
+      <c r="E32" s="13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2543,7 +2595,7 @@
           <t>sweep_x_c [deg]</t>
         </is>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="13" t="n">
         <v>2.454031674527076</v>
       </c>
     </row>
@@ -2553,8 +2605,8 @@
           <t>chord_root [m]</t>
         </is>
       </c>
-      <c r="E34" s="2" t="n">
-        <v>12.20193783978984</v>
+      <c r="E34" s="13" t="n">
+        <v>12.17385025824651</v>
       </c>
     </row>
     <row r="35">
@@ -2563,8 +2615,8 @@
           <t>chord_tip [m]</t>
         </is>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>4.880775135915937</v>
+      <c r="E35" s="13" t="n">
+        <v>4.869540103298605</v>
       </c>
     </row>
     <row r="36">
@@ -2573,8 +2625,8 @@
           <t>y_MAC [m]</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>18.30290675968476</v>
+      <c r="E36" s="13" t="n">
+        <v>18.26077538736977</v>
       </c>
     </row>
     <row r="37">
@@ -2583,7 +2635,7 @@
           <t>X_LEMAC [m]</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="13" t="n">
         <v>21.05644</v>
       </c>
     </row>
@@ -2593,8 +2645,8 @@
           <t>X_LE [m]</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>20.27202971029923</v>
+      <c r="E38" s="13" t="n">
+        <v>20.2738353405413</v>
       </c>
     </row>
     <row r="39">
@@ -2603,8 +2655,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>9.06429668098674</v>
+      <c r="E39" s="13" t="n">
+        <v>9.043431620411695</v>
       </c>
     </row>
     <row r="40">
@@ -2613,8 +2665,8 @@
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>729.5477065258664</v>
+      <c r="E40" s="13" t="n">
+        <v>726.1928875400224</v>
       </c>
     </row>
     <row r="41">
@@ -2623,8 +2675,8 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>85.41356487852889</v>
+      <c r="E41" s="13" t="n">
+        <v>85.21695180772558</v>
       </c>
     </row>
     <row r="42">
@@ -2633,7 +2685,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="13" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2660,7 +2712,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -2670,42 +2722,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>Requirements</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Inputs</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>General Outputs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="12" t="inlineStr">
         <is>
           <t>Design Mission</t>
         </is>
@@ -2717,7 +2769,7 @@
           <t>design_range [m]</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="13" t="n">
         <v>3704000</v>
       </c>
       <c r="D2" t="inlineStr">
@@ -2725,7 +2777,7 @@
           <t>cruise_altitude [m]</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="13" t="n">
         <v>10</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -2733,7 +2785,7 @@
           <t>d_fuselage [m]</t>
         </is>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="13" t="n">
         <v>8.832726010325398</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -2741,8 +2793,8 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K2" s="2" t="n">
-        <v>2605660.308783418</v>
+      <c r="K2" s="13" t="n">
+        <v>2605660.308785691</v>
       </c>
     </row>
     <row r="3">
@@ -2751,7 +2803,7 @@
           <t>design_payload [kg]</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D3" t="inlineStr">
@@ -2769,7 +2821,7 @@
           <t>r_fuselage [m]</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="13" t="n">
         <v>4.416363005162699</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -2777,8 +2829,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K3" s="2" t="n">
-        <v>434466.6841037282</v>
+      <c r="K3" s="13" t="n">
+        <v>434466.6841051969</v>
       </c>
     </row>
     <row r="4">
@@ -2787,7 +2839,7 @@
           <t>design_crew</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D4" t="inlineStr">
@@ -2805,7 +2857,7 @@
           <t>l_fuselage [m]</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="13" t="n">
         <v>75.07817108776588</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -2813,8 +2865,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K4" s="2" t="n">
-        <v>1281518.714370907</v>
+      <c r="K4" s="13" t="n">
+        <v>1281518.714371709</v>
       </c>
     </row>
     <row r="5">
@@ -2823,7 +2875,7 @@
           <t>ferry_range [m]</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="13" t="n">
         <v>12038000</v>
       </c>
       <c r="D5" t="inlineStr">
@@ -2831,7 +2883,7 @@
           <t>n_wings</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
@@ -2839,7 +2891,7 @@
           <t>l_tailcone [m]</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="13" t="n">
         <v>39.74726704646429</v>
       </c>
       <c r="J5" t="inlineStr">
@@ -2847,8 +2899,8 @@
           <t>EW [N]</t>
         </is>
       </c>
-      <c r="K5" s="2" t="n">
-        <v>1281093.714370907</v>
+      <c r="K5" s="13" t="n">
+        <v>1281093.714371709</v>
       </c>
     </row>
     <row r="6">
@@ -2857,7 +2909,7 @@
           <t>reserve_range [m]</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="13" t="n">
         <v>185200</v>
       </c>
       <c r="D6" t="inlineStr">
@@ -2865,7 +2917,7 @@
           <t>n_fuselages</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
@@ -2873,7 +2925,7 @@
           <t>l_nose [m]</t>
         </is>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="13" t="n">
         <v>13.2490890154881</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -2881,8 +2933,8 @@
           <t>ZFW [N]</t>
         </is>
       </c>
-      <c r="K6" s="2" t="n">
-        <v>2171193.62467969</v>
+      <c r="K6" s="13" t="n">
+        <v>2171193.624680494</v>
       </c>
     </row>
     <row r="7">
@@ -2891,7 +2943,7 @@
           <t>ferry_payload [kg]</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="14" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
@@ -2899,7 +2951,7 @@
           <t>depth</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="13" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" t="inlineStr">
@@ -2907,7 +2959,7 @@
           <t>l_cargo_straight [m]</t>
         </is>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="13" t="n">
         <v>15.31635142406773</v>
       </c>
       <c r="J7" t="inlineStr">
@@ -2915,8 +2967,8 @@
           <t>h_b</t>
         </is>
       </c>
-      <c r="K7" s="2" t="n">
-        <v>0.1165515941021191</v>
+      <c r="K7" s="13" t="n">
+        <v>0.1165515941027839</v>
       </c>
     </row>
     <row r="8">
@@ -2925,7 +2977,7 @@
           <t>ferry_crew</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="13" t="n">
         <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
@@ -2933,7 +2985,7 @@
           <t>jet_consumption [kg/(N·s)]</t>
         </is>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="15" t="n">
         <v>2.7e-05</v>
       </c>
       <c r="G8" t="inlineStr">
@@ -2941,7 +2993,7 @@
           <t>Re</t>
         </is>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="13" t="n">
         <v>4837280592.753655</v>
       </c>
       <c r="J8" t="inlineStr">
@@ -2949,8 +3001,8 @@
           <t>k</t>
         </is>
       </c>
-      <c r="K8" s="2" t="n">
-        <v>1.34234114146773</v>
+      <c r="K8" s="13" t="n">
+        <v>1.342341141465762</v>
       </c>
     </row>
     <row r="9">
@@ -2959,7 +3011,7 @@
           <t>altitude_range_WIG [m]</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="13" t="n">
         <v>943600</v>
       </c>
       <c r="D9" t="inlineStr">
@@ -2967,7 +3019,7 @@
           <t>prop_consumption [kg/J]</t>
         </is>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="15" t="n">
         <v>2.1e-08</v>
       </c>
       <c r="G9" t="inlineStr">
@@ -2975,7 +3027,7 @@
           <t>Cd</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="13" t="n">
         <v>0.001270043469758956</v>
       </c>
       <c r="J9" t="inlineStr">
@@ -2983,8 +3035,8 @@
           <t>WP [N/W]</t>
         </is>
       </c>
-      <c r="K9" s="2" t="n">
-        <v>0.09623828153247972</v>
+      <c r="K9" s="13" t="n">
+        <v>0.09623828153181459</v>
       </c>
     </row>
     <row r="10">
@@ -2993,7 +3045,7 @@
           <t>altitude_range_WOG [m]</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="13" t="n">
         <v>538000</v>
       </c>
       <c r="D10" t="inlineStr">
@@ -3001,7 +3053,7 @@
           <t>prop_efficiency</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G10" t="inlineStr">
@@ -3009,7 +3061,7 @@
           <t>hull_surface [m²]</t>
         </is>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="13" t="n">
         <v>227.1273881588691</v>
       </c>
       <c r="J10" t="inlineStr">
@@ -3024,7 +3076,7 @@
           <t>altitude_payload [kg]</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D11" t="inlineStr">
@@ -3032,15 +3084,15 @@
           <t>Cd0</t>
         </is>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02344053599430469</v>
+      <c r="E11" s="13" t="n">
+        <v>0.02344053599452553</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>take_off_power [W]</t>
         </is>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="13" t="n">
         <v>46205736.73514064</v>
       </c>
       <c r="J11" t="inlineStr">
@@ -3048,7 +3100,7 @@
           <t>WS [N/m²]</t>
         </is>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="13" t="n">
         <v>3539.60038145072</v>
       </c>
     </row>
@@ -3058,7 +3110,7 @@
           <t>altitude_crew</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D12" t="inlineStr">
@@ -3066,7 +3118,7 @@
           <t>oswald_factor</t>
         </is>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G12" t="inlineStr">
@@ -3079,8 +3131,8 @@
           <t>P [W]</t>
         </is>
       </c>
-      <c r="K12" s="2" t="n">
-        <v>27075091.81680501</v>
+      <c r="K12" s="13" t="n">
+        <v>27075091.81701575</v>
       </c>
     </row>
     <row r="13">
@@ -3089,7 +3141,7 @@
           <t>cruise_speed [m/s]</t>
         </is>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="13" t="n">
         <v>115.749</v>
       </c>
       <c r="D13" t="inlineStr">
@@ -3097,7 +3149,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="13" t="n">
         <v>10</v>
       </c>
       <c r="G13" t="inlineStr">
@@ -3105,7 +3157,7 @@
           <t>V_lof [m/s]</t>
         </is>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="13" t="n">
         <v>64.8165</v>
       </c>
       <c r="J13" t="inlineStr">
@@ -3120,7 +3172,7 @@
           <t>stall_speed_clean [m/s]</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="13" t="n">
         <v>77.16</v>
       </c>
       <c r="D14" t="inlineStr">
@@ -3128,7 +3180,7 @@
           <t>tfo</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="13" t="n">
         <v>0.001</v>
       </c>
       <c r="G14" t="inlineStr">
@@ -3136,16 +3188,16 @@
           <t>LD_g</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
-        <v>16.87604343537927</v>
+      <c r="H14" s="13" t="n">
+        <v>16.87604343529977</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>LD</t>
         </is>
       </c>
-      <c r="K14" s="2" t="n">
-        <v>22.65340740850599</v>
+      <c r="K14" s="13" t="n">
+        <v>22.65340740836607</v>
       </c>
     </row>
     <row r="15">
@@ -3154,7 +3206,7 @@
           <t>stall_speed_takeoff [m/s]</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="13" t="n">
         <v>61.73</v>
       </c>
       <c r="D15" t="inlineStr">
@@ -3162,7 +3214,7 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="inlineStr">
@@ -3170,7 +3222,7 @@
           <t>Cd_water</t>
         </is>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="13" t="n">
         <v>0.001270043469758956</v>
       </c>
       <c r="J15" t="inlineStr">
@@ -3178,8 +3230,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K15" s="2" t="n">
-        <v>477913.352514101</v>
+      <c r="K15" s="13" t="n">
+        <v>477913.3525157166</v>
       </c>
     </row>
     <row r="16">
@@ -3188,7 +3240,7 @@
           <t>stall_speed_landing [m/s]</t>
         </is>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="13" t="n">
         <v>61.73</v>
       </c>
       <c r="D16" t="inlineStr">
@@ -3196,7 +3248,7 @@
           <t>n_engines</t>
         </is>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="13" t="n">
         <v>8</v>
       </c>
       <c r="J16" t="inlineStr">
@@ -3204,8 +3256,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K16" s="2" t="n">
-        <v>425845.5147107402</v>
+      <c r="K16" s="13" t="n">
+        <v>430160.3699494032</v>
       </c>
     </row>
     <row r="17">
@@ -3214,7 +3266,7 @@
           <t>stall_speed_high</t>
         </is>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="13" t="n">
         <v>82.3</v>
       </c>
       <c r="D17" t="inlineStr">
@@ -3222,15 +3274,15 @@
           <t>CLmax_clean</t>
         </is>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="13" t="n">
         <v>1.5</v>
       </c>
-      <c r="G17" s="1" t="inlineStr">
+      <c r="G17" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="H17" s="1" t="inlineStr">
+      <c r="H17" s="12" t="inlineStr">
         <is>
           <t>Empennage Design</t>
         </is>
@@ -3240,8 +3292,8 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>8621.169392987969</v>
+      <c r="K17" s="13" t="n">
+        <v>4306.314155793691</v>
       </c>
     </row>
     <row r="18">
@@ -3250,7 +3302,7 @@
           <t>high_altitude [m]</t>
         </is>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="13" t="n">
         <v>3048</v>
       </c>
       <c r="D18" t="inlineStr">
@@ -3258,7 +3310,7 @@
           <t>CLmax_takeoff</t>
         </is>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G18" t="inlineStr">
@@ -3266,16 +3318,16 @@
           <t>S_h [m²]</t>
         </is>
       </c>
-      <c r="H18" s="2" t="n">
-        <v>186.9548079677261</v>
+      <c r="H18" s="13" t="n">
+        <v>185.6057148332545</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
-      <c r="K18" s="2" t="n">
-        <v>0.8332604282149961</v>
+      <c r="K18" s="13" t="n">
+        <v>0.8332604282145779</v>
       </c>
     </row>
     <row r="19">
@@ -3284,7 +3336,7 @@
           <t>cargo_width [m]</t>
         </is>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="13" t="n">
         <v>3.5</v>
       </c>
       <c r="D19" t="inlineStr">
@@ -3292,7 +3344,7 @@
           <t>CLmax_landing</t>
         </is>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G19" t="inlineStr">
@@ -3300,16 +3352,16 @@
           <t>S_v [m²]</t>
         </is>
       </c>
-      <c r="H19" s="2" t="n">
-        <v>174.0756989743939</v>
+      <c r="H19" s="13" t="n">
+        <v>172.8195433669636</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>MTOM [kg]</t>
         </is>
       </c>
-      <c r="K19" s="2" t="n">
-        <v>265612.6716394922</v>
+      <c r="K19" s="13" t="n">
+        <v>265612.6716397239</v>
       </c>
     </row>
     <row r="20">
@@ -3318,7 +3370,7 @@
           <t>cargo_height [m]</t>
         </is>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="13" t="n">
         <v>4</v>
       </c>
       <c r="D20" t="inlineStr">
@@ -3326,7 +3378,7 @@
           <t>CL_hydro</t>
         </is>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="13" t="n">
         <v>0.5</v>
       </c>
       <c r="G20" t="inlineStr">
@@ -3334,16 +3386,16 @@
           <t>l_h [m]</t>
         </is>
       </c>
-      <c r="H20" s="2" t="n">
-        <v>30.62931767049474</v>
+      <c r="H20" s="13" t="n">
+        <v>30.62643959261036</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="K20" s="2" t="n">
-        <v>736.1453350695695</v>
+      <c r="K20" s="13" t="n">
+        <v>736.1453350611716</v>
       </c>
     </row>
     <row r="21">
@@ -3352,7 +3404,7 @@
           <t>cargo_length [m]</t>
         </is>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="13" t="n">
         <v>7.32</v>
       </c>
       <c r="D21" t="inlineStr">
@@ -3360,7 +3412,7 @@
           <t>r_float</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="13" t="n">
         <v>4.416363005162699</v>
       </c>
       <c r="G21" t="inlineStr">
@@ -3368,16 +3420,16 @@
           <t>l_v [m]</t>
         </is>
       </c>
-      <c r="H21" s="2" t="n">
-        <v>30.62931767049474</v>
+      <c r="H21" s="13" t="n">
+        <v>30.62643959261036</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
           <t>b [m]</t>
         </is>
       </c>
-      <c r="K21" s="2" t="n">
-        <v>85.79891229319691</v>
+      <c r="K21" s="13" t="n">
+        <v>85.79891229270751</v>
       </c>
     </row>
     <row r="22">
@@ -3386,7 +3438,7 @@
           <t>cargo_density [kg/m³]</t>
         </is>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="13" t="n">
         <v>160</v>
       </c>
       <c r="D22" t="inlineStr">
@@ -3394,7 +3446,7 @@
           <t>upsweep</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="13" t="n">
         <v>11</v>
       </c>
       <c r="J22" t="inlineStr">
@@ -3402,8 +3454,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="K22" s="2" t="n">
-        <v>8.57989122931969</v>
+      <c r="K22" s="13" t="n">
+        <v>8.579891229270752</v>
       </c>
     </row>
     <row r="23">
@@ -3412,15 +3464,15 @@
           <t>xcg_OEW</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="E23" s="13" t="n">
         <v>0.45</v>
       </c>
-      <c r="G23" s="1" t="inlineStr">
+      <c r="G23" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="H23" s="1" t="inlineStr">
+      <c r="H23" s="12" t="inlineStr">
         <is>
           <t>CG Range</t>
         </is>
@@ -3430,17 +3482,17 @@
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
-      <c r="K23" s="2" t="n">
-        <v>0.0774643478551897</v>
+      <c r="K23" s="13" t="n">
+        <v>0.07824925091417723</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="B24" s="1" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t>General States</t>
         </is>
@@ -3450,7 +3502,7 @@
           <t>xcg_payload</t>
         </is>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="13" t="n">
         <v>0.55</v>
       </c>
       <c r="G24" t="inlineStr">
@@ -3458,16 +3510,16 @@
           <t>most_aft_cg [m]</t>
         </is>
       </c>
-      <c r="H24" s="2" t="n">
-        <v>36.94103630849455</v>
+      <c r="H24" s="13" t="n">
+        <v>36.94391438637893</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K24" s="2" t="n">
-        <v>1281518.714370907</v>
+      <c r="K24" s="13" t="n">
+        <v>1281518.714371709</v>
       </c>
     </row>
     <row r="25">
@@ -3476,7 +3528,7 @@
           <t>design_id</t>
         </is>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="13" t="n">
         <v>3</v>
       </c>
       <c r="D25" t="inlineStr">
@@ -3484,7 +3536,7 @@
           <t>V_h</t>
         </is>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="G25" t="inlineStr">
@@ -3502,8 +3554,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K25" s="2" t="n">
-        <v>434466.6841037282</v>
+      <c r="K25" s="13" t="n">
+        <v>434466.6841051969</v>
       </c>
     </row>
     <row r="26">
@@ -3512,7 +3564,7 @@
           <t>kinematic_viscosity [m²/s]</t>
         </is>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="15" t="n">
         <v>1.006e-06</v>
       </c>
       <c r="D26" t="inlineStr">
@@ -3520,7 +3572,7 @@
           <t>V_v</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="13" t="n">
         <v>0.0838</v>
       </c>
       <c r="G26" t="inlineStr">
@@ -3528,16 +3580,16 @@
           <t>most_forward_cg [m]</t>
         </is>
       </c>
-      <c r="H26" s="2" t="n">
-        <v>31.47020801445873</v>
+      <c r="H26" s="13" t="n">
+        <v>31.49295374709665</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K26" s="2" t="n">
-        <v>477913.352514101</v>
+      <c r="K26" s="13" t="n">
+        <v>477913.3525157166</v>
       </c>
     </row>
     <row r="27">
@@ -3546,7 +3598,7 @@
           <t>rho_water [kg/m³]</t>
         </is>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="13" t="n">
         <v>1000</v>
       </c>
       <c r="D27" t="inlineStr">
@@ -3554,7 +3606,7 @@
           <t>k</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E27" s="13" t="n">
         <v>1.174470038720226</v>
       </c>
       <c r="G27" t="inlineStr">
@@ -3572,8 +3624,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K27" s="2" t="n">
-        <v>425845.5147107402</v>
+      <c r="K27" s="13" t="n">
+        <v>430160.3699494032</v>
       </c>
     </row>
     <row r="28">
@@ -3582,7 +3634,7 @@
           <t>viscosity_air [m²/s]</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="15" t="n">
         <v>1.484e-05</v>
       </c>
       <c r="J28" t="inlineStr">
@@ -3590,8 +3642,8 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K28" s="2" t="n">
-        <v>8621.169392987969</v>
+      <c r="K28" s="13" t="n">
+        <v>4306.314155793691</v>
       </c>
     </row>
     <row r="29">
@@ -3600,15 +3652,15 @@
           <t>rho_air [kg/m³]</t>
         </is>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="13" t="n">
         <v>1.225</v>
       </c>
-      <c r="D29" s="1" t="inlineStr">
+      <c r="D29" s="12" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="E29" s="1" t="inlineStr">
+      <c r="E29" s="12" t="inlineStr">
         <is>
           <t>Wing Design</t>
         </is>
@@ -3618,8 +3670,8 @@
           <t>Mff</t>
         </is>
       </c>
-      <c r="K29" s="2" t="n">
-        <v>0.8186888779158671</v>
+      <c r="K29" s="13" t="n">
+        <v>0.8186888149662509</v>
       </c>
     </row>
     <row r="30">
@@ -3628,7 +3680,7 @@
           <t>taper_ratio</t>
         </is>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="E30" s="13" t="n">
         <v>0.4</v>
       </c>
       <c r="J30" t="inlineStr">
@@ -3636,7 +3688,7 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="K30" s="13" t="n">
         <v>1733790.843393344</v>
       </c>
     </row>
@@ -3646,7 +3698,7 @@
           <t>sweep_c_4 [deg]</t>
         </is>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3656,7 +3708,7 @@
           <t>dihedral [deg]</t>
         </is>
       </c>
-      <c r="E32" s="2" t="n">
+      <c r="E32" s="13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3666,7 +3718,7 @@
           <t>sweep_x_c [deg]</t>
         </is>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="13" t="n">
         <v>2.454031674527076</v>
       </c>
     </row>
@@ -3676,8 +3728,8 @@
           <t>chord_root [m]</t>
         </is>
       </c>
-      <c r="E34" s="2" t="n">
-        <v>12.28699770207048</v>
+      <c r="E34" s="13" t="n">
+        <v>12.25698747038679</v>
       </c>
     </row>
     <row r="35">
@@ -3686,8 +3738,8 @@
           <t>chord_tip [m]</t>
         </is>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>4.914799080828193</v>
+      <c r="E35" s="13" t="n">
+        <v>4.902794988154715</v>
       </c>
     </row>
     <row r="36">
@@ -3696,8 +3748,8 @@
           <t>y_MAC [m]</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>18.43049655310572</v>
+      <c r="E36" s="13" t="n">
+        <v>18.38548120558018</v>
       </c>
     </row>
     <row r="37">
@@ -3706,7 +3758,7 @@
           <t>X_LEMAC [m]</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="13" t="n">
         <v>21.05644</v>
       </c>
     </row>
@@ -3716,8 +3768,8 @@
           <t>X_LE [m]</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>20.26656157629547</v>
+      <c r="E38" s="13" t="n">
+        <v>20.26849080547514</v>
       </c>
     </row>
     <row r="39">
@@ -3726,8 +3778,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>9.127484007252358</v>
+      <c r="E39" s="13" t="n">
+        <v>9.105190692287326</v>
       </c>
     </row>
     <row r="40">
@@ -3736,8 +3788,8 @@
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>739.7545314003578</v>
+      <c r="E40" s="13" t="n">
+        <v>736.1453350611716</v>
       </c>
     </row>
     <row r="41">
@@ -3746,8 +3798,8 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>86.00898391449336</v>
+      <c r="E41" s="13" t="n">
+        <v>85.79891229270751</v>
       </c>
     </row>
     <row r="42">
@@ -3756,7 +3808,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="13" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3783,7 +3835,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -3793,42 +3845,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>Requirements</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Inputs</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>General Outputs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="12" t="inlineStr">
         <is>
           <t>Design Mission</t>
         </is>
@@ -3840,7 +3892,7 @@
           <t>design_range [m]</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="13" t="n">
         <v>3704000</v>
       </c>
       <c r="D2" t="inlineStr">
@@ -3848,7 +3900,7 @@
           <t>cruise_altitude [m]</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="13" t="n">
         <v>4</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -3856,7 +3908,7 @@
           <t>d_fuselage [m]</t>
         </is>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="13" t="n">
         <v>8.832726010325398</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -3864,8 +3916,8 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K2" s="2" t="n">
-        <v>2671601.222731659</v>
+      <c r="K2" s="13" t="n">
+        <v>2671601.222731658</v>
       </c>
     </row>
     <row r="3">
@@ -3874,7 +3926,7 @@
           <t>design_payload [kg]</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D3" t="inlineStr">
@@ -3892,7 +3944,7 @@
           <t>r_fuselage [m]</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="13" t="n">
         <v>4.416363005162699</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -3900,8 +3952,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K3" s="2" t="n">
-        <v>477054.4151611131</v>
+      <c r="K3" s="13" t="n">
+        <v>477054.4151611137</v>
       </c>
     </row>
     <row r="4">
@@ -3910,7 +3962,7 @@
           <t>design_crew</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D4" t="inlineStr">
@@ -3928,7 +3980,7 @@
           <t>l_fuselage [m]</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="13" t="n">
         <v>75.07817108776588</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -3936,8 +3988,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K4" s="2" t="n">
-        <v>1304805.956347814</v>
+      <c r="K4" s="13" t="n">
+        <v>1304805.956347813</v>
       </c>
     </row>
     <row r="5">
@@ -3946,7 +3998,7 @@
           <t>ferry_range [m]</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="13" t="n">
         <v>12038000</v>
       </c>
       <c r="D5" t="inlineStr">
@@ -3954,7 +4006,7 @@
           <t>n_wings</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="13" t="n">
         <v>2</v>
       </c>
       <c r="G5" t="inlineStr">
@@ -3962,7 +4014,7 @@
           <t>l_tailcone [m]</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="13" t="n">
         <v>39.74726704646429</v>
       </c>
       <c r="J5" t="inlineStr">
@@ -3970,8 +4022,8 @@
           <t>EW [N]</t>
         </is>
       </c>
-      <c r="K5" s="2" t="n">
-        <v>1304380.956347814</v>
+      <c r="K5" s="13" t="n">
+        <v>1304380.956347813</v>
       </c>
     </row>
     <row r="6">
@@ -3980,7 +4032,7 @@
           <t>reserve_range [m]</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="13" t="n">
         <v>185200</v>
       </c>
       <c r="D6" t="inlineStr">
@@ -3988,7 +4040,7 @@
           <t>n_fuselages</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
@@ -3996,7 +4048,7 @@
           <t>l_nose [m]</t>
         </is>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="13" t="n">
         <v>13.2490890154881</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -4004,7 +4056,7 @@
           <t>ZFW [N]</t>
         </is>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="13" t="n">
         <v>2194546.807570545</v>
       </c>
     </row>
@@ -4014,7 +4066,7 @@
           <t>ferry_payload [kg]</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="14" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
@@ -4022,7 +4074,7 @@
           <t>depth</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="13" t="n">
         <v>0.05</v>
       </c>
       <c r="G7" t="inlineStr">
@@ -4030,7 +4082,7 @@
           <t>l_cargo_straight [m]</t>
         </is>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="13" t="n">
         <v>15.31635142406773</v>
       </c>
       <c r="J7" t="inlineStr">
@@ -4038,8 +4090,8 @@
           <t>h_b</t>
         </is>
       </c>
-      <c r="K7" s="2" t="n">
-        <v>0.08431602766458753</v>
+      <c r="K7" s="13" t="n">
+        <v>0.08431602766458754</v>
       </c>
     </row>
     <row r="8">
@@ -4048,7 +4100,7 @@
           <t>ferry_crew</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="13" t="n">
         <v>170</v>
       </c>
       <c r="D8" t="inlineStr">
@@ -4056,7 +4108,7 @@
           <t>jet_consumption [kg/(N·s)]</t>
         </is>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="15" t="n">
         <v>2.7e-05</v>
       </c>
       <c r="G8" t="inlineStr">
@@ -4064,7 +4116,7 @@
           <t>Re</t>
         </is>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="13" t="n">
         <v>4850602117.146465</v>
       </c>
       <c r="J8" t="inlineStr">
@@ -4072,7 +4124,7 @@
           <t>k</t>
         </is>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="K8" s="13" t="n">
         <v>1.466260010108543</v>
       </c>
     </row>
@@ -4082,7 +4134,7 @@
           <t>altitude_range_WIG [m]</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="13" t="n">
         <v>943600</v>
       </c>
       <c r="D9" t="inlineStr">
@@ -4090,7 +4142,7 @@
           <t>prop_consumption [kg/J]</t>
         </is>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="15" t="n">
         <v>2.1e-08</v>
       </c>
       <c r="G9" t="inlineStr">
@@ -4098,7 +4150,7 @@
           <t>Cd_water</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="13" t="n">
         <v>0.00126964877111443</v>
       </c>
       <c r="J9" t="inlineStr">
@@ -4106,7 +4158,7 @@
           <t>WP [N/W]</t>
         </is>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="K9" s="13" t="n">
         <v>0.08235589165771333</v>
       </c>
     </row>
@@ -4116,7 +4168,7 @@
           <t>altitude_range_WOG [m]</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="13" t="n">
         <v>538000</v>
       </c>
       <c r="D10" t="inlineStr">
@@ -4124,7 +4176,7 @@
           <t>prop_efficiency</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G10" t="inlineStr">
@@ -4132,7 +4184,7 @@
           <t>hull_surface [m²]</t>
         </is>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="13" t="n">
         <v>50.9373226662635</v>
       </c>
       <c r="J10" t="inlineStr">
@@ -4147,7 +4199,7 @@
           <t>altitude_payload [kg]</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="D11" t="inlineStr">
@@ -4155,15 +4207,15 @@
           <t>Cd0</t>
         </is>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02320536089523371</v>
+      <c r="E11" s="13" t="n">
+        <v>0.02320536089523372</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>take_off_power [W]</t>
         </is>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="13" t="n">
         <v>10445052.65531117</v>
       </c>
       <c r="J11" t="inlineStr">
@@ -4171,7 +4223,7 @@
           <t>WS [N/m²]</t>
         </is>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="13" t="n">
         <v>3561.173893518813</v>
       </c>
     </row>
@@ -4181,7 +4233,7 @@
           <t>altitude_crew</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="13" t="n">
         <v>425</v>
       </c>
       <c r="D12" t="inlineStr">
@@ -4189,7 +4241,7 @@
           <t>oswald_factor</t>
         </is>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="13" t="n">
         <v>0.85</v>
       </c>
       <c r="G12" t="inlineStr">
@@ -4202,7 +4254,7 @@
           <t>P [W]</t>
         </is>
       </c>
-      <c r="K12" s="2" t="n">
+      <c r="K12" s="13" t="n">
         <v>32439709.76400011</v>
       </c>
     </row>
@@ -4212,7 +4264,7 @@
           <t>cruise_speed [m/s]</t>
         </is>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="13" t="n">
         <v>115.749</v>
       </c>
       <c r="D13" t="inlineStr">
@@ -4220,7 +4272,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="13" t="n">
         <v>6</v>
       </c>
       <c r="G13" t="inlineStr">
@@ -4228,7 +4280,7 @@
           <t>V_lof [m/s]</t>
         </is>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="13" t="n">
         <v>64.995</v>
       </c>
       <c r="J13" t="inlineStr">
@@ -4243,7 +4295,7 @@
           <t>stall_speed_clean [m/s]</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="13" t="n">
         <v>77.16</v>
       </c>
       <c r="D14" t="inlineStr">
@@ -4251,7 +4303,7 @@
           <t>Cl_alpha</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="13" t="n">
         <v>5</v>
       </c>
       <c r="G14" t="inlineStr">
@@ -4259,7 +4311,7 @@
           <t>LD_g</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="13" t="n">
         <v>13.13819989259052</v>
       </c>
       <c r="J14" t="inlineStr">
@@ -4267,8 +4319,8 @@
           <t>LD</t>
         </is>
       </c>
-      <c r="K14" s="2" t="n">
-        <v>19.26401710731784</v>
+      <c r="K14" s="13" t="n">
+        <v>19.26401710731783</v>
       </c>
     </row>
     <row r="15">
@@ -4277,7 +4329,7 @@
           <t>stall_speed_takeoff [m/s]</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="13" t="n">
         <v>61.9</v>
       </c>
       <c r="D15" t="inlineStr">
@@ -4285,7 +4337,7 @@
           <t>tfo</t>
         </is>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="13" t="n">
         <v>0.001</v>
       </c>
       <c r="J15" t="inlineStr">
@@ -4293,8 +4345,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K15" s="2" t="n">
-        <v>524759.8566772245</v>
+      <c r="K15" s="13" t="n">
+        <v>524759.8566772251</v>
       </c>
     </row>
     <row r="16">
@@ -4303,7 +4355,7 @@
           <t>stall_speed_landing [m/s]</t>
         </is>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="13" t="n">
         <v>61.9</v>
       </c>
       <c r="D16" t="inlineStr">
@@ -4311,15 +4363,15 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="E16" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="1" t="inlineStr">
+      <c r="G16" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="H16" s="1" t="inlineStr">
+      <c r="H16" s="12" t="inlineStr">
         <is>
           <t>Empennage Design</t>
         </is>
@@ -4329,8 +4381,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K16" s="2" t="n">
-        <v>466803.7826471923</v>
+      <c r="K16" s="13" t="n">
+        <v>471935.0699991412</v>
       </c>
     </row>
     <row r="17">
@@ -4339,7 +4391,7 @@
           <t>stall_speed_high</t>
         </is>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="13" t="n">
         <v>82.3</v>
       </c>
       <c r="D17" t="inlineStr">
@@ -4347,7 +4399,7 @@
           <t>n_engines</t>
         </is>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="13" t="n">
         <v>8</v>
       </c>
       <c r="G17" t="inlineStr">
@@ -4355,16 +4407,16 @@
           <t>S_h [m²]</t>
         </is>
       </c>
-      <c r="H17" s="2" t="n">
-        <v>348.4123905193871</v>
+      <c r="H17" s="13" t="n">
+        <v>348.4123905193982</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>10250.63251392083</v>
+      <c r="K17" s="13" t="n">
+        <v>5119.345161972451</v>
       </c>
     </row>
     <row r="18">
@@ -4373,7 +4425,7 @@
           <t>high_altitude [m]</t>
         </is>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="13" t="n">
         <v>3048</v>
       </c>
       <c r="D18" t="inlineStr">
@@ -4381,7 +4433,7 @@
           <t>CLmax_clean</t>
         </is>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="13" t="n">
         <v>1.5</v>
       </c>
       <c r="G18" t="inlineStr">
@@ -4389,16 +4441,16 @@
           <t>S_v [m²]</t>
         </is>
       </c>
-      <c r="H18" s="2" t="n">
-        <v>97.32319441841544</v>
+      <c r="H18" s="13" t="n">
+        <v>97.32319441841854</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
-      <c r="K18" s="2" t="n">
-        <v>0.8214350214013847</v>
+      <c r="K18" s="13" t="n">
+        <v>0.8214350214013845</v>
       </c>
     </row>
     <row r="19">
@@ -4407,7 +4459,7 @@
           <t>cargo_width [m]</t>
         </is>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="13" t="n">
         <v>3.5</v>
       </c>
       <c r="D19" t="inlineStr">
@@ -4415,7 +4467,7 @@
           <t>CLmax_takeoff</t>
         </is>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G19" t="inlineStr">
@@ -4423,15 +4475,15 @@
           <t>l_h [m]</t>
         </is>
       </c>
-      <c r="H19" s="2" t="n">
-        <v>30.64474202029018</v>
+      <c r="H19" s="13" t="n">
+        <v>30.6447420202892</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>MTOM [kg]</t>
         </is>
       </c>
-      <c r="K19" s="2" t="n">
+      <c r="K19" s="13" t="n">
         <v>272334.4773426767</v>
       </c>
     </row>
@@ -4441,7 +4493,7 @@
           <t>cargo_height [m]</t>
         </is>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="13" t="n">
         <v>4</v>
       </c>
       <c r="D20" t="inlineStr">
@@ -4449,7 +4501,7 @@
           <t>CLmax_landing</t>
         </is>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="G20" t="inlineStr">
@@ -4457,16 +4509,16 @@
           <t>l_v [m]</t>
         </is>
       </c>
-      <c r="H20" s="2" t="n">
-        <v>30.64474202029018</v>
+      <c r="H20" s="13" t="n">
+        <v>30.6447420202892</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="K20" s="2" t="n">
-        <v>750.2024058959494</v>
+      <c r="K20" s="13" t="n">
+        <v>750.202405895949</v>
       </c>
     </row>
     <row r="21">
@@ -4475,7 +4527,7 @@
           <t>cargo_length [m]</t>
         </is>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="13" t="n">
         <v>7.32</v>
       </c>
       <c r="D21" t="inlineStr">
@@ -4483,7 +4535,7 @@
           <t>CL_hydro</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="13" t="n">
         <v>0.5</v>
       </c>
       <c r="J21" t="inlineStr">
@@ -4491,7 +4543,7 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="K21" s="2" t="n">
+      <c r="K21" s="13" t="n">
         <v>47.44056510717223</v>
       </c>
     </row>
@@ -4501,7 +4553,7 @@
           <t>cargo_density [kg/m³]</t>
         </is>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="13" t="n">
         <v>160</v>
       </c>
       <c r="D22" t="inlineStr">
@@ -4509,15 +4561,15 @@
           <t>r_float</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="13" t="n">
         <v>1.5</v>
       </c>
-      <c r="G22" s="1" t="inlineStr">
+      <c r="G22" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="H22" s="1" t="inlineStr">
+      <c r="H22" s="12" t="inlineStr">
         <is>
           <t>CG Range</t>
         </is>
@@ -4527,8 +4579,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="K22" s="2" t="n">
-        <v>15.81352170239075</v>
+      <c r="K22" s="13" t="n">
+        <v>15.81352170239074</v>
       </c>
     </row>
     <row r="23">
@@ -4537,7 +4589,7 @@
           <t>upsweep</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="E23" s="13" t="n">
         <v>11</v>
       </c>
       <c r="G23" t="inlineStr">
@@ -4545,25 +4597,25 @@
           <t>most_aft_cg [m]</t>
         </is>
       </c>
-      <c r="H23" s="2" t="n">
-        <v>36.92561195869911</v>
+      <c r="H23" s="13" t="n">
+        <v>36.92561195870009</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
-      <c r="K23" s="2" t="n">
-        <v>0.08491495002281038</v>
+      <c r="K23" s="13" t="n">
+        <v>0.08584836792823627</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="B24" s="1" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t>General States</t>
         </is>
@@ -4573,7 +4625,7 @@
           <t>xcg_OEW</t>
         </is>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="13" t="n">
         <v>0.45</v>
       </c>
       <c r="G24" t="inlineStr">
@@ -4591,8 +4643,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K24" s="2" t="n">
-        <v>1304805.956347814</v>
+      <c r="K24" s="13" t="n">
+        <v>1304805.956347813</v>
       </c>
     </row>
     <row r="25">
@@ -4601,7 +4653,7 @@
           <t>design_id</t>
         </is>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="13" t="n">
         <v>4</v>
       </c>
       <c r="D25" t="inlineStr">
@@ -4609,7 +4661,7 @@
           <t>xcg_payload</t>
         </is>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="13" t="n">
         <v>0.55</v>
       </c>
       <c r="G25" t="inlineStr">
@@ -4617,7 +4669,7 @@
           <t>most_forward_cg [m]</t>
         </is>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="H25" s="13" t="n">
         <v>32.40212780415207</v>
       </c>
       <c r="J25" t="inlineStr">
@@ -4625,8 +4677,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K25" s="2" t="n">
-        <v>477054.4151611131</v>
+      <c r="K25" s="13" t="n">
+        <v>477054.4151611137</v>
       </c>
     </row>
     <row r="26">
@@ -4635,7 +4687,7 @@
           <t>kinematic_viscosity [m²/s]</t>
         </is>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="15" t="n">
         <v>1.006e-06</v>
       </c>
       <c r="D26" t="inlineStr">
@@ -4643,7 +4695,7 @@
           <t>V_h</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="G26" t="inlineStr">
@@ -4661,8 +4713,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K26" s="2" t="n">
-        <v>524759.8566772245</v>
+      <c r="K26" s="13" t="n">
+        <v>524759.8566772251</v>
       </c>
     </row>
     <row r="27">
@@ -4671,7 +4723,7 @@
           <t>rho_water [kg/m³]</t>
         </is>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="13" t="n">
         <v>1000</v>
       </c>
       <c r="D27" t="inlineStr">
@@ -4679,7 +4731,7 @@
           <t>V_v</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E27" s="13" t="n">
         <v>0.0838</v>
       </c>
       <c r="J27" t="inlineStr">
@@ -4687,8 +4739,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K27" s="2" t="n">
-        <v>466803.7826471923</v>
+      <c r="K27" s="13" t="n">
+        <v>471935.0699991412</v>
       </c>
     </row>
     <row r="28">
@@ -4697,7 +4749,7 @@
           <t>viscosity_air [m²/s]</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="15" t="n">
         <v>1.48e-05</v>
       </c>
       <c r="D28" t="inlineStr">
@@ -4705,7 +4757,7 @@
           <t>k</t>
         </is>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E28" s="13" t="n">
         <v>1.466271510318843</v>
       </c>
       <c r="J28" t="inlineStr">
@@ -4713,8 +4765,8 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K28" s="2" t="n">
-        <v>10250.63251392083</v>
+      <c r="K28" s="13" t="n">
+        <v>5119.345161972451</v>
       </c>
     </row>
     <row r="29">
@@ -4723,7 +4775,7 @@
           <t>rho_air [kg/m³]</t>
         </is>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="13" t="n">
         <v>1.225</v>
       </c>
       <c r="J29" t="inlineStr">
@@ -4731,17 +4783,17 @@
           <t>Mff</t>
         </is>
       </c>
-      <c r="K29" s="2" t="n">
-        <v>0.7948786627699523</v>
+      <c r="K29" s="13" t="n">
+        <v>0.7948786627141319</v>
       </c>
     </row>
     <row r="30">
-      <c r="D30" s="1" t="inlineStr">
+      <c r="D30" s="12" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="E30" s="1" t="inlineStr">
+      <c r="E30" s="12" t="inlineStr">
         <is>
           <t>Wing Design</t>
         </is>
@@ -4751,7 +4803,7 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="K30" s="13" t="n">
         <v>1744319.451377081</v>
       </c>
     </row>
@@ -4761,7 +4813,7 @@
           <t>taper_ratio</t>
         </is>
       </c>
-      <c r="E31" s="2" t="n">
+      <c r="E31" s="13" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -4771,7 +4823,7 @@
           <t>sweep_c_4 [deg]</t>
         </is>
       </c>
-      <c r="E32" s="4" t="n">
+      <c r="E32" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4781,7 +4833,7 @@
           <t>dihedral [deg]</t>
         </is>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4791,7 +4843,7 @@
           <t>sweep_x_c [deg]</t>
         </is>
       </c>
-      <c r="E34" s="2" t="n">
+      <c r="E34" s="13" t="n">
         <v>4.085616779974877</v>
       </c>
     </row>
@@ -4801,7 +4853,7 @@
           <t>chord_root [m]</t>
         </is>
       </c>
-      <c r="E35" s="2" t="n">
+      <c r="E35" s="13" t="n">
         <v>22.59074528912964</v>
       </c>
     </row>
@@ -4811,8 +4863,8 @@
           <t>chord_tip [m]</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>9.036298115651858</v>
+      <c r="E36" s="13" t="n">
+        <v>9.036298115651856</v>
       </c>
     </row>
     <row r="37">
@@ -4821,7 +4873,7 @@
           <t>y_MAC [m]</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="13" t="n">
         <v>10.16583538010834</v>
       </c>
     </row>
@@ -4831,7 +4883,7 @@
           <t>X_LEMAC [m]</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E38" s="13" t="n">
         <v>21.05644</v>
       </c>
     </row>
@@ -4841,7 +4893,7 @@
           <t>X_LE [m]</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="13" t="n">
         <v>20.33030890142084</v>
       </c>
     </row>
@@ -4851,8 +4903,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>16.78169650049631</v>
+      <c r="E40" s="13" t="n">
+        <v>16.7816965004963</v>
       </c>
     </row>
     <row r="41">
@@ -4861,8 +4913,8 @@
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>750.2024058959494</v>
+      <c r="E41" s="13" t="n">
+        <v>750.2024058959493</v>
       </c>
     </row>
     <row r="42">
@@ -4871,7 +4923,7 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="13" t="n">
         <v>47.44056510717223</v>
       </c>
     </row>
@@ -4881,7 +4933,7 @@
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E43" s="2" t="n">
+      <c r="E43" s="13" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance aircraft design parameters and calculations
- Updated design parameters in design2.json, design3.json, and design4.json including tail types, engine power, and aerodynamic coefficients.
- Adjusted calculations for fuselage height-to-depth ratio based on wing type in Iteration.py.
- Improved engine count determination logic in Iteration.py to ensure sufficient power during flight and takeoff.
- Introduced EmpType enumeration in empennage.py to categorize tail types and modified tail area calculations accordingly.
- Ensured consistency in fuel economy and performance metrics across different design configurations.
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -426,1149 +426,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="23" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Requirements</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Inputs</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>General Outputs</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Design Mission</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>design_range [m]</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>3704000</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>cruise_altitude [m]</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>d_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>8.832726010325398</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>MTOW [N]</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2535043.010301131</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>design_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aircraft_type</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>PROP</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>r_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>4.416363005162699</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>388858.7248612563</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>design_crew</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>wing_type</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>l_fuselage [m]</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>75.07817108776588</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>1256579.992429574</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ferry_range [m]</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>12038000</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>n_wings</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>l_tailcone [m]</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>39.74726704646429</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>EW [N]</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>1256154.992429574</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ferry_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>n_fuselages</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>l_nose [m]</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>13.2490890154881</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>ZFW [N]</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>2146184.285439875</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>reserve_range [m]</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>185200</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>depth</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>l_cargo_straight [m]</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>15.31635142406773</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>h_b</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>0.04740934087046762</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ferry_crew</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>170</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>jet_consumption [kg/(N·s)]</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>2.7e-05</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>LD_g</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>16.0696979793025</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>1.752476118452925</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>altitude_range_WIG [m]</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>943600</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>prop_consumption [kg/J]</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>2.1e-08</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>4850602117.146465</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>WP [N/W]</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>0.08975876618484213</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>altitude_range_WOG [m]</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>538000</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>prop_efficiency</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Cd_water</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>0.00126964877111443</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>altitude_payload [kg]</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>90000</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Cd0</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02585195421099691</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>hull_surface [m²]</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>154.2858147484878</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>WS [N/m²]</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>3561.173893518813</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>altitude_crew</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>425</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>oswald_factor</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>take_off_power [W]</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>31637380.50337056</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>P [W]</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>28242845.99768967</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>cruise_speed [m/s]</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>115.749</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>take_off_thrust [N]</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>T [N]</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>stall_speed_clean [m/s]</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>77.16</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>tfo</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>V_lof [m/s]</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>64.995</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>LD</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>28.16176193947887</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>stall_speed_takeoff [m/s]</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>n_engines</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>max_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>427744.597347382</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>stall_speed_landing [m/s]</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>61.9</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>CLmax_clean</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>Empennage Design</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>mission_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>382006.368650084</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>stall_speed_high</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>82.3</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CLmax_takeoff</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>S_h [m²]</t>
-        </is>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>166.7313236276682</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>6852.356211172359</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>high_altitude [m]</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>3048</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>CLmax_landing</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>S_v [m²]</t>
-        </is>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>149.6658822681303</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Mff</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>0.8466066558708742</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>cargo_width [m]</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CL_hydro</t>
-        </is>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>l_h [m]</t>
-        </is>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>30.61860656663953</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>MTOM [kg]</t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>258414.170265151</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>cargo_height [m]</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>r_float</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>l_v [m]</t>
-        </is>
-      </c>
-      <c r="H20" s="2" t="n">
-        <v>30.61860656663953</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>711.8559966653349</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>cargo_length [m]</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>upsweep</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>84.37155899148331</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>cargo_density [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>160</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>xcg_OEW</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="G22" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="H22" s="1" t="inlineStr">
-        <is>
-          <t>CG Range</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>8.437155899148332</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>xcg_payload</t>
-        </is>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>most_aft_cg [m]</t>
-        </is>
-      </c>
-      <c r="H23" s="2" t="n">
-        <v>36.95174741234976</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>fuel_economy [L/ton/km]</t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>0.06948969333188471</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>General States</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>V_h</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>most_aft_mission</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>ALTITUDE_OEW_PAYLOAD</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>OEW [N]</t>
-        </is>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>1256579.992429574</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>design_id</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>V_v</t>
-        </is>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>0.083867</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>most_forward_cg [m]</t>
-        </is>
-      </c>
-      <c r="H25" s="2" t="n">
-        <v>33.6303205104692</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>total_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>388858.7248612563</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>kinematic_viscosity [m²/s]</t>
-        </is>
-      </c>
-      <c r="B26" s="3" t="n">
-        <v>1.006e-06</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>xc_OEW</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>most_forward_mission</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>DESIGN_OEW_FUEL</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>max_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>427744.597347382</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>rho_water [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>xc_wing</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>mission_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>382006.368650084</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>viscosity_air [m²/s]</t>
-        </is>
-      </c>
-      <c r="B28" s="3" t="n">
-        <v>1.484e-05</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>xc_fuselage</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>reserve_fuel [N]</t>
-        </is>
-      </c>
-      <c r="K28" s="2" t="n">
-        <v>6852.356211172359</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>rho_air [kg/m³]</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="n">
-        <v>1.225</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>mf_wing</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Mff</t>
-        </is>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>0.8374736970559907</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>mf_fuselage</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>LD</t>
-        </is>
-      </c>
-      <c r="K30" s="2" t="n">
-        <v>28.16176193947887</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="D32" s="1" t="inlineStr">
-        <is>
-          <t>Design 1</t>
-        </is>
-      </c>
-      <c r="E32" s="1" t="inlineStr">
-        <is>
-          <t>Wing Design</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E34" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>sweep_x_c [deg]</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>2.454031674527076</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>chord_root [m]</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>12.0530379738033</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>4.821215189521321</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>18.07955696070495</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>X_LEMAC [m]</t>
-        </is>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>28.95682619287017</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>X_LE [m]</t>
-        </is>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>28.18198803741139</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>8.953685351968167</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="E43" s="2" t="n">
-        <v>711.8510495499273</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>84.37126581662309</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1593,7 +450,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1603,7 +460,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -1613,7 +470,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -1623,7 +480,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Design 2</t>
+          <t>Design 1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -1647,6 +504,1159 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>d_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>8.832726010325398</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>2521142.506681884</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>design_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>aircraft_type</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>PROP</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>r_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>4.416363005162699</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>379881.1284912184</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>design_crew</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>wing_type</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>l_fuselage [m]</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>75.07817108776588</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>1251670.985683984</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ferry_range [m]</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>12038000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>n_wings</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>l_tailcone [m]</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>39.74726704646429</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>EW [N]</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>1251245.985683984</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ferry_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>n_fuselages</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>l_nose [m]</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>13.2490890154881</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ZFW [N]</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>2141261.378190666</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>reserve_range [m]</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>185200</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>l_cargo_straight [m]</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>15.31635142406773</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>h_b</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0.04754245966496118</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ferry_crew</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jet_consumption [kg/(N·s)]</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>2.7e-05</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>LD_g</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>15.97796424723703</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>1.85334974708447</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>altitude_range_WIG [m]</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>943600</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>prop_consumption [kg/J]</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>2.1e-08</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Re</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>4850602117.146465</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>WP [N/W]</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0.08899019624017009</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>altitude_range_WOG [m]</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>538000</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>prop_efficiency</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Cd_water</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0.00126964877111443</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>altitude_payload [kg]</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>90000</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Cd0</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.02614965220289693</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>hull_surface [m²]</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>227.1273881588691</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WS [N/m²]</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>3561.173893518813</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>altitude_crew</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>425</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>oswald_factor</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>take_off_power [W]</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>46574052.27844714</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>P [W]</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>28330564.63745433</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cruise_speed [m/s]</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>115.749</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>take_off_thrust [N]</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>T [N]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>stall_speed_clean [m/s]</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>77.16</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tfo</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>V_lof [m/s]</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>64.995</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>29.61275599654145</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>stall_speed_takeoff [m/s]</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>n_engines</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>max_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>417869.2413403403</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>stall_speed_landing [m/s]</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>CLmax_clean</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>Empennage Design</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>mission_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>373379.9863114323</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>stall_speed_high</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CLmax_takeoff</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>S_h [m²]</t>
+        </is>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>176.706211845237</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>6501.142179786111</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>high_altitude [m]</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>3048</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CLmax_landing</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>S_v [m²]</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>164.664665209161</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0.8493218342539526</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cargo_width [m]</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CL_hydro</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>l_h [m]</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>30.61903360596358</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>MTOM [kg]</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>256997.1974191523</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>cargo_height [m]</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>r_float</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>4.416363005162699</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>l_v [m]</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>30.61903360596358</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>707.8751867993233</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>cargo_length [m]</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>upsweep</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>84.13531879058421</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>cargo_density [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>xcg_OEW</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="H22" s="1" t="inlineStr">
+        <is>
+          <t>CG Range</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>8.413531879058421</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xcg_payload</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>most_aft_cg [m]</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>36.95132037302571</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>fuel_economy [L/ton/km]</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0.06792049262616147</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>General States</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>V_h</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>most_aft_mission</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ALTITUDE_OEW_PAYLOAD</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>OEW [N]</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>1251670.985683984</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>design_id</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>V_v</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.083867</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>most_forward_cg [m]</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>33.78517698949464</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>total_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>379881.1284912184</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>kinematic_viscosity [m²/s]</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1.006e-06</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>xc_OEW</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>most_forward_mission</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>DESIGN_OEW</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>max_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>417869.2413403403</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>rho_water [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>xc_wing</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>mission_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>373379.9863114323</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>viscosity_air [m²/s]</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1.484e-05</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>xc_fuselage</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>6501.142179786111</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rho_air [kg/m³]</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1.225</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>mf_wing</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0.8426326238931933</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>mf_fuselage</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>29.61275599654145</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>engine_power</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>8202000</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>Design 1</t>
+        </is>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>Wing Design</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>dihedral [deg]</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>sweep_x_c [deg]</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>2.454031674527076</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>chord_root [m]</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>12.0568971316919</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>chord_tip [m]</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>4.82275885267676</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>y_MAC [m]</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>18.08534569753785</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>30.03126843510636</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>29.25618219092616</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>8.956552154971124</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>712.3069653765815</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>84.39827992184328</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="27" customWidth="1" min="8" max="8"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Requirements</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Inputs</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>General Outputs</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Design 2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Design Mission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>design_range [m]</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>3704000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>cruise_altitude [m]</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>8</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -1663,7 +1673,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2610442.412995288</v>
+        <v>2572890.464030238</v>
       </c>
     </row>
     <row r="3">
@@ -1699,7 +1709,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>437555.191008916</v>
+        <v>413302.3833444737</v>
       </c>
     </row>
     <row r="4">
@@ -1735,7 +1745,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1283207.529573377</v>
+        <v>1269945.940221734</v>
       </c>
     </row>
     <row r="5">
@@ -1769,7 +1779,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1282782.529573377</v>
+        <v>1269520.940221734</v>
       </c>
     </row>
     <row r="6">
@@ -1803,7 +1813,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2172887.221986372</v>
+        <v>2159588.080685764</v>
       </c>
     </row>
     <row r="7">
@@ -1837,7 +1847,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.09342134021245534</v>
+        <v>0.09410041021936817</v>
       </c>
     </row>
     <row r="8">
@@ -1871,7 +1881,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.424306358628104</v>
+        <v>1.585427912025167</v>
       </c>
     </row>
     <row r="9">
@@ -1905,7 +1915,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.08665443614762731</v>
+        <v>0.08663200611201775</v>
       </c>
     </row>
     <row r="10">
@@ -1954,7 +1964,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02707970372361656</v>
+        <v>0.02708894443781075</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2001,7 +2011,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>30124740.6254892</v>
+        <v>29699075.19749011</v>
       </c>
     </row>
     <row r="13">
@@ -2058,7 +2068,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>15.70118567185378</v>
+        <v>15.69850741052072</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -2066,7 +2076,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>22.36329859042182</v>
+        <v>24.88885182577347</v>
       </c>
     </row>
     <row r="15">
@@ -2084,7 +2094,7 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -2092,7 +2102,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>481310.7101098076</v>
+        <v>454632.6216789212</v>
       </c>
     </row>
     <row r="16">
@@ -2128,7 +2138,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>428815.146324671</v>
+        <v>405498.875336626</v>
       </c>
     </row>
     <row r="17">
@@ -2154,7 +2164,7 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>245.2699382238973</v>
+        <v>245.5976121050805</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2162,7 +2172,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>8740.04468424496</v>
+        <v>7803.508007847762</v>
       </c>
     </row>
     <row r="18">
@@ -2188,7 +2198,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>228.3735647018066</v>
+        <v>228.8614992712976</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2196,7 +2206,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.832382745227138</v>
+        <v>0.8393626199317219</v>
       </c>
     </row>
     <row r="19">
@@ -2222,7 +2232,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>23.04539858668156</v>
+        <v>23.01259444977482</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2230,7 +2240,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>266100.1440362169</v>
+        <v>262272.2185555798</v>
       </c>
     </row>
     <row r="20">
@@ -2256,7 +2266,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>23.04539858668156</v>
+        <v>23.01259444977482</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2264,7 +2274,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>733.3103037384867</v>
+        <v>722.7647120681589</v>
       </c>
     </row>
     <row r="21">
@@ -2290,7 +2300,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>85.63353920856517</v>
+        <v>85.0155698721216</v>
       </c>
     </row>
     <row r="22">
@@ -2326,7 +2336,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>8.563353920856516</v>
+        <v>8.50155698721216</v>
       </c>
     </row>
     <row r="23">
@@ -2344,7 +2354,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>24.42135806102785</v>
+        <v>24.45416219793459</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2352,7 +2362,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.07800454510606263</v>
+        <v>0.0737631484866086</v>
       </c>
     </row>
     <row r="24">
@@ -2381,7 +2391,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>ALTITUDE_OEW_PAYLOAD</t>
+          <t>ALTITUDE_OEW_PAYLOAD_FUEL</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2390,7 +2400,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1283207.529573377</v>
+        <v>1269945.940221734</v>
       </c>
     </row>
     <row r="25">
@@ -2424,7 +2434,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>437555.191008916</v>
+        <v>413302.3833444737</v>
       </c>
     </row>
     <row r="26">
@@ -2460,7 +2470,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>481310.7101098076</v>
+        <v>454632.6216789212</v>
       </c>
     </row>
     <row r="27">
@@ -2486,7 +2496,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>428815.146324671</v>
+        <v>405498.875336626</v>
       </c>
     </row>
     <row r="28">
@@ -2512,7 +2522,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>8740.04468424496</v>
+        <v>7803.508007847762</v>
       </c>
     </row>
     <row r="29">
@@ -2538,7 +2548,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8153246717564306</v>
+        <v>0.8280289117267952</v>
       </c>
     </row>
     <row r="30">
@@ -2574,148 +2584,158 @@
         </is>
       </c>
       <c r="K31" s="2" t="n">
-        <v>22.36329859042182</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" s="1" t="inlineStr">
+        <v>24.88885182577347</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>engine_power</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>8202000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" s="1" t="inlineStr">
         <is>
           <t>Design 2</t>
         </is>
       </c>
-      <c r="E33" s="1" t="inlineStr">
+      <c r="E34" s="1" t="inlineStr">
         <is>
           <t>Wing Design</t>
         </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>0.4</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E35" s="4" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>1</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>2.454031674527076</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>12.23387312081413</v>
+        <v>2.454031674527076</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>4.893549248325652</v>
+        <v>12.23350859609696</v>
       </c>
     </row>
     <row r="40">
       <c r="D40" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>18.35080968122119</v>
+        <v>4.893403438438786</v>
       </c>
     </row>
     <row r="41">
       <c r="D41" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>20.00577388395828</v>
+        <v>18.35026289414545</v>
       </c>
     </row>
     <row r="42">
       <c r="D42" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>19.21931061190594</v>
+        <v>20.36931634844566</v>
       </c>
     </row>
     <row r="43">
       <c r="D43" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>9.08802003260478</v>
+        <v>19.58287651012514</v>
       </c>
     </row>
     <row r="44">
       <c r="D44" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>733.371492527274</v>
+        <v>9.087749242814887</v>
       </c>
     </row>
     <row r="45">
       <c r="D45" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>85.63711184569888</v>
+        <v>733.3277895968137</v>
       </c>
     </row>
     <row r="46">
       <c r="D46" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>85.63456017267875</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E46" s="2" t="n">
+      <c r="E47" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2730,7 +2750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2824,7 +2844,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2622957.14200784</v>
+        <v>2536391.764317184</v>
       </c>
     </row>
     <row r="3">
@@ -2860,7 +2880,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>445637.789224964</v>
+        <v>389729.8133836765</v>
       </c>
     </row>
     <row r="4">
@@ -2896,7 +2916,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1287627.145640868</v>
+        <v>1257056.30916919</v>
       </c>
     </row>
     <row r="5">
@@ -2930,7 +2950,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1287202.145640868</v>
+        <v>1256631.30916919</v>
       </c>
     </row>
     <row r="6">
@@ -2964,7 +2984,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>2177319.352782876</v>
+        <v>2146661.950933507</v>
       </c>
     </row>
     <row r="7">
@@ -2998,7 +3018,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.1161666644374126</v>
+        <v>0.1181319598228359</v>
       </c>
     </row>
     <row r="8">
@@ -3032,7 +3052,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1.343483387947545</v>
+        <v>1.740078814689093</v>
       </c>
     </row>
     <row r="9">
@@ -3066,7 +3086,7 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.08980979329635373</v>
+        <v>0.08980557350154059</v>
       </c>
     </row>
     <row r="10">
@@ -3115,7 +3135,7 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.02572776629574262</v>
+        <v>0.02572937522498603</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3162,7 +3182,7 @@
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>29205691.78188201</v>
+        <v>28243144.22170772</v>
       </c>
     </row>
     <row r="13">
@@ -3219,7 +3239,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.10843550119909</v>
+        <v>16.10793184073512</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -3227,7 +3247,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>21.64141550168546</v>
+        <v>28.02907094451908</v>
       </c>
     </row>
     <row r="15">
@@ -3245,7 +3265,7 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -3261,7 +3281,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>490201.5681474604</v>
+        <v>428702.7947220441</v>
       </c>
     </row>
     <row r="16">
@@ -3287,7 +3307,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>436587.1783089098</v>
+        <v>382843.4334799301</v>
       </c>
     </row>
     <row r="17">
@@ -3323,7 +3343,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>9050.610916054167</v>
+        <v>6886.379903746361</v>
       </c>
     </row>
     <row r="18">
@@ -3349,7 +3369,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>187.4330750456031</v>
+        <v>187.4343404788231</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -3357,7 +3377,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.8301010023809104</v>
+        <v>0.8463447883459775</v>
       </c>
     </row>
     <row r="19">
@@ -3383,7 +3403,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>174.5210187646838</v>
+        <v>174.6617314770828</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -3391,7 +3411,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>267375.8554544179</v>
+        <v>258551.6579324346</v>
       </c>
     </row>
     <row r="20">
@@ -3417,7 +3437,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.63033313524951</v>
+        <v>30.63033581839167</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3425,7 +3445,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>741.03199779522</v>
+        <v>716.5808237974703</v>
       </c>
     </row>
     <row r="21">
@@ -3451,7 +3471,7 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>30.63033313524951</v>
+        <v>30.63033581839167</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -3459,7 +3479,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>86.08321542526278</v>
+        <v>84.65109708665743</v>
       </c>
     </row>
     <row r="22">
@@ -3485,7 +3505,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>8.608321542526278</v>
+        <v>8.465109708665745</v>
       </c>
     </row>
     <row r="23">
@@ -3513,7 +3533,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.07941833336582084</v>
+        <v>0.0696419614171799</v>
       </c>
     </row>
     <row r="24">
@@ -3541,7 +3561,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>36.94002084373978</v>
+        <v>36.94001816059762</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -3549,7 +3569,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1287627.145640868</v>
+        <v>1257056.30916919</v>
       </c>
     </row>
     <row r="25">
@@ -3585,7 +3605,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>445637.789224964</v>
+        <v>389729.8133836765</v>
       </c>
     </row>
     <row r="26">
@@ -3611,7 +3631,7 @@
         </is>
       </c>
       <c r="H26" s="2" t="n">
-        <v>33.63463057823858</v>
+        <v>33.73538822407701</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3619,7 +3639,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>490201.5681474604</v>
+        <v>428702.7947220441</v>
       </c>
     </row>
     <row r="27">
@@ -3655,7 +3675,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>436587.1783089098</v>
+        <v>382843.4334799301</v>
       </c>
     </row>
     <row r="28">
@@ -3681,7 +3701,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>9050.610916054167</v>
+        <v>6886.379903746361</v>
       </c>
     </row>
     <row r="29">
@@ -3707,7 +3727,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.8130244787342943</v>
+        <v>0.8423798213667267</v>
       </c>
     </row>
     <row r="30">
@@ -3743,148 +3763,158 @@
         </is>
       </c>
       <c r="K31" s="2" t="n">
-        <v>21.64141550168546</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" s="1" t="inlineStr">
+        <v>28.02907094451908</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>engine_power</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>8202000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" s="1" t="inlineStr">
         <is>
           <t>Design 3</t>
         </is>
       </c>
-      <c r="E33" s="1" t="inlineStr">
+      <c r="E34" s="1" t="inlineStr">
         <is>
           <t>Wing Design</t>
         </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>0.4</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E35" s="4" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>1</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>2.454031674527076</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>12.29760219641277</v>
+        <v>2.454031674527076</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
+          <t>chord_root [m]</t>
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>4.919040878565108</v>
+        <v>12.29763023072162</v>
       </c>
     </row>
     <row r="40">
       <c r="D40" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
+          <t>chord_tip [m]</t>
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>18.44640329461915</v>
+        <v>4.919052092288649</v>
       </c>
     </row>
     <row r="41">
       <c r="D41" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
+          <t>y_MAC [m]</t>
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>28.93502503931185</v>
+        <v>18.44644534608243</v>
       </c>
     </row>
     <row r="42">
       <c r="D42" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
+          <t>X_LEMAC [m]</t>
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>28.14446489811388</v>
+        <v>29.30043783853776</v>
       </c>
     </row>
     <row r="43">
       <c r="D43" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>X_LE [m]</t>
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>9.135361631620913</v>
+        <v>28.50987589513423</v>
       </c>
     </row>
     <row r="44">
       <c r="D44" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>741.0319969279589</v>
+        <v>9.13538245710749</v>
       </c>
     </row>
     <row r="45">
       <c r="D45" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>86.08321537488936</v>
+        <v>741.0353755286358</v>
       </c>
     </row>
     <row r="46">
       <c r="D46" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>86.08341161505135</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E46" s="2" t="n">
+      <c r="E47" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3899,7 +3929,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3911,13 +3941,13 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3992,8 +4022,8 @@
           <t>MTOW [N]</t>
         </is>
       </c>
-      <c r="K2" s="2" t="n">
-        <v>2700961.475400982</v>
+      <c r="K2" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -4028,8 +4058,8 @@
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K3" s="2" t="n">
-        <v>496016.6416391923</v>
+      <c r="K3" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -4064,8 +4094,8 @@
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K4" s="2" t="n">
-        <v>1315174.622286388</v>
+      <c r="K4" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -4098,8 +4128,8 @@
           <t>EW [N]</t>
         </is>
       </c>
-      <c r="K5" s="2" t="n">
-        <v>1314749.622286388</v>
+      <c r="K5" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -4132,8 +4162,8 @@
           <t>ZFW [N]</t>
         </is>
       </c>
-      <c r="K6" s="2" t="n">
-        <v>2204944.83376179</v>
+      <c r="K6" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -4166,8 +4196,8 @@
           <t>h_b</t>
         </is>
       </c>
-      <c r="K7" s="2" t="n">
-        <v>0.08385649659017519</v>
+      <c r="K7" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -4200,8 +4230,8 @@
           <t>k</t>
         </is>
       </c>
-      <c r="K8" s="2" t="n">
-        <v>1.468568290239539</v>
+      <c r="K8" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -4234,8 +4264,8 @@
           <t>WP [N/W]</t>
         </is>
       </c>
-      <c r="K9" s="2" t="n">
-        <v>0.07590230305533839</v>
+      <c r="K9" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -4283,8 +4313,8 @@
           <t>Cd0</t>
         </is>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>0.02639956891071301</v>
+      <c r="E11" s="3" t="n">
+        <v/>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -4330,8 +4360,8 @@
           <t>P [W]</t>
         </is>
       </c>
-      <c r="K12" s="2" t="n">
-        <v>35584710.43272272</v>
+      <c r="K12" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -4387,16 +4417,16 @@
           <t>LD_g</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
-        <v>12.31775640184354</v>
+      <c r="H14" s="3" t="n">
+        <v/>
       </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>LD</t>
         </is>
       </c>
-      <c r="K14" s="2" t="n">
-        <v>18.08946645864251</v>
+      <c r="K14" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -4421,8 +4451,8 @@
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K15" s="2" t="n">
-        <v>545618.3058031115</v>
+      <c r="K15" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -4439,8 +4469,8 @@
           <t>n_engines</t>
         </is>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>8</v>
+      <c r="E16" s="3" t="n">
+        <v/>
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
@@ -4457,8 +4487,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K16" s="2" t="n">
-        <v>485047.0515637147</v>
+      <c r="K16" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="17">
@@ -4483,16 +4513,16 @@
           <t>S_h [m²]</t>
         </is>
       </c>
-      <c r="H17" s="2" t="n">
-        <v>354.1396874821904</v>
+      <c r="H17" s="3" t="n">
+        <v/>
       </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>10969.59007547755</v>
+      <c r="K17" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -4517,16 +4547,16 @@
           <t>S_v [m²]</t>
         </is>
       </c>
-      <c r="H18" s="2" t="n">
-        <v>98.92301937002517</v>
+      <c r="H18" s="3" t="n">
+        <v/>
       </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Mff</t>
         </is>
       </c>
-      <c r="K18" s="2" t="n">
-        <v>0.8163555288897432</v>
+      <c r="K18" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -4552,15 +4582,15 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>30.65149497925002</v>
+        <v/>
       </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>MTOM [kg]</t>
         </is>
       </c>
-      <c r="K19" s="2" t="n">
-        <v>275327.3675230358</v>
+      <c r="K19" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -4586,15 +4616,15 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>30.65149497925002</v>
+        <v/>
       </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>S [m²]</t>
         </is>
       </c>
-      <c r="K20" s="2" t="n">
-        <v>758.4471076824697</v>
+      <c r="K20" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="21">
@@ -4619,8 +4649,8 @@
           <t>b [m]</t>
         </is>
       </c>
-      <c r="K21" s="2" t="n">
-        <v>47.70053797440244</v>
+      <c r="K21" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="22">
@@ -4655,8 +4685,8 @@
           <t>MAC [m]</t>
         </is>
       </c>
-      <c r="K22" s="2" t="n">
-        <v>15.90017932480081</v>
+      <c r="K22" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -4674,15 +4704,15 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>36.91885899973926</v>
+        <v/>
       </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
-      <c r="K23" s="2" t="n">
-        <v>0.08823353124662627</v>
+      <c r="K23" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -4709,18 +4739,13 @@
           <t>most_aft_mission</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>ALTITUDE_OEW_PAYLOAD</t>
-        </is>
-      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>OEW [N]</t>
         </is>
       </c>
-      <c r="K24" s="2" t="n">
-        <v>1315174.622286388</v>
+      <c r="K24" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="25">
@@ -4746,15 +4771,15 @@
         </is>
       </c>
       <c r="H25" s="2" t="n">
-        <v>33.78517698949464</v>
+        <v/>
       </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>total_fuel [N]</t>
         </is>
       </c>
-      <c r="K25" s="2" t="n">
-        <v>496016.6416391923</v>
+      <c r="K25" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="26">
@@ -4779,18 +4804,13 @@
           <t>most_forward_mission</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>DESIGN_OEW</t>
-        </is>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
           <t>max_fuel [N]</t>
         </is>
       </c>
-      <c r="K26" s="2" t="n">
-        <v>545618.3058031115</v>
+      <c r="K26" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="27">
@@ -4815,8 +4835,8 @@
           <t>mission_fuel [N]</t>
         </is>
       </c>
-      <c r="K27" s="2" t="n">
-        <v>485047.0515637147</v>
+      <c r="K27" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="28">
@@ -4841,8 +4861,8 @@
           <t>reserve_fuel [N]</t>
         </is>
       </c>
-      <c r="K28" s="2" t="n">
-        <v>10969.59007547755</v>
+      <c r="K28" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="29">
@@ -4867,8 +4887,8 @@
           <t>Mff</t>
         </is>
       </c>
-      <c r="K29" s="2" t="n">
-        <v>0.7858151769334533</v>
+      <c r="K29" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -4903,8 +4923,8 @@
           <t>LD</t>
         </is>
       </c>
-      <c r="K31" s="2" t="n">
-        <v>18.08946645864251</v>
+      <c r="K31" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="32">
@@ -4917,146 +4937,156 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="33"/>
-    <row r="34">
-      <c r="D34" s="1" t="inlineStr">
+    <row r="33">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>engine_power</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>8202000</v>
+      </c>
+    </row>
+    <row r="34"/>
+    <row r="35">
+      <c r="D35" s="1" t="inlineStr">
         <is>
           <t>Design 4</t>
         </is>
       </c>
-      <c r="E34" s="1" t="inlineStr">
+      <c r="E35" s="1" t="inlineStr">
         <is>
           <t>Wing Design</t>
         </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>taper_ratio</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>0.4</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>sweep_c_4 [deg]</t>
-        </is>
-      </c>
-      <c r="E36" s="4" t="n">
-        <v>0</v>
+          <t>taper_ratio</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
         <is>
-          <t>dihedral [deg]</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>5</v>
+          <t>sweep_c_4 [deg]</t>
+        </is>
+      </c>
+      <c r="E37" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
-          <t>sweep_x_c [deg]</t>
+          <t>dihedral [deg]</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>4.085616779974877</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="inlineStr">
         <is>
-          <t>chord_root [m]</t>
+          <t>sweep_x_c [deg]</t>
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>22.7155257137488</v>
+        <v>4.085616779974877</v>
       </c>
     </row>
     <row r="40">
       <c r="D40" t="inlineStr">
         <is>
-          <t>chord_tip [m]</t>
-        </is>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>9.086210285499522</v>
+          <t>chord_root [m]</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="41">
       <c r="D41" t="inlineStr">
         <is>
-          <t>y_MAC [m]</t>
-        </is>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>10.22198657118696</v>
+          <t>chord_tip [m]</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="D42" t="inlineStr">
         <is>
-          <t>X_LEMAC [m]</t>
-        </is>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>28.00634157148075</v>
+          <t>y_MAC [m]</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="D43" t="inlineStr">
         <is>
-          <t>X_LE [m]</t>
-        </is>
-      </c>
-      <c r="E43" s="2" t="n">
-        <v>27.27619967353882</v>
+          <t>X_LEMAC [m]</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="44">
       <c r="D44" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
-        </is>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>16.8743905302134</v>
+          <t>X_LE [m]</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="D45" t="inlineStr">
         <is>
-          <t>S [m²]</t>
-        </is>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>758.5128094244151</v>
+          <t>MAC [m]</t>
+        </is>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="46">
       <c r="D46" t="inlineStr">
         <is>
-          <t>b [m]</t>
-        </is>
-      </c>
-      <c r="E46" s="2" t="n">
-        <v>47.70260399887248</v>
+          <t>S [m²]</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v/>
       </c>
     </row>
     <row r="47">
       <c r="D47" t="inlineStr">
         <is>
+          <t>b [m]</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="D48" t="inlineStr">
+        <is>
           <t>aspect_ratio</t>
         </is>
       </c>
-      <c r="E47" s="2" t="n">
+      <c r="E48" s="2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lekker maannnn Co-authored-by: OM00n <OM00n@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Concept_Data.xlsx
+++ b/Concept_Data.xlsx
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2551444.849727417</v>
+        <v>5063828.278001635</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1262372.353813677</v>
+        <v>2149628.494650865</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1261947.353813677</v>
+        <v>2149203.494650865</v>
       </c>
     </row>
     <row r="5">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2151993.048663405</v>
+        <v>3041761.572928867</v>
       </c>
     </row>
     <row r="6">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.07248959032389077</v>
+        <v>0.1782473313794926</v>
       </c>
     </row>
     <row r="7">
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.645420237712711</v>
+        <v>1.306615576957792</v>
       </c>
     </row>
     <row r="8">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>16.18725274058268</v>
+        <v>3.447769133030232</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09892120449745467</v>
+        <v>0.01175470307537344</v>
       </c>
     </row>
     <row r="9">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>25792698.97378845</v>
+        <v>430791679.3415694</v>
       </c>
     </row>
     <row r="12">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01528670068596075</v>
+        <v>0.02808034614239474</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>260086.1212770048</v>
+        <v>516190.4462794735</v>
       </c>
     </row>
     <row r="14">
@@ -909,7 +909,7 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -921,11 +921,11 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>MTOW [N]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>2551444.849727417</v>
+        <v>1007.172606663031</v>
       </c>
     </row>
     <row r="15">
@@ -955,11 +955,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>507.4782593866299</v>
+        <v>22.44072867202657</v>
       </c>
     </row>
     <row r="16">
@@ -981,11 +981,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>55.18033668182698</v>
+        <v>44.88145734405313</v>
       </c>
     </row>
     <row r="17">
@@ -1003,7 +1003,7 @@
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
@@ -1017,11 +1017,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>9.196722780304494</v>
+        <v>0.3447722582329494</v>
       </c>
     </row>
     <row r="18">
@@ -1047,15 +1047,15 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>104.008307348075</v>
+        <v>126.0113097725951</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.07200287928211609</v>
+        <v>2149628.494650865</v>
       </c>
     </row>
     <row r="19">
@@ -1081,15 +1081,15 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>42.85803760908085</v>
+        <v>42.75652417695105</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Mff</t>
+          <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>0.833789611797864</v>
+        <v>2022066.705072768</v>
       </c>
     </row>
     <row r="20">
@@ -1119,11 +1119,11 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>1262372.353813677</v>
+        <v>2224273.375580045</v>
       </c>
     </row>
     <row r="21">
@@ -1149,15 +1149,15 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>21.63417165195694</v>
+        <v>23.81283044866103</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>399451.8010640119</v>
+        <v>1991607.755342387</v>
       </c>
     </row>
     <row r="22">
@@ -1183,15 +1183,15 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>7.396298000669041</v>
+        <v>8.141138614926849</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>mission_fuel [N]</t>
+          <t>reserve_fuel [N]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>395822.1302768486</v>
+        <v>30458.94973038044</v>
       </c>
     </row>
     <row r="23">
@@ -1209,15 +1209,15 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>2.218889400200712</v>
+        <v>2.442341584478055</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>Mff</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>3629.670787163253</v>
+        <v>0.4760825108746616</v>
       </c>
     </row>
     <row r="24">
@@ -1249,11 +1249,11 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>max_fuel [N]</t>
+          <t>LD</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>439396.9811704131</v>
+        <v>4.504908854971563</v>
       </c>
     </row>
     <row r="25">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>MTOW [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>26.63483325232527</v>
+        <v>5063828.278001635</v>
       </c>
     </row>
     <row r="26">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="H27" s="2" t="n">
-        <v>5.272232933810239</v>
+        <v>5.803170602435036</v>
       </c>
     </row>
     <row r="28">
@@ -1409,7 +1409,7 @@
         </is>
       </c>
       <c r="H30" s="2" t="n">
-        <v>18.41186132815308</v>
+        <v>19.44530708478115</v>
       </c>
     </row>
     <row r="31">
@@ -1427,7 +1427,7 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>71.77910835987775</v>
+        <v>71.47725075457996</v>
       </c>
     </row>
     <row r="32">
@@ -1445,7 +1445,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>0.9963038415361176</v>
+        <v>0.9963361721857805</v>
       </c>
     </row>
     <row r="34">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>61.17322229150245</v>
+        <v>75.08458470793089</v>
       </c>
     </row>
     <row r="36">
@@ -1503,7 +1503,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>38.39118683937023</v>
+        <v>37.80538984967581</v>
       </c>
     </row>
     <row r="37">
@@ -1539,7 +1539,7 @@
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>9.579135317827683</v>
+        <v>10.61258107445575</v>
       </c>
     </row>
     <row r="39">
@@ -1549,7 +1549,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>13.13817540043679</v>
+        <v>13.99497923125437</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>7.513047308100144</v>
+        <v>8.323592999573135</v>
       </c>
     </row>
     <row r="40">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>5.255270160174716</v>
+        <v>5.597991692501751</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>5.2591331156701</v>
+        <v>5.826515099701195</v>
       </c>
     </row>
     <row r="41">
@@ -1585,7 +1585,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>11.82435786039311</v>
+        <v>12.59548130812894</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1621,7 +1621,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>29.18667144507828</v>
+        <v>29.13159119881143</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1629,7 +1629,7 @@
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>6.452381805780124</v>
+        <v>7.148497517280457</v>
       </c>
     </row>
     <row r="44">
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>9.759787440324471</v>
+        <v>10.39627028607468</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>507.4782593867685</v>
+        <v>575.8267644287293</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1665,7 +1665,7 @@
         </is>
       </c>
       <c r="H45" s="2" t="n">
-        <v>67.26512377966574</v>
+        <v>66.45457808819275</v>
       </c>
     </row>
     <row r="46">
@@ -1675,7 +1675,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>55.18033668183451</v>
+        <v>58.77891277126837</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1683,7 +1683,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>0.9369158465496081</v>
+        <v>0.9305410987545986</v>
       </c>
     </row>
     <row r="47">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="H49" s="2" t="n">
-        <v>31.94267357844819</v>
+        <v>32.04663074560832</v>
       </c>
     </row>
     <row r="50">
@@ -1775,7 +1775,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2477113.486910657</v>
+        <v>2570378.747851773</v>
       </c>
     </row>
     <row r="3">
@@ -1893,7 +1893,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1236121.998325037</v>
+        <v>1269058.919722274</v>
       </c>
     </row>
     <row r="4">
@@ -1929,7 +1929,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1235696.998325037</v>
+        <v>1268633.919722274</v>
       </c>
     </row>
     <row r="5">
@@ -1965,7 +1965,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2125668.361811948</v>
+        <v>2158698.548470126</v>
       </c>
     </row>
     <row r="6">
@@ -1999,7 +1999,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.1139503221852491</v>
+        <v>0.1118651563325267</v>
       </c>
     </row>
     <row r="7">
@@ -2033,7 +2033,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.751122171484751</v>
+        <v>1.760781169118705</v>
       </c>
     </row>
     <row r="8">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.1159173987792671</v>
+        <v>0.0905172449519278</v>
       </c>
     </row>
     <row r="9">
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>21369643.49612125</v>
+        <v>28396564.09358083</v>
       </c>
     </row>
     <row r="12">
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01624170321277417</v>
+        <v>0.01999736626769847</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.85</v>
+        <v>0.5165840932860424</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>252509.0200724421</v>
+        <v>262016.1822478872</v>
       </c>
     </row>
     <row r="14">
@@ -2254,7 +2254,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>20.27396154450959</v>
+        <v>14.24390454879271</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>492.8886971391199</v>
+        <v>511.4348358128607</v>
       </c>
     </row>
     <row r="15">
@@ -2296,7 +2296,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>70.20603230058795</v>
+        <v>71.51467232763223</v>
       </c>
     </row>
     <row r="16">
@@ -2330,7 +2330,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>7.020603230058796</v>
+        <v>7.151467232763223</v>
       </c>
     </row>
     <row r="17">
@@ -2356,7 +2356,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.06344119704400235</v>
+        <v>0.07418416905868408</v>
       </c>
     </row>
     <row r="18">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1236121.998325037</v>
+        <v>1269058.919722274</v>
       </c>
     </row>
     <row r="19">
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>125.961341768606</v>
+        <v>134.3956670107062</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2426,7 +2426,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>351445.1250987092</v>
+        <v>411680.1993816475</v>
       </c>
     </row>
     <row r="20">
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>26.23830548984</v>
+        <v>25.9926144704699</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2460,7 +2460,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>386589.6376085802</v>
+        <v>452848.2193198123</v>
       </c>
     </row>
     <row r="21">
@@ -2494,7 +2494,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>348755.9110362888</v>
+        <v>407813.3558322787</v>
       </c>
     </row>
     <row r="22">
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>23.80810865983955</v>
+        <v>24.59228540717958</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>2689.214062420477</v>
+        <v>3866.843549368728</v>
       </c>
     </row>
     <row r="23">
@@ -2546,7 +2546,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>8.139524328150275</v>
+        <v>8.407618942625497</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8581231231609757</v>
+        <v>0.8301777012940091</v>
       </c>
     </row>
     <row r="24">
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>2.441857298445082</v>
+        <v>2.522285682787649</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2477113.486910657</v>
+        <v>2570378.747851773</v>
       </c>
     </row>
     <row r="25">
@@ -2624,7 +2624,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>35.50218356441998</v>
+        <v>25.08039890423847</v>
       </c>
     </row>
     <row r="26">
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="H28" s="2" t="n">
-        <v>5.802019905707118</v>
+        <v>5.993123246281764</v>
       </c>
     </row>
     <row r="29">
@@ -2764,7 +2764,7 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>13.04409064985536</v>
+        <v>13.29015825016814</v>
       </c>
     </row>
     <row r="32">
@@ -2774,7 +2774,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>46.15370972540087</v>
+        <v>45.93321849069467</v>
       </c>
     </row>
     <row r="33">
@@ -2794,7 +2794,7 @@
         </is>
       </c>
       <c r="H33" s="2" t="n">
-        <v>0.9107075979361759</v>
+        <v>0.907699639517493</v>
       </c>
     </row>
     <row r="34">
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>62.36777475372117</v>
+        <v>66.93631153029222</v>
       </c>
     </row>
     <row r="37">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>23.26613013509861</v>
+        <v>22.91314980677214</v>
       </c>
     </row>
     <row r="38">
@@ -2870,7 +2870,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>10.02943319137639</v>
+        <v>10.21638176109032</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>4.011773276550556</v>
+        <v>4.086552704436128</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2896,7 +2896,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>6.839285859305114</v>
+        <v>7.085353459617887</v>
       </c>
     </row>
     <row r="40">
@@ -2906,7 +2906,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>15.04414978706459</v>
+        <v>15.32457264163548</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2914,7 +2914,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>10.72829154400802</v>
+        <v>11.11427993665551</v>
       </c>
     </row>
     <row r="41">
@@ -2924,7 +2924,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>20.50030140106906</v>
+        <v>20.48919131464034</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="H41" s="2" t="n">
-        <v>7.509804080805615</v>
+        <v>7.779995955658856</v>
       </c>
     </row>
     <row r="42">
@@ -2942,7 +2942,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>19.85555212448057</v>
+        <v>19.8324239157131</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2960,7 +2960,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>7.45043608502246</v>
+        <v>7.58931216538138</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>492.8886976873837</v>
+        <v>511.4348358128607</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>9.21370920838336</v>
+        <v>9.54520512206885</v>
       </c>
     </row>
     <row r="45">
@@ -2996,7 +2996,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>70.20603233963473</v>
+        <v>71.51467232763223</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>41.7125491756691</v>
+        <v>41.32656078302162</v>
       </c>
     </row>
     <row r="47">
@@ -3032,7 +3032,7 @@
         </is>
       </c>
       <c r="H47" s="2" t="n">
-        <v>0.8543859172794795</v>
+        <v>0.8493515863578955</v>
       </c>
     </row>
     <row r="49">
@@ -3054,7 +3054,7 @@
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>21.79062188848577</v>
+        <v>21.87705207123873</v>
       </c>
     </row>
     <row r="51">
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="H52" s="2" t="n">
-        <v>20.35699806851514</v>
+        <v>20.36271449551757</v>
       </c>
     </row>
     <row r="53">
@@ -3114,7 +3114,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
@@ -3196,7 +3196,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2581229.318008765</v>
+        <v>2660727.319954871</v>
       </c>
     </row>
     <row r="3">
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1272890.832835149</v>
+        <v>1300965.803246581</v>
       </c>
     </row>
     <row r="4">
@@ -3268,7 +3268,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1272465.832835149</v>
+        <v>1300540.803246581</v>
       </c>
     </row>
     <row r="5">
@@ -3304,7 +3304,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2162541.312153158</v>
+        <v>2190695.780566536</v>
       </c>
     </row>
     <row r="6">
@@ -3338,7 +3338,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.1555636565419782</v>
+        <v>0.1532238839175074</v>
       </c>
     </row>
     <row r="7">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.659597520283095</v>
+        <v>1.666673256498418</v>
       </c>
     </row>
     <row r="8">
@@ -3406,7 +3406,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.1075410126279081</v>
+        <v>0.09462125105302413</v>
       </c>
     </row>
     <row r="9">
@@ -3505,7 +3505,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>24002278.33951888</v>
+        <v>28119764.74992753</v>
       </c>
     </row>
     <row r="12">
@@ -3523,7 +3523,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01563875653706044</v>
+        <v>0.01840271117319238</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3551,7 +3551,7 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.85</v>
+        <v>0.6560637537879077</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -3567,7 +3567,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>263122.2546390178</v>
+        <v>271226.0264989675</v>
       </c>
     </row>
     <row r="14">
@@ -3593,7 +3593,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>18.47984344561729</v>
+        <v>14.96656207991779</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -3601,7 +3601,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>516.5278320170655</v>
+        <v>532.4233329153501</v>
       </c>
     </row>
     <row r="15">
@@ -3635,7 +3635,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>64.28236660342029</v>
+        <v>65.26397676607517</v>
       </c>
     </row>
     <row r="16">
@@ -3669,7 +3669,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>8.035295825427538</v>
+        <v>8.157997095759399</v>
       </c>
     </row>
     <row r="17">
@@ -3695,7 +3695,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.05982790345049654</v>
+        <v>0.06710844155612598</v>
       </c>
     </row>
     <row r="18">
@@ -3731,7 +3731,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1272890.832835149</v>
+        <v>1300965.803246581</v>
       </c>
     </row>
     <row r="19">
@@ -3757,7 +3757,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>102.4252394820564</v>
+        <v>107.560982202006</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>418688.0058556065</v>
+        <v>470031.5393883352</v>
       </c>
     </row>
     <row r="20">
@@ -3791,7 +3791,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>38.70244338581857</v>
+        <v>38.56875535520682</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3799,7 +3799,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>460556.8064411671</v>
+        <v>517034.6933271688</v>
       </c>
     </row>
     <row r="21">
@@ -3833,7 +3833,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>415520.6887051093</v>
+        <v>466085.9606487952</v>
       </c>
     </row>
     <row r="22">
@@ -3859,7 +3859,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>21.46889791464047</v>
+        <v>22.00055499093209</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -3867,7 +3867,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>3167.317150497169</v>
+        <v>3945.578739540011</v>
       </c>
     </row>
     <row r="23">
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>7.339794158851442</v>
+        <v>7.521557261857124</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -3893,7 +3893,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8377951145469731</v>
+        <v>0.823344716362627</v>
       </c>
     </row>
     <row r="24">
@@ -3921,7 +3921,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>2.201938247655432</v>
+        <v>2.256467178557137</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -3929,7 +3929,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2581229.318008765</v>
+        <v>2660727.319954871</v>
       </c>
     </row>
     <row r="25">
@@ -3963,7 +3963,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>30.66910235756628</v>
+        <v>24.94436876032232</v>
       </c>
     </row>
     <row r="26">
@@ -4041,7 +4041,7 @@
         </is>
       </c>
       <c r="H28" s="2" t="n">
-        <v>5.231955836309488</v>
+        <v>5.361520304605847</v>
       </c>
     </row>
     <row r="29">
@@ -4113,7 +4113,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>67.43837692891444</v>
+        <v>67.25661382590876</v>
       </c>
     </row>
     <row r="33">
@@ -4133,7 +4133,7 @@
         </is>
       </c>
       <c r="H33" s="2" t="n">
-        <v>0.9381802282708679</v>
+        <v>0.9367482728370877</v>
       </c>
     </row>
     <row r="34">
@@ -4181,7 +4181,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>79.041179764836</v>
+        <v>83.2667191776651</v>
       </c>
     </row>
     <row r="37">
@@ -4199,7 +4199,7 @@
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>35.2308628961525</v>
+        <v>34.99856616369847</v>
       </c>
     </row>
     <row r="38">
@@ -4209,7 +4209,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>11.47899404719035</v>
+        <v>11.65428142466143</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4227,7 +4227,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>4.59159761887614</v>
+        <v>4.661712569864574</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -4235,7 +4235,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>10.88860733277006</v>
+        <v>11.17587038071298</v>
       </c>
     </row>
     <row r="40">
@@ -4245,7 +4245,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>13.77479285662842</v>
+        <v>13.98513770959372</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>11.2543745041551</v>
+        <v>11.55128721520721</v>
       </c>
     </row>
     <row r="41">
@@ -4263,7 +4263,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>29.34908821744476</v>
+        <v>29.33867113901219</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4271,7 +4271,7 @@
         </is>
       </c>
       <c r="H41" s="2" t="n">
-        <v>3.26376860620498</v>
+        <v>3.349873292410091</v>
       </c>
     </row>
     <row r="42">
@@ -4281,7 +4281,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>28.61115288583966</v>
+        <v>28.58946733314109</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4299,7 +4299,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>8.527252720769974</v>
+        <v>8.657466201177066</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4317,7 +4317,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>516.5278329948915</v>
+        <v>532.4233200588175</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4325,7 +4325,7 @@
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>7.992059951503632</v>
+        <v>8.202906337166011</v>
       </c>
     </row>
     <row r="45">
@@ -4335,7 +4335,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>64.28236666426596</v>
+        <v>65.26397597810403</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -4361,7 +4361,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>63.52379658361079</v>
+        <v>63.22688387255867</v>
       </c>
     </row>
     <row r="47">
@@ -4371,7 +4371,7 @@
         </is>
       </c>
       <c r="H47" s="2" t="n">
-        <v>0.891940682125739</v>
+        <v>0.88919528114889</v>
       </c>
     </row>
     <row r="49">
@@ -4393,7 +4393,7 @@
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>31.73441232728653</v>
+        <v>31.76059205294476</v>
       </c>
     </row>
     <row r="51">
@@ -4535,7 +4535,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2577428.867806494</v>
+        <v>2585704.03231381</v>
       </c>
     </row>
     <row r="3">
@@ -4571,7 +4571,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1271548.691845855</v>
+        <v>1274471.092321406</v>
       </c>
     </row>
     <row r="4">
@@ -4607,7 +4607,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1271123.691845855</v>
+        <v>1274046.092321406</v>
       </c>
     </row>
     <row r="5">
@@ -4643,7 +4643,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2161195.370713661</v>
+        <v>2164126.04635372</v>
       </c>
     </row>
     <row r="6">
@@ -4677,7 +4677,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.09765387697344766</v>
+        <v>0.09749748833112409</v>
       </c>
     </row>
     <row r="7">
@@ -4711,7 +4711,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.489326385455202</v>
+        <v>1.489981645027543</v>
       </c>
     </row>
     <row r="8">
@@ -4745,7 +4745,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09508268494521059</v>
+        <v>0.09357096497711698</v>
       </c>
     </row>
     <row r="9">
@@ -4844,7 +4844,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>27107236.92007313</v>
+        <v>27633615.11710551</v>
       </c>
     </row>
     <row r="12">
@@ -4862,7 +4862,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01474047648809187</v>
+        <v>0.01470646584450298</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -4890,7 +4890,7 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.85</v>
+        <v>0.806962284413828</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -4906,7 +4906,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>262734.8489099382</v>
+        <v>263578.3926925393</v>
       </c>
     </row>
     <row r="14">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.48444263477726</v>
+        <v>16.08025846911854</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -4940,7 +4940,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>559.2677131811857</v>
+        <v>561.0633135905323</v>
       </c>
     </row>
     <row r="15">
@@ -4974,7 +4974,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>40.9609953436627</v>
+        <v>41.02669790236105</v>
       </c>
     </row>
     <row r="16">
@@ -5000,7 +5000,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>13.65366511455423</v>
+        <v>13.67556596745369</v>
       </c>
     </row>
     <row r="17">
@@ -5036,7 +5036,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.07499642543164681</v>
+        <v>0.07594985111932576</v>
       </c>
     </row>
     <row r="18">
@@ -5062,7 +5062,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1271548.691845855</v>
+        <v>1274471.092321406</v>
       </c>
     </row>
     <row r="19">
@@ -5098,7 +5098,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>416233.4970928326</v>
+        <v>421577.9859600904</v>
       </c>
     </row>
     <row r="20">
@@ -5124,7 +5124,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>457856.8468021158</v>
+        <v>463735.7845560995</v>
       </c>
     </row>
     <row r="21">
@@ -5160,7 +5160,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>412278.5807105413</v>
+        <v>417519.857038938</v>
       </c>
     </row>
     <row r="22">
@@ -5186,7 +5186,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>32.14236261986618</v>
+        <v>32.14959439464186</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -5194,7 +5194,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>3954.916382291296</v>
+        <v>4058.128921152442</v>
       </c>
     </row>
     <row r="23">
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8267460417882306</v>
+        <v>0.8239224430163152</v>
       </c>
     </row>
     <row r="24">
@@ -5258,7 +5258,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2577428.867806494</v>
+        <v>2585704.03231381</v>
       </c>
     </row>
     <row r="25">
@@ -5294,7 +5294,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>24.55071536549643</v>
+        <v>23.95928996628532</v>
       </c>
     </row>
     <row r="26">
@@ -5459,7 +5459,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>19.50523587787797</v>
+        <v>19.53652281064812</v>
       </c>
     </row>
     <row r="40">
@@ -5469,7 +5469,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>7.802094351151189</v>
+        <v>7.814609124259249</v>
       </c>
     </row>
     <row r="41">
@@ -5479,7 +5479,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>8.77735614504509</v>
+        <v>8.791435264791655</v>
       </c>
     </row>
     <row r="42">
@@ -5489,7 +5489,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>28.87210013150675</v>
+        <v>28.87024079378784</v>
       </c>
     </row>
     <row r="43">
@@ -5499,7 +5499,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>28.24514612114638</v>
+        <v>28.24228113201701</v>
       </c>
     </row>
     <row r="44">
@@ -5509,7 +5509,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>14.48960379499507</v>
+        <v>14.51284551648146</v>
       </c>
     </row>
     <row r="45">
@@ -5519,7 +5519,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>559.2677131779375</v>
+        <v>561.0633135905323</v>
       </c>
     </row>
     <row r="46">
@@ -5529,7 +5529,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>40.96099534354375</v>
+        <v>41.02669790236105</v>
       </c>
     </row>
     <row r="47">

</xml_diff>